<commit_message>
Change format of input sheets, fix efficacy sheet values for x dependent, fix beta PERT distribution values.
</commit_message>
<xml_diff>
--- a/InputFiles/DefineScenario.xlsx
+++ b/InputFiles/DefineScenario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\EPA\WideAreaDecon\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B200BA9-1C76-4046-9920-64940E54B2A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94096A9C-973A-4A08-9C16-514CFB20D764}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal - File Info" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="136">
   <si>
     <t>SCWAD</t>
   </si>
@@ -423,24 +423,6 @@
     <t>UniformXDependent</t>
   </si>
   <si>
-    <t>Slope (m)</t>
-  </si>
-  <si>
-    <t>Y Intercept (b)</t>
-  </si>
-  <si>
-    <t>Starting Point X</t>
-  </si>
-  <si>
-    <t>Starting Point Y</t>
-  </si>
-  <si>
-    <t>Ending Point X</t>
-  </si>
-  <si>
-    <t>Ending Point Y</t>
-  </si>
-  <si>
     <t>BimodalTruncatedNormal</t>
   </si>
   <si>
@@ -456,19 +438,19 @@
     <t>Std Dev 2</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Indoor;Underground;Outdoor</t>
   </si>
   <si>
-    <t>Param 7 Description</t>
-  </si>
-  <si>
     <t>Dependent Variable</t>
   </si>
   <si>
-    <t>Parameter 7</t>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
   </si>
 </sst>
 </file>
@@ -750,18 +732,13 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="172">
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
+  <dxfs count="157">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -811,20 +788,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <i/>
         <strike/>
@@ -836,6 +799,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <i/>
         <strike/>
@@ -908,6 +878,27 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <i/>
         <strike/>
@@ -919,34 +910,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <i/>
         <strike/>
@@ -958,6 +921,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <i/>
         <strike/>
@@ -994,6 +964,20 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <i/>
         <strike/>
@@ -1012,20 +996,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <i/>
         <strike/>
@@ -1037,6 +1007,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <i/>
         <strike/>
@@ -1084,20 +1061,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <i/>
         <strike/>
@@ -1109,6 +1072,13 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <i/>
         <strike/>
@@ -1145,810 +1115,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <i/>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color indexed="64"/>
@@ -3129,6 +2295,598 @@
           <color indexed="64"/>
         </right>
         <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
           <color indexed="64"/>
         </top>
         <bottom style="thin">
@@ -3520,185 +3278,171 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{77E3C927-1FC6-443B-87ED-00E2959DD317}" name="Table1568" displayName="Table1568" ref="A1:Q4" totalsRowShown="0" tableBorderDxfId="73">
-  <autoFilter ref="A1:Q4" xr:uid="{58F00973-C0E2-47D9-9C5E-C7B7F684A0C3}"/>
-  <tableColumns count="17">
-    <tableColumn id="9" xr3:uid="{62A6D655-D638-4005-9525-C140421ED9AB}" name="Phase" dataDxfId="72"/>
-    <tableColumn id="1" xr3:uid="{1BC04ADD-0426-4785-9F97-FCE0BCC1E547}" name="Category" dataDxfId="71"/>
-    <tableColumn id="2" xr3:uid="{3089FC2E-257C-4BA5-A9A7-5D0E01D5E6F5}" name="Name" dataDxfId="70"/>
-    <tableColumn id="10" xr3:uid="{E1A27E6E-82E5-4CF6-9164-A680FF7F05A5}" name="Description" dataDxfId="69"/>
-    <tableColumn id="3" xr3:uid="{BA85C23F-8236-43E3-885F-DF8CCDB84F06}" name="Units" dataDxfId="68"/>
-    <tableColumn id="16" xr3:uid="{F53AF906-8DA2-4F8A-8B2C-B716247EEA39}" name="Notes" dataDxfId="57"/>
-    <tableColumn id="4" xr3:uid="{9121EDDE-A8D8-4E28-AAAC-953CC1A14CB2}" name="Distribution Type" dataDxfId="67"/>
-    <tableColumn id="5" xr3:uid="{67D6DF1C-45B3-456F-B960-B8F495F6867D}" name="Parameter 1" dataDxfId="66"/>
-    <tableColumn id="6" xr3:uid="{A2BB8730-6626-47D8-AABB-90C19B218AFB}" name="Parameter 2" dataDxfId="65"/>
-    <tableColumn id="7" xr3:uid="{B7BC4EB1-7616-4A3A-899A-F01A87DD3B48}" name="Parameter 3" dataDxfId="64"/>
-    <tableColumn id="8" xr3:uid="{32D71C9B-2B39-4A83-9EB0-1934F2F6FC91}" name="Parameter 4" dataDxfId="63"/>
-    <tableColumn id="14" xr3:uid="{31AC778C-1A4A-45DD-8A12-F22858D3CD3A}" name="Parameter 5" dataDxfId="62"/>
-    <tableColumn id="15" xr3:uid="{91C3BDC4-4893-4CF7-9830-76CC4A9BF6F1}" name="Parameter 6" dataDxfId="61"/>
-    <tableColumn id="17" xr3:uid="{A57DECD4-8229-4172-AA85-114E7177A2B6}" name="Parameter 7"/>
-    <tableColumn id="11" xr3:uid="{6BCEB05C-9FCE-48DE-91F0-D2ACC21C6C3E}" name="Lower Limit" dataDxfId="60"/>
-    <tableColumn id="12" xr3:uid="{CDC89704-43FE-407F-B8B4-079E5E991263}" name="Upper Limit" dataDxfId="59"/>
-    <tableColumn id="13" xr3:uid="{0758CB79-3F38-44D8-B78B-CC33BB1D2C70}" name="Step" dataDxfId="58"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{77E3C927-1FC6-443B-87ED-00E2959DD317}" name="Table1568" displayName="Table1568" ref="A1:O4" totalsRowShown="0" tableBorderDxfId="156">
+  <autoFilter ref="A1:O4" xr:uid="{58F00973-C0E2-47D9-9C5E-C7B7F684A0C3}"/>
+  <tableColumns count="15">
+    <tableColumn id="9" xr3:uid="{62A6D655-D638-4005-9525-C140421ED9AB}" name="Phase" dataDxfId="155"/>
+    <tableColumn id="1" xr3:uid="{1BC04ADD-0426-4785-9F97-FCE0BCC1E547}" name="Category" dataDxfId="154"/>
+    <tableColumn id="2" xr3:uid="{3089FC2E-257C-4BA5-A9A7-5D0E01D5E6F5}" name="Name" dataDxfId="153"/>
+    <tableColumn id="10" xr3:uid="{E1A27E6E-82E5-4CF6-9164-A680FF7F05A5}" name="Description" dataDxfId="152"/>
+    <tableColumn id="3" xr3:uid="{BA85C23F-8236-43E3-885F-DF8CCDB84F06}" name="Units" dataDxfId="151"/>
+    <tableColumn id="4" xr3:uid="{9121EDDE-A8D8-4E28-AAAC-953CC1A14CB2}" name="Distribution Type" dataDxfId="150"/>
+    <tableColumn id="5" xr3:uid="{67D6DF1C-45B3-456F-B960-B8F495F6867D}" name="Parameter 1" dataDxfId="149"/>
+    <tableColumn id="6" xr3:uid="{A2BB8730-6626-47D8-AABB-90C19B218AFB}" name="Parameter 2" dataDxfId="148"/>
+    <tableColumn id="7" xr3:uid="{B7BC4EB1-7616-4A3A-899A-F01A87DD3B48}" name="Parameter 3" dataDxfId="147"/>
+    <tableColumn id="8" xr3:uid="{32D71C9B-2B39-4A83-9EB0-1934F2F6FC91}" name="Parameter 4" dataDxfId="146"/>
+    <tableColumn id="14" xr3:uid="{31AC778C-1A4A-45DD-8A12-F22858D3CD3A}" name="Parameter 5" dataDxfId="145"/>
+    <tableColumn id="15" xr3:uid="{91C3BDC4-4893-4CF7-9830-76CC4A9BF6F1}" name="Parameter 6" dataDxfId="144"/>
+    <tableColumn id="11" xr3:uid="{6BCEB05C-9FCE-48DE-91F0-D2ACC21C6C3E}" name="Lower Limit" dataDxfId="143"/>
+    <tableColumn id="12" xr3:uid="{CDC89704-43FE-407F-B8B4-079E5E991263}" name="Upper Limit" dataDxfId="142"/>
+    <tableColumn id="13" xr3:uid="{0758CB79-3F38-44D8-B78B-CC33BB1D2C70}" name="Step" dataDxfId="141"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{B77B7895-2678-4EA1-91B2-B6248E05AA0A}" name="Table156810" displayName="Table156810" ref="A1:Q8" totalsRowShown="0" tableBorderDxfId="89">
-  <autoFilter ref="A1:Q8" xr:uid="{60C5A2AF-4D3E-4976-AA8F-8961FE4EE49E}"/>
-  <tableColumns count="17">
-    <tableColumn id="9" xr3:uid="{DF77AA95-0523-4660-B964-676ECCB79418}" name="Phase" dataDxfId="88"/>
-    <tableColumn id="1" xr3:uid="{423292BC-9F1E-4EDC-9CC2-9890D4B1F00A}" name="Category" dataDxfId="87"/>
-    <tableColumn id="2" xr3:uid="{916CDEF4-7288-42C6-AD00-C6D0D8F8D560}" name="Name" dataDxfId="86"/>
-    <tableColumn id="10" xr3:uid="{C69B0C1F-B3A6-4CB4-B855-8A573BA536A2}" name="Description" dataDxfId="85"/>
-    <tableColumn id="3" xr3:uid="{23E3372F-48DE-4E64-88D3-C7EE1A32F34A}" name="Units" dataDxfId="84"/>
-    <tableColumn id="16" xr3:uid="{47D22AA2-1052-467B-855F-D3E336C9A1BA}" name="Notes" dataDxfId="56"/>
-    <tableColumn id="4" xr3:uid="{9D790DCF-5822-477B-8DCC-93F90CAB183B}" name="Distribution Type" dataDxfId="83"/>
-    <tableColumn id="5" xr3:uid="{337DB99B-F988-4680-87F5-A4BCFAF1A3C2}" name="Parameter 1" dataDxfId="82"/>
-    <tableColumn id="6" xr3:uid="{8C90C787-B669-453A-8F0E-A46E3018D380}" name="Parameter 2" dataDxfId="81"/>
-    <tableColumn id="7" xr3:uid="{041FF432-9543-4EE3-A9CF-1500CC344FFA}" name="Parameter 3" dataDxfId="80"/>
-    <tableColumn id="8" xr3:uid="{CDC02AC4-4C95-4220-B404-681CADF416D2}" name="Parameter 4" dataDxfId="79"/>
-    <tableColumn id="14" xr3:uid="{97B53FFA-4984-4D47-817E-8D167978BD8D}" name="Parameter 5" dataDxfId="78"/>
-    <tableColumn id="15" xr3:uid="{823939D4-F4DD-4DB0-89DB-EF0A01ECB48B}" name="Parameter 6" dataDxfId="77"/>
-    <tableColumn id="17" xr3:uid="{BE3DF7EB-D49F-4DDE-A86D-B7735A6890C6}" name="Parameter 7" dataDxfId="50"/>
-    <tableColumn id="11" xr3:uid="{20A93856-0EFF-4271-832C-04F7E9AC0A1E}" name="Lower Limit" dataDxfId="76"/>
-    <tableColumn id="12" xr3:uid="{A36F5215-EB9D-448B-AE9F-58A4F8E9D0C7}" name="Upper Limit" dataDxfId="75"/>
-    <tableColumn id="13" xr3:uid="{39173C83-06DA-436D-B107-9D64D97B7F39}" name="Step" dataDxfId="74"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{B77B7895-2678-4EA1-91B2-B6248E05AA0A}" name="Table156810" displayName="Table156810" ref="A1:O8" totalsRowShown="0" tableBorderDxfId="140">
+  <autoFilter ref="A1:O8" xr:uid="{60C5A2AF-4D3E-4976-AA8F-8961FE4EE49E}"/>
+  <tableColumns count="15">
+    <tableColumn id="9" xr3:uid="{DF77AA95-0523-4660-B964-676ECCB79418}" name="Phase" dataDxfId="139"/>
+    <tableColumn id="1" xr3:uid="{423292BC-9F1E-4EDC-9CC2-9890D4B1F00A}" name="Category" dataDxfId="138"/>
+    <tableColumn id="2" xr3:uid="{916CDEF4-7288-42C6-AD00-C6D0D8F8D560}" name="Name" dataDxfId="137"/>
+    <tableColumn id="10" xr3:uid="{C69B0C1F-B3A6-4CB4-B855-8A573BA536A2}" name="Description" dataDxfId="136"/>
+    <tableColumn id="3" xr3:uid="{23E3372F-48DE-4E64-88D3-C7EE1A32F34A}" name="Units" dataDxfId="135"/>
+    <tableColumn id="4" xr3:uid="{9D790DCF-5822-477B-8DCC-93F90CAB183B}" name="Distribution Type" dataDxfId="134"/>
+    <tableColumn id="5" xr3:uid="{337DB99B-F988-4680-87F5-A4BCFAF1A3C2}" name="Parameter 1" dataDxfId="133"/>
+    <tableColumn id="6" xr3:uid="{8C90C787-B669-453A-8F0E-A46E3018D380}" name="Parameter 2" dataDxfId="132"/>
+    <tableColumn id="7" xr3:uid="{041FF432-9543-4EE3-A9CF-1500CC344FFA}" name="Parameter 3" dataDxfId="131"/>
+    <tableColumn id="8" xr3:uid="{CDC02AC4-4C95-4220-B404-681CADF416D2}" name="Parameter 4" dataDxfId="130"/>
+    <tableColumn id="14" xr3:uid="{97B53FFA-4984-4D47-817E-8D167978BD8D}" name="Parameter 5" dataDxfId="129"/>
+    <tableColumn id="15" xr3:uid="{823939D4-F4DD-4DB0-89DB-EF0A01ECB48B}" name="Parameter 6" dataDxfId="128"/>
+    <tableColumn id="11" xr3:uid="{20A93856-0EFF-4271-832C-04F7E9AC0A1E}" name="Lower Limit" dataDxfId="127"/>
+    <tableColumn id="12" xr3:uid="{A36F5215-EB9D-448B-AE9F-58A4F8E9D0C7}" name="Upper Limit" dataDxfId="126"/>
+    <tableColumn id="13" xr3:uid="{39173C83-06DA-436D-B107-9D64D97B7F39}" name="Step" dataDxfId="125"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table156" displayName="Table156" ref="A1:Q3" totalsRowShown="0" tableBorderDxfId="171">
-  <autoFilter ref="A1:Q3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="17">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Phase" dataDxfId="170"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Category" dataDxfId="169"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="168"/>
-    <tableColumn id="10" xr3:uid="{115A314C-6A1B-4509-AD17-EBA48B227F1D}" name="Description" dataDxfId="167"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Units" dataDxfId="166"/>
-    <tableColumn id="16" xr3:uid="{8CA48522-E269-47F7-AB4F-A0B53480306B}" name="Notes" dataDxfId="55"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Distribution Type" dataDxfId="165"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Parameter 1" dataDxfId="164"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Parameter 2" dataDxfId="163"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Parameter 3" dataDxfId="162"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Parameter 4" dataDxfId="161"/>
-    <tableColumn id="14" xr3:uid="{D27F5CDB-A68A-4129-930A-F29B15C22636}" name="Parameter 5" dataDxfId="160"/>
-    <tableColumn id="15" xr3:uid="{0AB42936-B3F8-4E7C-8152-8CB99EFF7215}" name="Parameter 6" dataDxfId="159"/>
-    <tableColumn id="17" xr3:uid="{A2F41808-5B98-4F78-A6E2-0A2796A552B3}" name="Parameter 7" dataDxfId="49"/>
-    <tableColumn id="11" xr3:uid="{1D961365-C163-4709-AB34-FA18998E1C0C}" name="Lower Limit" dataDxfId="158"/>
-    <tableColumn id="12" xr3:uid="{DD91A285-8CA3-48CC-8B2D-6AD307B1829A}" name="Upper Limit" dataDxfId="157"/>
-    <tableColumn id="13" xr3:uid="{289708CC-2479-44B9-8E21-211759607199}" name="Step" dataDxfId="156"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table156" displayName="Table156" ref="A1:O3" totalsRowShown="0" tableBorderDxfId="124">
+  <autoFilter ref="A1:O3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="15">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Phase" dataDxfId="123"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Category" dataDxfId="122"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="121"/>
+    <tableColumn id="10" xr3:uid="{115A314C-6A1B-4509-AD17-EBA48B227F1D}" name="Description" dataDxfId="120"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Units" dataDxfId="119"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Distribution Type" dataDxfId="118"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Parameter 1" dataDxfId="117"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Parameter 2" dataDxfId="116"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Parameter 3" dataDxfId="115"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Parameter 4" dataDxfId="114"/>
+    <tableColumn id="14" xr3:uid="{D27F5CDB-A68A-4129-930A-F29B15C22636}" name="Parameter 5" dataDxfId="113"/>
+    <tableColumn id="15" xr3:uid="{0AB42936-B3F8-4E7C-8152-8CB99EFF7215}" name="Parameter 6" dataDxfId="112"/>
+    <tableColumn id="11" xr3:uid="{1D961365-C163-4709-AB34-FA18998E1C0C}" name="Lower Limit" dataDxfId="111"/>
+    <tableColumn id="12" xr3:uid="{DD91A285-8CA3-48CC-8B2D-6AD307B1829A}" name="Upper Limit" dataDxfId="110"/>
+    <tableColumn id="13" xr3:uid="{289708CC-2479-44B9-8E21-211759607199}" name="Step" dataDxfId="109"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table15" displayName="Table15" ref="A1:Q4" totalsRowShown="0" tableBorderDxfId="155">
-  <autoFilter ref="A1:Q4" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
-  <tableColumns count="17">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Phase" dataDxfId="154"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Category" dataDxfId="153"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="152"/>
-    <tableColumn id="10" xr3:uid="{E238511C-0575-407F-83C7-4D6E37CAA1C8}" name="Description" dataDxfId="151"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Units" dataDxfId="150"/>
-    <tableColumn id="16" xr3:uid="{3AF040ED-2D4F-41AD-9714-FE54F686DA23}" name="Notes" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Distribution Type" dataDxfId="149"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Parameter 1" dataDxfId="148"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Parameter 2" dataDxfId="147"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Parameter 3" dataDxfId="146"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Parameter 4" dataDxfId="145"/>
-    <tableColumn id="14" xr3:uid="{0CCC8750-3EB9-4A09-95AB-3BEC14F064B0}" name="Parameter 5" dataDxfId="144"/>
-    <tableColumn id="15" xr3:uid="{8430512F-5835-4882-88A6-3BDD8313812B}" name="Parameter 6" dataDxfId="143"/>
-    <tableColumn id="17" xr3:uid="{10C1E54A-C737-4956-92E2-EE13E1A7CACC}" name="Parameter 7" dataDxfId="48"/>
-    <tableColumn id="11" xr3:uid="{1D5D06E3-C2FF-4E33-A67E-846C813585DD}" name="Lower Limit" dataDxfId="142"/>
-    <tableColumn id="12" xr3:uid="{59B419A3-4B50-4E25-9295-12F6E479C7C1}" name="Upper Limit" dataDxfId="141"/>
-    <tableColumn id="13" xr3:uid="{B44B2162-0D76-4003-8141-9F91F7CB1D51}" name="Step" dataDxfId="140"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table15" displayName="Table15" ref="A1:O4" totalsRowShown="0" tableBorderDxfId="108">
+  <autoFilter ref="A1:O4" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+  <tableColumns count="15">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Phase" dataDxfId="107"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Category" dataDxfId="106"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="105"/>
+    <tableColumn id="10" xr3:uid="{E238511C-0575-407F-83C7-4D6E37CAA1C8}" name="Description" dataDxfId="104"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Units" dataDxfId="103"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Distribution Type" dataDxfId="102"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Parameter 1" dataDxfId="101"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Parameter 2" dataDxfId="100"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Parameter 3" dataDxfId="99"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Parameter 4" dataDxfId="98"/>
+    <tableColumn id="14" xr3:uid="{0CCC8750-3EB9-4A09-95AB-3BEC14F064B0}" name="Parameter 5" dataDxfId="97"/>
+    <tableColumn id="15" xr3:uid="{8430512F-5835-4882-88A6-3BDD8313812B}" name="Parameter 6" dataDxfId="96"/>
+    <tableColumn id="11" xr3:uid="{1D5D06E3-C2FF-4E33-A67E-846C813585DD}" name="Lower Limit" dataDxfId="95"/>
+    <tableColumn id="12" xr3:uid="{59B419A3-4B50-4E25-9295-12F6E479C7C1}" name="Upper Limit" dataDxfId="94"/>
+    <tableColumn id="13" xr3:uid="{B44B2162-0D76-4003-8141-9F91F7CB1D51}" name="Step" dataDxfId="93"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table157" displayName="Table157" ref="A1:Q4" totalsRowShown="0" tableBorderDxfId="139">
-  <autoFilter ref="A1:Q4" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <tableColumns count="17">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Internal" dataDxfId="138"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Category" dataDxfId="137"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="136"/>
-    <tableColumn id="10" xr3:uid="{82317EA3-EFA1-4204-866F-27AD4E7F4565}" name="Description" dataDxfId="135"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Units" dataDxfId="134"/>
-    <tableColumn id="16" xr3:uid="{DF03E324-1E5E-4D8E-A1B6-A4B0C189A15A}" name="Notes" dataDxfId="53"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Distribution Type" dataDxfId="133"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Parameter 1" dataDxfId="132"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Parameter 2" dataDxfId="131"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Parameter 3" dataDxfId="130"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Parameter 4" dataDxfId="129"/>
-    <tableColumn id="14" xr3:uid="{66AAE767-9060-4329-9FA8-8309678C711A}" name="Parameter 5" dataDxfId="128"/>
-    <tableColumn id="15" xr3:uid="{EB2740C5-3F80-408E-8F68-D65D3DE04CB6}" name="Parameter 6" dataDxfId="127"/>
-    <tableColumn id="17" xr3:uid="{E7CBD621-3EAB-410B-B049-AF8ED63D19BF}" name="Parameter 7" dataDxfId="47"/>
-    <tableColumn id="11" xr3:uid="{D8432F00-68F0-499E-8310-7BEAF2D5BFFA}" name="Lower Limit" dataDxfId="126"/>
-    <tableColumn id="12" xr3:uid="{BCED7806-F146-4B52-AF53-D5DE4EBA4D11}" name="Upper Limit" dataDxfId="125"/>
-    <tableColumn id="13" xr3:uid="{A3158C91-CCDA-42BB-98F8-B1415C87FD9F}" name="Step" dataDxfId="124"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table157" displayName="Table157" ref="A1:O4" totalsRowShown="0" tableBorderDxfId="92">
+  <autoFilter ref="A1:O4" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="15">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Internal" dataDxfId="91"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Category" dataDxfId="90"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="89"/>
+    <tableColumn id="10" xr3:uid="{82317EA3-EFA1-4204-866F-27AD4E7F4565}" name="Description" dataDxfId="88"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Units" dataDxfId="87"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Distribution Type" dataDxfId="86"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Parameter 1" dataDxfId="85"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Parameter 2" dataDxfId="84"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Parameter 3" dataDxfId="83"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Parameter 4" dataDxfId="82"/>
+    <tableColumn id="14" xr3:uid="{66AAE767-9060-4329-9FA8-8309678C711A}" name="Parameter 5" dataDxfId="81"/>
+    <tableColumn id="15" xr3:uid="{EB2740C5-3F80-408E-8F68-D65D3DE04CB6}" name="Parameter 6" dataDxfId="80"/>
+    <tableColumn id="11" xr3:uid="{D8432F00-68F0-499E-8310-7BEAF2D5BFFA}" name="Lower Limit" dataDxfId="79"/>
+    <tableColumn id="12" xr3:uid="{BCED7806-F146-4B52-AF53-D5DE4EBA4D11}" name="Upper Limit" dataDxfId="78"/>
+    <tableColumn id="13" xr3:uid="{A3158C91-CCDA-42BB-98F8-B1415C87FD9F}" name="Step" dataDxfId="77"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1579" displayName="Table1579" ref="A1:Q6" totalsRowShown="0" headerRowBorderDxfId="123" tableBorderDxfId="122">
-  <autoFilter ref="A1:Q6" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
-  <tableColumns count="17">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Internal" dataDxfId="121"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Category" dataDxfId="120"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Name" dataDxfId="119"/>
-    <tableColumn id="10" xr3:uid="{832C45C5-9E76-4B8A-83B0-2EB32C68E2FD}" name="Description" dataDxfId="118"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Units" dataDxfId="117"/>
-    <tableColumn id="16" xr3:uid="{A76C293E-4F8D-48E8-8E9B-1F8E969B63DA}" name="Notes" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Distribution Type" dataDxfId="116"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Parameter 1" dataDxfId="115"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Parameter 2" dataDxfId="114"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Parameter 3" dataDxfId="113"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Parameter 4" dataDxfId="112"/>
-    <tableColumn id="14" xr3:uid="{1289F8CF-6170-44F2-AD7D-9E9A4F12BCD1}" name="Parameter 5" dataDxfId="111"/>
-    <tableColumn id="15" xr3:uid="{6D5C8F75-1A51-48AD-90E7-17A2F3986BE7}" name="Parameter 6" dataDxfId="110"/>
-    <tableColumn id="17" xr3:uid="{E2911AC1-4B61-46E6-92D6-047FCE0DFBB6}" name="Parameter 7" dataDxfId="46"/>
-    <tableColumn id="11" xr3:uid="{DB8C4311-5A85-4D8D-A5C2-F47C77E8643D}" name="Lower Limit" dataDxfId="109"/>
-    <tableColumn id="12" xr3:uid="{96A08B49-5A79-4F13-BC86-FC5E2B426E49}" name="Upper Limit" dataDxfId="108"/>
-    <tableColumn id="13" xr3:uid="{D4252238-C1B7-4D7A-B8C5-A52164228F94}" name="Step" dataDxfId="107"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1579" displayName="Table1579" ref="A1:O6" totalsRowShown="0" headerRowBorderDxfId="76" tableBorderDxfId="75">
+  <autoFilter ref="A1:O6" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+  <tableColumns count="15">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Internal" dataDxfId="74"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Category" dataDxfId="73"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Name" dataDxfId="72"/>
+    <tableColumn id="10" xr3:uid="{832C45C5-9E76-4B8A-83B0-2EB32C68E2FD}" name="Description" dataDxfId="71"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Units" dataDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Distribution Type" dataDxfId="69"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Parameter 1" dataDxfId="68"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Parameter 2" dataDxfId="67"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Parameter 3" dataDxfId="66"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Parameter 4" dataDxfId="65"/>
+    <tableColumn id="14" xr3:uid="{1289F8CF-6170-44F2-AD7D-9E9A4F12BCD1}" name="Parameter 5" dataDxfId="64"/>
+    <tableColumn id="15" xr3:uid="{6D5C8F75-1A51-48AD-90E7-17A2F3986BE7}" name="Parameter 6" dataDxfId="63"/>
+    <tableColumn id="11" xr3:uid="{DB8C4311-5A85-4D8D-A5C2-F47C77E8643D}" name="Lower Limit" dataDxfId="62"/>
+    <tableColumn id="12" xr3:uid="{96A08B49-5A79-4F13-BC86-FC5E2B426E49}" name="Upper Limit" dataDxfId="61"/>
+    <tableColumn id="13" xr3:uid="{D4252238-C1B7-4D7A-B8C5-A52164228F94}" name="Step" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157910" displayName="Table157910" ref="A1:Q3" totalsRowShown="0" headerRowBorderDxfId="106" tableBorderDxfId="105">
-  <autoFilter ref="A1:Q3" xr:uid="{C58E5582-2A25-434F-8C6A-2EF9AC741C58}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157910" displayName="Table157910" ref="A1:O3" totalsRowShown="0" headerRowBorderDxfId="59" tableBorderDxfId="58">
+  <autoFilter ref="A1:O3" xr:uid="{C58E5582-2A25-434F-8C6A-2EF9AC741C58}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J2">
     <sortCondition ref="B1:B2"/>
   </sortState>
-  <tableColumns count="17">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="Internal" dataDxfId="104"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Category" dataDxfId="103"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Name" dataDxfId="102"/>
-    <tableColumn id="10" xr3:uid="{63BA373B-667A-4A36-BB6C-997B9631910B}" name="Description" dataDxfId="101"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Units" dataDxfId="100"/>
-    <tableColumn id="16" xr3:uid="{D3234437-8633-4633-A761-859E090311B3}" name="Notes" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Distribution Type" dataDxfId="99"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Parameter 1" dataDxfId="98"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Parameter 2" dataDxfId="97"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Parameter 3" dataDxfId="96"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Parameter 4" dataDxfId="95"/>
-    <tableColumn id="14" xr3:uid="{64E7458C-1D65-4712-ABFC-9DAF3D21B670}" name="Parameter 5" dataDxfId="94"/>
-    <tableColumn id="15" xr3:uid="{ABD8345F-8CFE-4FF4-A3F7-F6DB1042FE28}" name="Parameter 6" dataDxfId="93"/>
-    <tableColumn id="17" xr3:uid="{7A8E236B-9AF4-42BB-B2D7-1F94DA03337A}" name="Parameter 7" dataDxfId="0"/>
-    <tableColumn id="11" xr3:uid="{B286B466-1F40-4449-900C-61ACE92313F0}" name="Lower Limit" dataDxfId="92"/>
-    <tableColumn id="12" xr3:uid="{4CAE3350-4ABC-40B6-B059-3A8198700CE1}" name="Upper Limit" dataDxfId="91"/>
-    <tableColumn id="13" xr3:uid="{BC38CFEA-8053-4CB7-B237-C848302F26B7}" name="Step" dataDxfId="90"/>
+  <tableColumns count="15">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="Internal" dataDxfId="57"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Category" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Name" dataDxfId="55"/>
+    <tableColumn id="10" xr3:uid="{63BA373B-667A-4A36-BB6C-997B9631910B}" name="Description" dataDxfId="54"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Units" dataDxfId="53"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Distribution Type" dataDxfId="52"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Parameter 1" dataDxfId="51"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Parameter 2" dataDxfId="50"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Parameter 3" dataDxfId="49"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Parameter 4" dataDxfId="48"/>
+    <tableColumn id="14" xr3:uid="{64E7458C-1D65-4712-ABFC-9DAF3D21B670}" name="Parameter 5" dataDxfId="47"/>
+    <tableColumn id="15" xr3:uid="{ABD8345F-8CFE-4FF4-A3F7-F6DB1042FE28}" name="Parameter 6" dataDxfId="46"/>
+    <tableColumn id="11" xr3:uid="{B286B466-1F40-4449-900C-61ACE92313F0}" name="Lower Limit" dataDxfId="45"/>
+    <tableColumn id="12" xr3:uid="{4CAE3350-4ABC-40B6-B059-3A8198700CE1}" name="Upper Limit" dataDxfId="44"/>
+    <tableColumn id="13" xr3:uid="{BC38CFEA-8053-4CB7-B237-C848302F26B7}" name="Step" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4026,10 +3770,10 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4037,10 +3781,10 @@
     <col min="1" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="45.7109375" customWidth="1"/>
-    <col min="5" max="17" width="15.7109375" customWidth="1"/>
+    <col min="5" max="15" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -4057,45 +3801,39 @@
         <v>28</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>137</v>
+        <v>29</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>141</v>
+        <v>63</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q1" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>31</v>
@@ -4109,30 +3847,28 @@
       <c r="E2" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="17"/>
       <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
+      <c r="M2" s="15">
+        <v>20</v>
+      </c>
+      <c r="N2" s="15">
+        <v>500</v>
+      </c>
       <c r="O2" s="15">
-        <v>20</v>
-      </c>
-      <c r="P2" s="15">
-        <v>500</v>
-      </c>
-      <c r="Q2" s="15">
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>31</v>
@@ -4146,51 +3882,49 @@
       <c r="E3" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13" t="s">
+      <c r="F3" s="13" t="s">
         <v>3</v>
       </c>
+      <c r="G3" s="13"/>
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="17"/>
       <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
       <c r="O3" s="13"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="H2:N3">
-    <cfRule type="expression" dxfId="8" priority="33">
-      <formula>NOT((COLUMN(H2)-COLUMN($G:$G))&lt;=IFERROR(VLOOKUP($G2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:N3">
-    <cfRule type="expression" dxfId="7" priority="34">
-      <formula>ISBLANK($G2)</formula>
+  <conditionalFormatting sqref="G2:L3">
+    <cfRule type="expression" dxfId="5" priority="33">
+      <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="expression" dxfId="6" priority="1">
-      <formula>ISBLANK($G3)</formula>
+    <cfRule type="expression" dxfId="4" priority="1">
+      <formula>ISBLANK($F3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="2">
-      <formula>NOT((COLUMN(A3)-COLUMN($G:$G))&lt;=IFERROR(VLOOKUP($G3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>NOT((COLUMN(A3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="4" priority="3">
-      <formula>ISBLANK($G2)</formula>
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>NOT((COLUMN(A2)-COLUMN($G:$G))&lt;=IFERROR(VLOOKUP($G2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    <cfRule type="expression" dxfId="1" priority="4">
+      <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:L3">
+    <cfRule type="expression" dxfId="0" priority="50">
+      <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G2:G3" xr:uid="{00000000-0002-0000-0900-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F3" xr:uid="{00000000-0002-0000-0900-000000000000}">
       <formula1>Validation_Distribution_Types</formula1>
     </dataValidation>
   </dataValidations>
@@ -4204,10 +3938,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4215,10 +3949,9 @@
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
@@ -4243,11 +3976,8 @@
       <c r="H1" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="I1" s="15" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
@@ -4262,9 +3992,8 @@
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
       <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
@@ -4281,9 +4010,8 @@
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>74</v>
       </c>
@@ -4304,9 +4032,8 @@
       </c>
       <c r="G4" s="16"/>
       <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>77</v>
       </c>
@@ -4325,9 +4052,8 @@
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
       <c r="H5" s="16"/>
-      <c r="I5" s="16"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>79</v>
       </c>
@@ -4344,9 +4070,8 @@
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>80</v>
       </c>
@@ -4367,9 +4092,8 @@
       </c>
       <c r="G7" s="16"/>
       <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>118</v>
       </c>
@@ -4386,9 +4110,8 @@
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
       <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>120</v>
       </c>
@@ -4407,9 +4130,8 @@
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>122</v>
       </c>
@@ -4426,9 +4148,8 @@
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>125</v>
       </c>
@@ -4436,45 +4157,38 @@
         <v>6</v>
       </c>
       <c r="C11" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
         <v>126</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>132</v>
       </c>
       <c r="B12" s="10">
         <v>6</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>72</v>
@@ -4482,7 +4196,6 @@
       <c r="H12" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="I12" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4637,10 +4350,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097870CC-1A0F-461E-BDFD-29BDDFDDF05C}">
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4648,10 +4361,10 @@
     <col min="1" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="45.7109375" customWidth="1"/>
-    <col min="5" max="17" width="15.7109375" customWidth="1"/>
+    <col min="5" max="15" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>112</v>
       </c>
@@ -4668,43 +4381,37 @@
         <v>28</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>137</v>
+        <v>29</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>141</v>
+        <v>63</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q1" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>113</v>
       </c>
@@ -4720,28 +4427,26 @@
       <c r="E2" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="3"/>
       <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="M2" s="19">
+        <v>10000</v>
+      </c>
+      <c r="N2" s="19">
+        <v>50000000</v>
+      </c>
       <c r="O2" s="19">
         <v>10000</v>
       </c>
-      <c r="P2" s="19">
-        <v>50000000</v>
-      </c>
-      <c r="Q2" s="19">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>114</v>
       </c>
@@ -4757,28 +4462,26 @@
       <c r="E3" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13" t="s">
+      <c r="F3" s="13" t="s">
         <v>3</v>
       </c>
+      <c r="G3" s="13"/>
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
+      <c r="J3" s="14"/>
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
+      <c r="M3" s="20">
+        <v>10000</v>
+      </c>
+      <c r="N3" s="20">
+        <v>50000000</v>
+      </c>
       <c r="O3" s="20">
         <v>10000</v>
       </c>
-      <c r="P3" s="20">
-        <v>50000000</v>
-      </c>
-      <c r="Q3" s="20">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>115</v>
       </c>
@@ -4794,39 +4497,37 @@
       <c r="E4" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13" t="s">
+      <c r="F4" s="13" t="s">
         <v>3</v>
       </c>
+      <c r="G4" s="13"/>
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="20">
+        <v>10000</v>
+      </c>
+      <c r="N4" s="20">
+        <v>50000000</v>
+      </c>
       <c r="O4" s="20">
         <v>10000</v>
       </c>
-      <c r="P4" s="20">
-        <v>50000000</v>
-      </c>
-      <c r="Q4" s="20">
-        <v>10000</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A2:N4">
-    <cfRule type="expression" dxfId="45" priority="1">
-      <formula>ISBLANK($G2)</formula>
+  <conditionalFormatting sqref="A2:L4">
+    <cfRule type="expression" dxfId="42" priority="43">
+      <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="2">
-      <formula>NOT((COLUMN(A2)-COLUMN($G:$G))&lt;=IFERROR(VLOOKUP($G2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    <cfRule type="expression" dxfId="41" priority="44">
+      <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G2:G4" xr:uid="{330BE9FB-867A-4350-A3CC-F1598E7F7C5E}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F4" xr:uid="{330BE9FB-867A-4350-A3CC-F1598E7F7C5E}">
       <formula1>Validation_Distribution_Types</formula1>
     </dataValidation>
   </dataValidations>
@@ -4839,19 +4540,21 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2E755C4-38C6-4293-91DA-AE4F2174B63E}">
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="45.7109375" customWidth="1"/>
-    <col min="5" max="17" width="15.7109375" customWidth="1"/>
+    <col min="5" max="15" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>112</v>
       </c>
@@ -4868,43 +4571,37 @@
         <v>28</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>137</v>
+        <v>29</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>141</v>
+        <v>63</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q1" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>114</v>
       </c>
@@ -4920,28 +4617,26 @@
       <c r="E2" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="3"/>
       <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="M2" s="19">
+        <v>0</v>
+      </c>
+      <c r="N2" s="19">
+        <v>1</v>
+      </c>
       <c r="O2" s="19">
-        <v>0</v>
-      </c>
-      <c r="P2" s="19">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="19">
         <v>0.01</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>114</v>
       </c>
@@ -4957,28 +4652,26 @@
       <c r="E3" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13" t="s">
+      <c r="F3" s="13" t="s">
         <v>3</v>
       </c>
+      <c r="G3" s="13"/>
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="20">
+        <v>0</v>
+      </c>
+      <c r="N3" s="20">
+        <v>1</v>
+      </c>
       <c r="O3" s="20">
-        <v>0</v>
-      </c>
-      <c r="P3" s="20">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="20">
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>114</v>
       </c>
@@ -4994,28 +4687,26 @@
       <c r="E4" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13" t="s">
+      <c r="F4" s="13" t="s">
         <v>3</v>
       </c>
+      <c r="G4" s="13"/>
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="14"/>
-      <c r="L4" s="17"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="19">
+        <v>0</v>
+      </c>
+      <c r="N4" s="19">
+        <v>1</v>
+      </c>
       <c r="O4" s="19">
-        <v>0</v>
-      </c>
-      <c r="P4" s="19">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="19">
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>114</v>
       </c>
@@ -5031,28 +4722,26 @@
       <c r="E5" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13" t="s">
+      <c r="F5" s="13" t="s">
         <v>3</v>
       </c>
+      <c r="G5" s="13"/>
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="19">
+        <v>0</v>
+      </c>
+      <c r="N5" s="19">
+        <v>1</v>
+      </c>
       <c r="O5" s="19">
-        <v>0</v>
-      </c>
-      <c r="P5" s="19">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="19">
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>114</v>
       </c>
@@ -5068,28 +4757,26 @@
       <c r="E6" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13" t="s">
+      <c r="F6" s="13" t="s">
         <v>3</v>
       </c>
+      <c r="G6" s="13"/>
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="19">
+        <v>0</v>
+      </c>
+      <c r="N6" s="19">
+        <v>1</v>
+      </c>
       <c r="O6" s="19">
-        <v>0</v>
-      </c>
-      <c r="P6" s="19">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="19">
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>114</v>
       </c>
@@ -5105,28 +4792,26 @@
       <c r="E7" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13" t="s">
+      <c r="F7" s="13" t="s">
         <v>3</v>
       </c>
+      <c r="G7" s="13"/>
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="14"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="19">
+        <v>0</v>
+      </c>
+      <c r="N7" s="19">
+        <v>1</v>
+      </c>
       <c r="O7" s="19">
-        <v>0</v>
-      </c>
-      <c r="P7" s="19">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="19">
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>114</v>
       </c>
@@ -5142,39 +4827,37 @@
       <c r="E8" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="F8" s="13"/>
-      <c r="G8" s="13" t="s">
+      <c r="F8" s="13" t="s">
         <v>3</v>
       </c>
+      <c r="G8" s="13"/>
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="17"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="13"/>
+      <c r="L8" s="13"/>
+      <c r="M8" s="19">
+        <v>0</v>
+      </c>
+      <c r="N8" s="19">
+        <v>1</v>
+      </c>
       <c r="O8" s="19">
-        <v>0</v>
-      </c>
-      <c r="P8" s="19">
-        <v>1</v>
-      </c>
-      <c r="Q8" s="19">
         <v>0.01</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A2:N8">
-    <cfRule type="expression" dxfId="43" priority="1">
-      <formula>ISBLANK($G2)</formula>
+  <conditionalFormatting sqref="A2:L8">
+    <cfRule type="expression" dxfId="40" priority="45">
+      <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="2">
-      <formula>NOT((COLUMN(A2)-COLUMN($G:$G))&lt;=IFERROR(VLOOKUP($G2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    <cfRule type="expression" dxfId="39" priority="46">
+      <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G2:G8" xr:uid="{698F0607-DC03-45F0-A4F2-E36B0A9EB77D}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F8" xr:uid="{698F0607-DC03-45F0-A4F2-E36B0A9EB77D}">
       <formula1>Validation_Distribution_Types</formula1>
     </dataValidation>
   </dataValidations>
@@ -5188,19 +4871,21 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="A1:Q3"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="45.7109375" customWidth="1"/>
-    <col min="5" max="17" width="15.7109375" customWidth="1"/>
+    <col min="5" max="15" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>112</v>
       </c>
@@ -5217,45 +4902,39 @@
         <v>28</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>137</v>
+        <v>29</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>141</v>
+        <v>63</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q1" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>30</v>
@@ -5269,30 +4948,28 @@
       <c r="E2" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="3"/>
       <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>10</v>
+      </c>
       <c r="O2" s="1">
-        <v>0</v>
-      </c>
-      <c r="P2" s="1">
-        <v>10</v>
-      </c>
-      <c r="Q2" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B3" s="12" t="s">
         <v>31</v>
@@ -5306,39 +4983,37 @@
       <c r="E3" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13" t="s">
+      <c r="F3" s="13" t="s">
         <v>3</v>
       </c>
+      <c r="G3" s="13"/>
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
+      <c r="J3" s="14"/>
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
+      <c r="M3" s="13">
+        <v>0</v>
+      </c>
+      <c r="N3" s="13">
+        <v>10</v>
+      </c>
       <c r="O3" s="13">
-        <v>0</v>
-      </c>
-      <c r="P3" s="13">
-        <v>10</v>
-      </c>
-      <c r="Q3" s="13">
         <v>0.1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A2:N3">
-    <cfRule type="expression" dxfId="41" priority="33">
-      <formula>ISBLANK($G2)</formula>
+  <conditionalFormatting sqref="A2:L3">
+    <cfRule type="expression" dxfId="38" priority="47">
+      <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="34">
-      <formula>NOT((COLUMN(A2)-COLUMN($G:$G))&lt;=IFERROR(VLOOKUP($G2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    <cfRule type="expression" dxfId="37" priority="48">
+      <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G2:G3" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F3" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>Validation_Distribution_Types</formula1>
     </dataValidation>
   </dataValidations>
@@ -5353,19 +5028,21 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Sheet6"/>
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="45.7109375" customWidth="1"/>
-    <col min="5" max="17" width="15.7109375" customWidth="1"/>
+    <col min="5" max="15" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>112</v>
       </c>
@@ -5382,45 +5059,39 @@
         <v>28</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>137</v>
+        <v>29</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>141</v>
+        <v>63</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q1" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>31</v>
@@ -5434,30 +5105,28 @@
       <c r="E2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="3"/>
       <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>20</v>
+      </c>
       <c r="O2" s="1">
-        <v>0</v>
-      </c>
-      <c r="P2" s="1">
-        <v>20</v>
-      </c>
-      <c r="Q2" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>38</v>
@@ -5471,30 +5140,28 @@
       <c r="E3" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>3</v>
       </c>
+      <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
+      <c r="J3" s="11"/>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
+      <c r="M3" s="10">
+        <v>0</v>
+      </c>
+      <c r="N3" s="10">
+        <v>20</v>
+      </c>
       <c r="O3" s="10">
-        <v>0</v>
-      </c>
-      <c r="P3" s="10">
-        <v>20</v>
-      </c>
-      <c r="Q3" s="10">
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>31</v>
@@ -5508,65 +5175,63 @@
       <c r="E4" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10" t="s">
+      <c r="F4" s="10" t="s">
         <v>3</v>
       </c>
+      <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="14"/>
       <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
+      <c r="M4" s="13">
+        <v>0</v>
+      </c>
+      <c r="N4" s="13">
+        <v>48</v>
+      </c>
       <c r="O4" s="13">
-        <v>0</v>
-      </c>
-      <c r="P4" s="13">
-        <v>48</v>
-      </c>
-      <c r="Q4" s="13">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="H2:N4">
-    <cfRule type="expression" dxfId="39" priority="23">
-      <formula>NOT((COLUMN(H2)-COLUMN($G:$G))&lt;=IFERROR(VLOOKUP($G2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B2:N4">
-    <cfRule type="expression" dxfId="38" priority="40">
-      <formula>ISBLANK($G2)</formula>
+  <conditionalFormatting sqref="G2:L4">
+    <cfRule type="expression" dxfId="36" priority="23">
+      <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="37" priority="5">
-      <formula>ISBLANK($G2)</formula>
+    <cfRule type="expression" dxfId="35" priority="5">
+      <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="6">
-      <formula>NOT((COLUMN(A2)-COLUMN($G:$G))&lt;=IFERROR(VLOOKUP($G2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    <cfRule type="expression" dxfId="34" priority="6">
+      <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="expression" dxfId="35" priority="3">
-      <formula>ISBLANK($G3)</formula>
+    <cfRule type="expression" dxfId="33" priority="3">
+      <formula>ISBLANK($F3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="4">
-      <formula>NOT((COLUMN(A3)-COLUMN($G:$G))&lt;=IFERROR(VLOOKUP($G3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    <cfRule type="expression" dxfId="32" priority="4">
+      <formula>NOT((COLUMN(A3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="expression" dxfId="33" priority="1">
-      <formula>ISBLANK($G4)</formula>
+    <cfRule type="expression" dxfId="31" priority="1">
+      <formula>ISBLANK($F4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="2">
-      <formula>NOT((COLUMN(A4)-COLUMN($G:$G))&lt;=IFERROR(VLOOKUP($G4, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    <cfRule type="expression" dxfId="30" priority="2">
+      <formula>NOT((COLUMN(A4)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F4, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:L4">
+    <cfRule type="expression" dxfId="29" priority="49">
+      <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G2:G4" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F4" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>Validation_Distribution_Types</formula1>
     </dataValidation>
   </dataValidations>
@@ -5580,10 +5245,10 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:Q4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5591,10 +5256,10 @@
     <col min="1" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="45.7109375" customWidth="1"/>
-    <col min="5" max="17" width="15.7109375" customWidth="1"/>
+    <col min="5" max="15" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -5611,45 +5276,39 @@
         <v>28</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>137</v>
+        <v>29</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>141</v>
+        <v>63</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q1" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>30</v>
@@ -5663,30 +5322,28 @@
       <c r="E2" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6" t="s">
+      <c r="F2" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="3"/>
       <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>10</v>
+      </c>
       <c r="O2" s="1">
-        <v>0</v>
-      </c>
-      <c r="P2" s="1">
-        <v>10</v>
-      </c>
-      <c r="Q2" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>43</v>
@@ -5700,30 +5357,28 @@
       <c r="E3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>3</v>
       </c>
+      <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
+      <c r="J3" s="11"/>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
+      <c r="M3" s="10">
+        <v>0</v>
+      </c>
+      <c r="N3" s="10">
+        <v>10000</v>
+      </c>
       <c r="O3" s="10">
-        <v>0</v>
-      </c>
-      <c r="P3" s="10">
-        <v>10000</v>
-      </c>
-      <c r="Q3" s="10">
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>38</v>
@@ -5737,70 +5392,68 @@
       <c r="E4" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10" t="s">
+      <c r="F4" s="10" t="s">
         <v>3</v>
       </c>
+      <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="14"/>
       <c r="L4" s="14"/>
-      <c r="M4" s="14"/>
-      <c r="N4" s="14"/>
+      <c r="M4" s="13">
+        <v>0</v>
+      </c>
+      <c r="N4" s="13">
+        <v>10</v>
+      </c>
       <c r="O4" s="13">
-        <v>0</v>
-      </c>
-      <c r="P4" s="13">
-        <v>10</v>
-      </c>
-      <c r="Q4" s="13">
         <v>0.1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="H2:N4">
-    <cfRule type="expression" dxfId="31" priority="25">
-      <formula>NOT((COLUMN(H2)-COLUMN($G:$G))&lt;=IFERROR(VLOOKUP($G2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+  <conditionalFormatting sqref="G2:L4">
+    <cfRule type="expression" dxfId="28" priority="25">
+      <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B4:C4 E4:N4 B2:N3">
-    <cfRule type="expression" dxfId="30" priority="38">
-      <formula>ISBLANK($G2)</formula>
+  <conditionalFormatting sqref="B4:C4 E4:L4 B2:L3">
+    <cfRule type="expression" dxfId="27" priority="38">
+      <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="expression" dxfId="29" priority="7">
-      <formula>ISBLANK($G4)</formula>
+    <cfRule type="expression" dxfId="26" priority="7">
+      <formula>ISBLANK($F4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="28" priority="5">
-      <formula>ISBLANK($G2)</formula>
+    <cfRule type="expression" dxfId="25" priority="5">
+      <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="6">
-      <formula>NOT((COLUMN(A2)-COLUMN($G:$G))&lt;=IFERROR(VLOOKUP($G2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    <cfRule type="expression" dxfId="24" priority="6">
+      <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="expression" dxfId="26" priority="3">
-      <formula>ISBLANK($G3)</formula>
+    <cfRule type="expression" dxfId="23" priority="3">
+      <formula>ISBLANK($F3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="4">
-      <formula>NOT((COLUMN(A3)-COLUMN($G:$G))&lt;=IFERROR(VLOOKUP($G3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    <cfRule type="expression" dxfId="22" priority="4">
+      <formula>NOT((COLUMN(A3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="expression" dxfId="24" priority="1">
-      <formula>ISBLANK($G4)</formula>
+    <cfRule type="expression" dxfId="21" priority="1">
+      <formula>ISBLANK($F4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="2">
-      <formula>NOT((COLUMN(A4)-COLUMN($G:$G))&lt;=IFERROR(VLOOKUP($G4, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    <cfRule type="expression" dxfId="20" priority="2">
+      <formula>NOT((COLUMN(A4)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F4, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G2:G4" xr:uid="{00000000-0002-0000-0600-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F4" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>Validation_Distribution_Types</formula1>
     </dataValidation>
   </dataValidations>
@@ -5814,10 +5467,10 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:Q6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5825,10 +5478,10 @@
     <col min="1" max="2" width="15.7109375" customWidth="1"/>
     <col min="3" max="3" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="45.7109375" customWidth="1"/>
-    <col min="5" max="17" width="15.7109375" customWidth="1"/>
+    <col min="5" max="15" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -5845,45 +5498,39 @@
         <v>28</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>137</v>
+        <v>29</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>141</v>
+        <v>63</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q1" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>30</v>
@@ -5897,30 +5544,28 @@
       <c r="E2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
+      <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>10</v>
+      </c>
       <c r="O2" s="1">
-        <v>0</v>
-      </c>
-      <c r="P2" s="1">
-        <v>10</v>
-      </c>
-      <c r="Q2" s="1">
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>31</v>
@@ -5934,30 +5579,28 @@
       <c r="E3" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10" t="s">
+      <c r="F3" s="10" t="s">
         <v>3</v>
       </c>
+      <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
+      <c r="J3" s="11"/>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
+      <c r="M3" s="10">
+        <v>100</v>
+      </c>
+      <c r="N3" s="10">
+        <v>2000</v>
+      </c>
       <c r="O3" s="10">
-        <v>100</v>
-      </c>
-      <c r="P3" s="10">
-        <v>2000</v>
-      </c>
-      <c r="Q3" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>31</v>
@@ -5971,30 +5614,28 @@
       <c r="E4" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10" t="s">
+      <c r="F4" s="10" t="s">
         <v>3</v>
       </c>
+      <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
+      <c r="J4" s="11"/>
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
+      <c r="M4" s="10">
+        <v>100</v>
+      </c>
+      <c r="N4" s="10">
+        <v>2000</v>
+      </c>
       <c r="O4" s="10">
-        <v>100</v>
-      </c>
-      <c r="P4" s="10">
-        <v>2000</v>
-      </c>
-      <c r="Q4" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>31</v>
@@ -6008,30 +5649,28 @@
       <c r="E5" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10" t="s">
+      <c r="F5" s="10" t="s">
         <v>3</v>
       </c>
+      <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
+      <c r="J5" s="11"/>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
+      <c r="M5" s="10">
+        <v>0</v>
+      </c>
+      <c r="N5" s="10">
+        <v>1</v>
+      </c>
       <c r="O5" s="10">
-        <v>0</v>
-      </c>
-      <c r="P5" s="10">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="10">
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>38</v>
@@ -6045,91 +5684,89 @@
       <c r="E6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10" t="s">
+      <c r="F6" s="10" t="s">
         <v>3</v>
       </c>
+      <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="14"/>
       <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
+      <c r="M6" s="13">
+        <v>0</v>
+      </c>
+      <c r="N6" s="13">
+        <v>10</v>
+      </c>
       <c r="O6" s="13">
-        <v>0</v>
-      </c>
-      <c r="P6" s="13">
-        <v>10</v>
-      </c>
-      <c r="Q6" s="13">
         <v>0.1</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="H2:N6">
-    <cfRule type="expression" dxfId="22" priority="33">
-      <formula>NOT((COLUMN(H2)-COLUMN($G:$G))&lt;=IFERROR(VLOOKUP($G2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+  <conditionalFormatting sqref="G2:L6">
+    <cfRule type="expression" dxfId="19" priority="33">
+      <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:C2 E2:N2 B6:C6 E6:N6 B3:N5">
-    <cfRule type="expression" dxfId="21" priority="42">
-      <formula>ISBLANK($G2)</formula>
+  <conditionalFormatting sqref="B2:C2 E2:L2 B6:C6 E6:L6 B3:L5">
+    <cfRule type="expression" dxfId="18" priority="42">
+      <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="20" priority="12">
-      <formula>ISBLANK($G2)</formula>
+    <cfRule type="expression" dxfId="17" priority="12">
+      <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="19" priority="11">
-      <formula>ISBLANK($G6)</formula>
+    <cfRule type="expression" dxfId="16" priority="11">
+      <formula>ISBLANK($F6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="18" priority="9">
-      <formula>ISBLANK($G2)</formula>
+    <cfRule type="expression" dxfId="15" priority="9">
+      <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="10">
-      <formula>NOT((COLUMN(A2)-COLUMN($G:$G))&lt;=IFERROR(VLOOKUP($G2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    <cfRule type="expression" dxfId="14" priority="10">
+      <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="expression" dxfId="16" priority="7">
-      <formula>ISBLANK($G3)</formula>
+    <cfRule type="expression" dxfId="13" priority="7">
+      <formula>ISBLANK($F3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="8">
-      <formula>NOT((COLUMN(A3)-COLUMN($G:$G))&lt;=IFERROR(VLOOKUP($G3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    <cfRule type="expression" dxfId="12" priority="8">
+      <formula>NOT((COLUMN(A3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="expression" dxfId="14" priority="5">
-      <formula>ISBLANK($G4)</formula>
+    <cfRule type="expression" dxfId="11" priority="5">
+      <formula>ISBLANK($F4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="6">
-      <formula>NOT((COLUMN(A4)-COLUMN($G:$G))&lt;=IFERROR(VLOOKUP($G4, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    <cfRule type="expression" dxfId="10" priority="6">
+      <formula>NOT((COLUMN(A4)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F4, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="expression" dxfId="12" priority="3">
-      <formula>ISBLANK($G5)</formula>
+    <cfRule type="expression" dxfId="9" priority="3">
+      <formula>ISBLANK($F5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="4">
-      <formula>NOT((COLUMN(A5)-COLUMN($G:$G))&lt;=IFERROR(VLOOKUP($G5, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    <cfRule type="expression" dxfId="8" priority="4">
+      <formula>NOT((COLUMN(A5)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F5, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="expression" dxfId="10" priority="1">
-      <formula>ISBLANK($G6)</formula>
+    <cfRule type="expression" dxfId="7" priority="1">
+      <formula>ISBLANK($F6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="2">
-      <formula>NOT((COLUMN(A6)-COLUMN($G:$G))&lt;=IFERROR(VLOOKUP($G6, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>NOT((COLUMN(A6)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F6, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G2:G6" xr:uid="{00000000-0002-0000-0700-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F6" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>Validation_Distribution_Types</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Refactored sheets based on new format
</commit_message>
<xml_diff>
--- a/InputFiles/DefineScenario.xlsx
+++ b/InputFiles/DefineScenario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\EPA\WideAreaDecon\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94096A9C-973A-4A08-9C16-514CFB20D764}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A41AE93-BF8E-4E71-81BD-3952684F538B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4353,7 +4353,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added necessary parameters to all input files
</commit_message>
<xml_diff>
--- a/InputFiles/DefineScenario.xlsx
+++ b/InputFiles/DefineScenario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERAZA\Documents\Tasking\(4) EPA Stuff\Task 5 Repo\WideAreaDecon\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0513E95-B7B6-4D29-9F89-35422BBA0171}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359F83A2-ABED-4C38-A0FC-068D44CCCDCE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal - File Info" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="135">
   <si>
     <t>SCWAD</t>
   </si>
@@ -439,6 +439,15 @@
   </si>
   <si>
     <t>Surface Area to be Source Reduced</t>
+  </si>
+  <si>
+    <t>Rental Car Cost</t>
+  </si>
+  <si>
+    <t>Cost of rental car per day</t>
+  </si>
+  <si>
+    <t>$ / day</t>
   </si>
 </sst>
 </file>
@@ -720,7 +729,25 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="157">
+  <dxfs count="159">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -3266,171 +3293,171 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{77E3C927-1FC6-443B-87ED-00E2959DD317}" name="Table1568" displayName="Table1568" ref="A1:O4" totalsRowShown="0" tableBorderDxfId="154">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{77E3C927-1FC6-443B-87ED-00E2959DD317}" name="Table1568" displayName="Table1568" ref="A1:O4" totalsRowShown="0" tableBorderDxfId="156">
   <autoFilter ref="A1:O4" xr:uid="{58F00973-C0E2-47D9-9C5E-C7B7F684A0C3}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{62A6D655-D638-4005-9525-C140421ED9AB}" name="Phase" dataDxfId="153"/>
-    <tableColumn id="1" xr3:uid="{1BC04ADD-0426-4785-9F97-FCE0BCC1E547}" name="Category" dataDxfId="152"/>
-    <tableColumn id="2" xr3:uid="{3089FC2E-257C-4BA5-A9A7-5D0E01D5E6F5}" name="Name" dataDxfId="151"/>
-    <tableColumn id="10" xr3:uid="{E1A27E6E-82E5-4CF6-9164-A680FF7F05A5}" name="Description" dataDxfId="150"/>
-    <tableColumn id="3" xr3:uid="{BA85C23F-8236-43E3-885F-DF8CCDB84F06}" name="Units" dataDxfId="149"/>
-    <tableColumn id="4" xr3:uid="{9121EDDE-A8D8-4E28-AAAC-953CC1A14CB2}" name="Distribution Type" dataDxfId="148"/>
-    <tableColumn id="5" xr3:uid="{67D6DF1C-45B3-456F-B960-B8F495F6867D}" name="Parameter 1" dataDxfId="147"/>
-    <tableColumn id="6" xr3:uid="{A2BB8730-6626-47D8-AABB-90C19B218AFB}" name="Parameter 2" dataDxfId="146"/>
-    <tableColumn id="7" xr3:uid="{B7BC4EB1-7616-4A3A-899A-F01A87DD3B48}" name="Parameter 3" dataDxfId="145"/>
-    <tableColumn id="8" xr3:uid="{32D71C9B-2B39-4A83-9EB0-1934F2F6FC91}" name="Parameter 4" dataDxfId="144"/>
-    <tableColumn id="14" xr3:uid="{31AC778C-1A4A-45DD-8A12-F22858D3CD3A}" name="Parameter 5" dataDxfId="143"/>
-    <tableColumn id="15" xr3:uid="{91C3BDC4-4893-4CF7-9830-76CC4A9BF6F1}" name="Parameter 6" dataDxfId="142"/>
-    <tableColumn id="11" xr3:uid="{6BCEB05C-9FCE-48DE-91F0-D2ACC21C6C3E}" name="Lower Limit" dataDxfId="141"/>
-    <tableColumn id="12" xr3:uid="{CDC89704-43FE-407F-B8B4-079E5E991263}" name="Upper Limit" dataDxfId="140"/>
-    <tableColumn id="13" xr3:uid="{0758CB79-3F38-44D8-B78B-CC33BB1D2C70}" name="Step" dataDxfId="139"/>
+    <tableColumn id="9" xr3:uid="{62A6D655-D638-4005-9525-C140421ED9AB}" name="Phase" dataDxfId="155"/>
+    <tableColumn id="1" xr3:uid="{1BC04ADD-0426-4785-9F97-FCE0BCC1E547}" name="Category" dataDxfId="154"/>
+    <tableColumn id="2" xr3:uid="{3089FC2E-257C-4BA5-A9A7-5D0E01D5E6F5}" name="Name" dataDxfId="153"/>
+    <tableColumn id="10" xr3:uid="{E1A27E6E-82E5-4CF6-9164-A680FF7F05A5}" name="Description" dataDxfId="152"/>
+    <tableColumn id="3" xr3:uid="{BA85C23F-8236-43E3-885F-DF8CCDB84F06}" name="Units" dataDxfId="151"/>
+    <tableColumn id="4" xr3:uid="{9121EDDE-A8D8-4E28-AAAC-953CC1A14CB2}" name="Distribution Type" dataDxfId="150"/>
+    <tableColumn id="5" xr3:uid="{67D6DF1C-45B3-456F-B960-B8F495F6867D}" name="Parameter 1" dataDxfId="149"/>
+    <tableColumn id="6" xr3:uid="{A2BB8730-6626-47D8-AABB-90C19B218AFB}" name="Parameter 2" dataDxfId="148"/>
+    <tableColumn id="7" xr3:uid="{B7BC4EB1-7616-4A3A-899A-F01A87DD3B48}" name="Parameter 3" dataDxfId="147"/>
+    <tableColumn id="8" xr3:uid="{32D71C9B-2B39-4A83-9EB0-1934F2F6FC91}" name="Parameter 4" dataDxfId="146"/>
+    <tableColumn id="14" xr3:uid="{31AC778C-1A4A-45DD-8A12-F22858D3CD3A}" name="Parameter 5" dataDxfId="145"/>
+    <tableColumn id="15" xr3:uid="{91C3BDC4-4893-4CF7-9830-76CC4A9BF6F1}" name="Parameter 6" dataDxfId="144"/>
+    <tableColumn id="11" xr3:uid="{6BCEB05C-9FCE-48DE-91F0-D2ACC21C6C3E}" name="Lower Limit" dataDxfId="143"/>
+    <tableColumn id="12" xr3:uid="{CDC89704-43FE-407F-B8B4-079E5E991263}" name="Upper Limit" dataDxfId="142"/>
+    <tableColumn id="13" xr3:uid="{0758CB79-3F38-44D8-B78B-CC33BB1D2C70}" name="Step" dataDxfId="141"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{B77B7895-2678-4EA1-91B2-B6248E05AA0A}" name="Table156810" displayName="Table156810" ref="A1:O8" totalsRowShown="0" tableBorderDxfId="136">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{B77B7895-2678-4EA1-91B2-B6248E05AA0A}" name="Table156810" displayName="Table156810" ref="A1:O8" totalsRowShown="0" tableBorderDxfId="138">
   <autoFilter ref="A1:O8" xr:uid="{60C5A2AF-4D3E-4976-AA8F-8961FE4EE49E}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{DF77AA95-0523-4660-B964-676ECCB79418}" name="Phase" dataDxfId="135"/>
-    <tableColumn id="1" xr3:uid="{423292BC-9F1E-4EDC-9CC2-9890D4B1F00A}" name="Category" dataDxfId="134"/>
-    <tableColumn id="2" xr3:uid="{916CDEF4-7288-42C6-AD00-C6D0D8F8D560}" name="Name" dataDxfId="133"/>
-    <tableColumn id="10" xr3:uid="{C69B0C1F-B3A6-4CB4-B855-8A573BA536A2}" name="Description" dataDxfId="132"/>
-    <tableColumn id="3" xr3:uid="{23E3372F-48DE-4E64-88D3-C7EE1A32F34A}" name="Units" dataDxfId="131"/>
-    <tableColumn id="4" xr3:uid="{9D790DCF-5822-477B-8DCC-93F90CAB183B}" name="Distribution Type" dataDxfId="130"/>
-    <tableColumn id="5" xr3:uid="{337DB99B-F988-4680-87F5-A4BCFAF1A3C2}" name="Parameter 1" dataDxfId="129"/>
-    <tableColumn id="6" xr3:uid="{8C90C787-B669-453A-8F0E-A46E3018D380}" name="Parameter 2" dataDxfId="128"/>
-    <tableColumn id="7" xr3:uid="{041FF432-9543-4EE3-A9CF-1500CC344FFA}" name="Parameter 3" dataDxfId="127"/>
-    <tableColumn id="8" xr3:uid="{CDC02AC4-4C95-4220-B404-681CADF416D2}" name="Parameter 4" dataDxfId="126"/>
-    <tableColumn id="14" xr3:uid="{97B53FFA-4984-4D47-817E-8D167978BD8D}" name="Parameter 5" dataDxfId="125"/>
-    <tableColumn id="15" xr3:uid="{823939D4-F4DD-4DB0-89DB-EF0A01ECB48B}" name="Parameter 6" dataDxfId="124"/>
-    <tableColumn id="11" xr3:uid="{20A93856-0EFF-4271-832C-04F7E9AC0A1E}" name="Lower Limit" dataDxfId="123"/>
-    <tableColumn id="12" xr3:uid="{A36F5215-EB9D-448B-AE9F-58A4F8E9D0C7}" name="Upper Limit" dataDxfId="122"/>
-    <tableColumn id="13" xr3:uid="{39173C83-06DA-436D-B107-9D64D97B7F39}" name="Step" dataDxfId="121"/>
+    <tableColumn id="9" xr3:uid="{DF77AA95-0523-4660-B964-676ECCB79418}" name="Phase" dataDxfId="137"/>
+    <tableColumn id="1" xr3:uid="{423292BC-9F1E-4EDC-9CC2-9890D4B1F00A}" name="Category" dataDxfId="136"/>
+    <tableColumn id="2" xr3:uid="{916CDEF4-7288-42C6-AD00-C6D0D8F8D560}" name="Name" dataDxfId="135"/>
+    <tableColumn id="10" xr3:uid="{C69B0C1F-B3A6-4CB4-B855-8A573BA536A2}" name="Description" dataDxfId="134"/>
+    <tableColumn id="3" xr3:uid="{23E3372F-48DE-4E64-88D3-C7EE1A32F34A}" name="Units" dataDxfId="133"/>
+    <tableColumn id="4" xr3:uid="{9D790DCF-5822-477B-8DCC-93F90CAB183B}" name="Distribution Type" dataDxfId="132"/>
+    <tableColumn id="5" xr3:uid="{337DB99B-F988-4680-87F5-A4BCFAF1A3C2}" name="Parameter 1" dataDxfId="131"/>
+    <tableColumn id="6" xr3:uid="{8C90C787-B669-453A-8F0E-A46E3018D380}" name="Parameter 2" dataDxfId="130"/>
+    <tableColumn id="7" xr3:uid="{041FF432-9543-4EE3-A9CF-1500CC344FFA}" name="Parameter 3" dataDxfId="129"/>
+    <tableColumn id="8" xr3:uid="{CDC02AC4-4C95-4220-B404-681CADF416D2}" name="Parameter 4" dataDxfId="128"/>
+    <tableColumn id="14" xr3:uid="{97B53FFA-4984-4D47-817E-8D167978BD8D}" name="Parameter 5" dataDxfId="127"/>
+    <tableColumn id="15" xr3:uid="{823939D4-F4DD-4DB0-89DB-EF0A01ECB48B}" name="Parameter 6" dataDxfId="126"/>
+    <tableColumn id="11" xr3:uid="{20A93856-0EFF-4271-832C-04F7E9AC0A1E}" name="Lower Limit" dataDxfId="125"/>
+    <tableColumn id="12" xr3:uid="{A36F5215-EB9D-448B-AE9F-58A4F8E9D0C7}" name="Upper Limit" dataDxfId="124"/>
+    <tableColumn id="13" xr3:uid="{39173C83-06DA-436D-B107-9D64D97B7F39}" name="Step" dataDxfId="123"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table156" displayName="Table156" ref="A1:O3" totalsRowShown="0" tableBorderDxfId="118">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table156" displayName="Table156" ref="A1:O3" totalsRowShown="0" tableBorderDxfId="120">
   <autoFilter ref="A1:O3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Phase" dataDxfId="117"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Category" dataDxfId="116"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="115"/>
-    <tableColumn id="10" xr3:uid="{115A314C-6A1B-4509-AD17-EBA48B227F1D}" name="Description" dataDxfId="114"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Units" dataDxfId="113"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Distribution Type" dataDxfId="112"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Parameter 1" dataDxfId="111"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Parameter 2" dataDxfId="110"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Parameter 3" dataDxfId="109"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Parameter 4" dataDxfId="108"/>
-    <tableColumn id="14" xr3:uid="{D27F5CDB-A68A-4129-930A-F29B15C22636}" name="Parameter 5" dataDxfId="107"/>
-    <tableColumn id="15" xr3:uid="{0AB42936-B3F8-4E7C-8152-8CB99EFF7215}" name="Parameter 6" dataDxfId="106"/>
-    <tableColumn id="11" xr3:uid="{1D961365-C163-4709-AB34-FA18998E1C0C}" name="Lower Limit" dataDxfId="105"/>
-    <tableColumn id="12" xr3:uid="{DD91A285-8CA3-48CC-8B2D-6AD307B1829A}" name="Upper Limit" dataDxfId="104"/>
-    <tableColumn id="13" xr3:uid="{289708CC-2479-44B9-8E21-211759607199}" name="Step" dataDxfId="103"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Phase" dataDxfId="119"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Category" dataDxfId="118"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Name" dataDxfId="117"/>
+    <tableColumn id="10" xr3:uid="{115A314C-6A1B-4509-AD17-EBA48B227F1D}" name="Description" dataDxfId="116"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Units" dataDxfId="115"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Distribution Type" dataDxfId="114"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Parameter 1" dataDxfId="113"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Parameter 2" dataDxfId="112"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Parameter 3" dataDxfId="111"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Parameter 4" dataDxfId="110"/>
+    <tableColumn id="14" xr3:uid="{D27F5CDB-A68A-4129-930A-F29B15C22636}" name="Parameter 5" dataDxfId="109"/>
+    <tableColumn id="15" xr3:uid="{0AB42936-B3F8-4E7C-8152-8CB99EFF7215}" name="Parameter 6" dataDxfId="108"/>
+    <tableColumn id="11" xr3:uid="{1D961365-C163-4709-AB34-FA18998E1C0C}" name="Lower Limit" dataDxfId="107"/>
+    <tableColumn id="12" xr3:uid="{DD91A285-8CA3-48CC-8B2D-6AD307B1829A}" name="Upper Limit" dataDxfId="106"/>
+    <tableColumn id="13" xr3:uid="{289708CC-2479-44B9-8E21-211759607199}" name="Step" dataDxfId="105"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table15" displayName="Table15" ref="A1:O4" totalsRowShown="0" tableBorderDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table15" displayName="Table15" ref="A1:O4" totalsRowShown="0" tableBorderDxfId="96">
   <autoFilter ref="A1:O4" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Phase" dataDxfId="93"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Category" dataDxfId="92"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="91"/>
-    <tableColumn id="10" xr3:uid="{E238511C-0575-407F-83C7-4D6E37CAA1C8}" name="Description" dataDxfId="90"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Units" dataDxfId="89"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Distribution Type" dataDxfId="88"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Parameter 1" dataDxfId="87"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Parameter 2" dataDxfId="86"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Parameter 3" dataDxfId="85"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Parameter 4" dataDxfId="84"/>
-    <tableColumn id="14" xr3:uid="{0CCC8750-3EB9-4A09-95AB-3BEC14F064B0}" name="Parameter 5" dataDxfId="83"/>
-    <tableColumn id="15" xr3:uid="{8430512F-5835-4882-88A6-3BDD8313812B}" name="Parameter 6" dataDxfId="82"/>
-    <tableColumn id="11" xr3:uid="{1D5D06E3-C2FF-4E33-A67E-846C813585DD}" name="Lower Limit" dataDxfId="81"/>
-    <tableColumn id="12" xr3:uid="{59B419A3-4B50-4E25-9295-12F6E479C7C1}" name="Upper Limit" dataDxfId="80"/>
-    <tableColumn id="13" xr3:uid="{B44B2162-0D76-4003-8141-9F91F7CB1D51}" name="Step" dataDxfId="79"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Phase" dataDxfId="95"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Category" dataDxfId="94"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Name" dataDxfId="93"/>
+    <tableColumn id="10" xr3:uid="{E238511C-0575-407F-83C7-4D6E37CAA1C8}" name="Description" dataDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Units" dataDxfId="91"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Distribution Type" dataDxfId="90"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Parameter 1" dataDxfId="89"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Parameter 2" dataDxfId="88"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Parameter 3" dataDxfId="87"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Parameter 4" dataDxfId="86"/>
+    <tableColumn id="14" xr3:uid="{0CCC8750-3EB9-4A09-95AB-3BEC14F064B0}" name="Parameter 5" dataDxfId="85"/>
+    <tableColumn id="15" xr3:uid="{8430512F-5835-4882-88A6-3BDD8313812B}" name="Parameter 6" dataDxfId="84"/>
+    <tableColumn id="11" xr3:uid="{1D5D06E3-C2FF-4E33-A67E-846C813585DD}" name="Lower Limit" dataDxfId="83"/>
+    <tableColumn id="12" xr3:uid="{59B419A3-4B50-4E25-9295-12F6E479C7C1}" name="Upper Limit" dataDxfId="82"/>
+    <tableColumn id="13" xr3:uid="{B44B2162-0D76-4003-8141-9F91F7CB1D51}" name="Step" dataDxfId="81"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table157" displayName="Table157" ref="A1:O4" totalsRowShown="0" tableBorderDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table157" displayName="Table157" ref="A1:O4" totalsRowShown="0" tableBorderDxfId="71">
   <autoFilter ref="A1:O4" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Internal" dataDxfId="68"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Category" dataDxfId="67"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="66"/>
-    <tableColumn id="10" xr3:uid="{82317EA3-EFA1-4204-866F-27AD4E7F4565}" name="Description" dataDxfId="65"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Units" dataDxfId="64"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Distribution Type" dataDxfId="63"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Parameter 1" dataDxfId="62"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Parameter 2" dataDxfId="61"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Parameter 3" dataDxfId="60"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Parameter 4" dataDxfId="59"/>
-    <tableColumn id="14" xr3:uid="{66AAE767-9060-4329-9FA8-8309678C711A}" name="Parameter 5" dataDxfId="58"/>
-    <tableColumn id="15" xr3:uid="{EB2740C5-3F80-408E-8F68-D65D3DE04CB6}" name="Parameter 6" dataDxfId="57"/>
-    <tableColumn id="11" xr3:uid="{D8432F00-68F0-499E-8310-7BEAF2D5BFFA}" name="Lower Limit" dataDxfId="56"/>
-    <tableColumn id="12" xr3:uid="{BCED7806-F146-4B52-AF53-D5DE4EBA4D11}" name="Upper Limit" dataDxfId="55"/>
-    <tableColumn id="13" xr3:uid="{A3158C91-CCDA-42BB-98F8-B1415C87FD9F}" name="Step" dataDxfId="54"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0200-000009000000}" name="Internal" dataDxfId="70"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Category" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Name" dataDxfId="68"/>
+    <tableColumn id="10" xr3:uid="{82317EA3-EFA1-4204-866F-27AD4E7F4565}" name="Description" dataDxfId="67"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="Units" dataDxfId="66"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="Distribution Type" dataDxfId="65"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="Parameter 1" dataDxfId="64"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="Parameter 2" dataDxfId="63"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="Parameter 3" dataDxfId="62"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="Parameter 4" dataDxfId="61"/>
+    <tableColumn id="14" xr3:uid="{66AAE767-9060-4329-9FA8-8309678C711A}" name="Parameter 5" dataDxfId="60"/>
+    <tableColumn id="15" xr3:uid="{EB2740C5-3F80-408E-8F68-D65D3DE04CB6}" name="Parameter 6" dataDxfId="59"/>
+    <tableColumn id="11" xr3:uid="{D8432F00-68F0-499E-8310-7BEAF2D5BFFA}" name="Lower Limit" dataDxfId="58"/>
+    <tableColumn id="12" xr3:uid="{BCED7806-F146-4B52-AF53-D5DE4EBA4D11}" name="Upper Limit" dataDxfId="57"/>
+    <tableColumn id="13" xr3:uid="{A3158C91-CCDA-42BB-98F8-B1415C87FD9F}" name="Step" dataDxfId="56"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1579" displayName="Table1579" ref="A1:O6" totalsRowShown="0" headerRowBorderDxfId="39" tableBorderDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1579" displayName="Table1579" ref="A1:O6" totalsRowShown="0" headerRowBorderDxfId="41" tableBorderDxfId="40">
   <autoFilter ref="A1:O6" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Internal" dataDxfId="37"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Category" dataDxfId="36"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Name" dataDxfId="35"/>
-    <tableColumn id="10" xr3:uid="{832C45C5-9E76-4B8A-83B0-2EB32C68E2FD}" name="Description" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Units" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Distribution Type" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Parameter 1" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Parameter 2" dataDxfId="30"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Parameter 3" dataDxfId="29"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Parameter 4" dataDxfId="28"/>
-    <tableColumn id="14" xr3:uid="{1289F8CF-6170-44F2-AD7D-9E9A4F12BCD1}" name="Parameter 5" dataDxfId="27"/>
-    <tableColumn id="15" xr3:uid="{6D5C8F75-1A51-48AD-90E7-17A2F3986BE7}" name="Parameter 6" dataDxfId="26"/>
-    <tableColumn id="11" xr3:uid="{DB8C4311-5A85-4D8D-A5C2-F47C77E8643D}" name="Lower Limit" dataDxfId="25"/>
-    <tableColumn id="12" xr3:uid="{96A08B49-5A79-4F13-BC86-FC5E2B426E49}" name="Upper Limit" dataDxfId="24"/>
-    <tableColumn id="13" xr3:uid="{D4252238-C1B7-4D7A-B8C5-A52164228F94}" name="Step" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0300-000009000000}" name="Internal" dataDxfId="39"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Category" dataDxfId="38"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Name" dataDxfId="37"/>
+    <tableColumn id="10" xr3:uid="{832C45C5-9E76-4B8A-83B0-2EB32C68E2FD}" name="Description" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Units" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="Distribution Type" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="Parameter 1" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="Parameter 2" dataDxfId="32"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0300-000007000000}" name="Parameter 3" dataDxfId="31"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0300-000008000000}" name="Parameter 4" dataDxfId="30"/>
+    <tableColumn id="14" xr3:uid="{1289F8CF-6170-44F2-AD7D-9E9A4F12BCD1}" name="Parameter 5" dataDxfId="29"/>
+    <tableColumn id="15" xr3:uid="{6D5C8F75-1A51-48AD-90E7-17A2F3986BE7}" name="Parameter 6" dataDxfId="28"/>
+    <tableColumn id="11" xr3:uid="{DB8C4311-5A85-4D8D-A5C2-F47C77E8643D}" name="Lower Limit" dataDxfId="27"/>
+    <tableColumn id="12" xr3:uid="{96A08B49-5A79-4F13-BC86-FC5E2B426E49}" name="Upper Limit" dataDxfId="26"/>
+    <tableColumn id="13" xr3:uid="{D4252238-C1B7-4D7A-B8C5-A52164228F94}" name="Step" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157910" displayName="Table157910" ref="A1:O3" totalsRowShown="0" headerRowBorderDxfId="16" tableBorderDxfId="15">
-  <autoFilter ref="A1:O3" xr:uid="{C58E5582-2A25-434F-8C6A-2EF9AC741C58}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table157910" displayName="Table157910" ref="A1:O4" totalsRowShown="0" headerRowBorderDxfId="18" tableBorderDxfId="17">
+  <autoFilter ref="A1:O4" xr:uid="{C58E5582-2A25-434F-8C6A-2EF9AC741C58}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J2">
     <sortCondition ref="B1:B2"/>
   </sortState>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="Internal" dataDxfId="14"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Category" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Name" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{63BA373B-667A-4A36-BB6C-997B9631910B}" name="Description" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Units" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Distribution Type" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Parameter 1" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Parameter 2" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Parameter 3" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Parameter 4" dataDxfId="5"/>
-    <tableColumn id="14" xr3:uid="{64E7458C-1D65-4712-ABFC-9DAF3D21B670}" name="Parameter 5" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{ABD8345F-8CFE-4FF4-A3F7-F6DB1042FE28}" name="Parameter 6" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{B286B466-1F40-4449-900C-61ACE92313F0}" name="Lower Limit" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{4CAE3350-4ABC-40B6-B059-3A8198700CE1}" name="Upper Limit" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{BC38CFEA-8053-4CB7-B237-C848302F26B7}" name="Step" dataDxfId="0"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="Internal" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Category" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Name" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{63BA373B-667A-4A36-BB6C-997B9631910B}" name="Description" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Units" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Distribution Type" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Parameter 1" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Parameter 2" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Parameter 3" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Parameter 4" dataDxfId="7"/>
+    <tableColumn id="14" xr3:uid="{64E7458C-1D65-4712-ABFC-9DAF3D21B670}" name="Parameter 5" dataDxfId="6"/>
+    <tableColumn id="15" xr3:uid="{ABD8345F-8CFE-4FF4-A3F7-F6DB1042FE28}" name="Parameter 6" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{B286B466-1F40-4449-900C-61ACE92313F0}" name="Lower Limit" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{4CAE3350-4ABC-40B6-B059-3A8198700CE1}" name="Upper Limit" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{BC38CFEA-8053-4CB7-B237-C848302F26B7}" name="Step" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3758,10 +3785,10 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Sheet10"/>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3889,36 +3916,65 @@
         <v>0.1</v>
       </c>
     </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="13"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="G2:L3">
-    <cfRule type="expression" dxfId="22" priority="33">
+  <conditionalFormatting sqref="G2:L4">
+    <cfRule type="expression" dxfId="24" priority="33">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="expression" dxfId="21" priority="1">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>ISBLANK($F3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="2">
+    <cfRule type="expression" dxfId="22" priority="2">
       <formula>NOT((COLUMN(A3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="19" priority="3">
+    <cfRule type="expression" dxfId="21" priority="3">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="4">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:L3">
-    <cfRule type="expression" dxfId="17" priority="50">
+  <conditionalFormatting sqref="B2:L4">
+    <cfRule type="expression" dxfId="19" priority="50">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F3" xr:uid="{00000000-0002-0000-0900-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F4" xr:uid="{00000000-0002-0000-0900-000000000000}">
       <formula1>Validation_Distribution_Types</formula1>
     </dataValidation>
   </dataValidations>
@@ -3934,7 +3990,7 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -4493,10 +4549,10 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A2:L4">
-    <cfRule type="expression" dxfId="156" priority="43">
+    <cfRule type="expression" dxfId="158" priority="43">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="155" priority="44">
+    <cfRule type="expression" dxfId="157" priority="44">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4837,10 +4893,10 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A2:L8">
-    <cfRule type="expression" dxfId="138" priority="45">
+    <cfRule type="expression" dxfId="140" priority="45">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="137" priority="46">
+    <cfRule type="expression" dxfId="139" priority="46">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4993,10 +5049,10 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A2:L3">
-    <cfRule type="expression" dxfId="120" priority="47">
+    <cfRule type="expression" dxfId="122" priority="47">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="119" priority="48">
+    <cfRule type="expression" dxfId="121" priority="48">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5185,36 +5241,36 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G2:L4">
-    <cfRule type="expression" dxfId="102" priority="23">
+    <cfRule type="expression" dxfId="104" priority="23">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="101" priority="5">
+    <cfRule type="expression" dxfId="103" priority="5">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="100" priority="6">
+    <cfRule type="expression" dxfId="102" priority="6">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="expression" dxfId="99" priority="3">
+    <cfRule type="expression" dxfId="101" priority="3">
       <formula>ISBLANK($F3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="4">
+    <cfRule type="expression" dxfId="100" priority="4">
       <formula>NOT((COLUMN(A3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="expression" dxfId="97" priority="1">
+    <cfRule type="expression" dxfId="99" priority="1">
       <formula>ISBLANK($F4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="96" priority="2">
+    <cfRule type="expression" dxfId="98" priority="2">
       <formula>NOT((COLUMN(A4)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F4, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:L4">
-    <cfRule type="expression" dxfId="95" priority="49">
+    <cfRule type="expression" dxfId="97" priority="49">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5402,41 +5458,41 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G2:L4">
-    <cfRule type="expression" dxfId="78" priority="25">
+    <cfRule type="expression" dxfId="80" priority="25">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:C4 E4:L4 B2:L3">
-    <cfRule type="expression" dxfId="77" priority="38">
+    <cfRule type="expression" dxfId="79" priority="38">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4">
-    <cfRule type="expression" dxfId="76" priority="7">
+    <cfRule type="expression" dxfId="78" priority="7">
       <formula>ISBLANK($F4)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="75" priority="5">
+    <cfRule type="expression" dxfId="77" priority="5">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="6">
+    <cfRule type="expression" dxfId="76" priority="6">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="expression" dxfId="73" priority="3">
+    <cfRule type="expression" dxfId="75" priority="3">
       <formula>ISBLANK($F3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="4">
+    <cfRule type="expression" dxfId="74" priority="4">
       <formula>NOT((COLUMN(A3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="expression" dxfId="71" priority="1">
+    <cfRule type="expression" dxfId="73" priority="1">
       <formula>ISBLANK($F4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="2">
+    <cfRule type="expression" dxfId="72" priority="2">
       <formula>NOT((COLUMN(A4)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F4, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5694,62 +5750,62 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="G2:L6">
-    <cfRule type="expression" dxfId="53" priority="33">
+    <cfRule type="expression" dxfId="55" priority="33">
       <formula>NOT((COLUMN(G2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:C2 E2:L2 B6:C6 E6:L6 B3:L5">
-    <cfRule type="expression" dxfId="52" priority="42">
+    <cfRule type="expression" dxfId="54" priority="42">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="expression" dxfId="51" priority="12">
+    <cfRule type="expression" dxfId="53" priority="12">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D6">
-    <cfRule type="expression" dxfId="50" priority="11">
+    <cfRule type="expression" dxfId="52" priority="11">
       <formula>ISBLANK($F6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="49" priority="9">
+    <cfRule type="expression" dxfId="51" priority="9">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="10">
+    <cfRule type="expression" dxfId="50" priority="10">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="expression" dxfId="47" priority="7">
+    <cfRule type="expression" dxfId="49" priority="7">
       <formula>ISBLANK($F3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="8">
+    <cfRule type="expression" dxfId="48" priority="8">
       <formula>NOT((COLUMN(A3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="expression" dxfId="45" priority="5">
+    <cfRule type="expression" dxfId="47" priority="5">
       <formula>ISBLANK($F4)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="6">
+    <cfRule type="expression" dxfId="46" priority="6">
       <formula>NOT((COLUMN(A4)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F4, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="expression" dxfId="43" priority="3">
+    <cfRule type="expression" dxfId="45" priority="3">
       <formula>ISBLANK($F5)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="4">
+    <cfRule type="expression" dxfId="44" priority="4">
       <formula>NOT((COLUMN(A5)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F5, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="expression" dxfId="41" priority="1">
+    <cfRule type="expression" dxfId="43" priority="1">
       <formula>ISBLANK($F6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="2">
+    <cfRule type="expression" dxfId="42" priority="2">
       <formula>NOT((COLUMN(A6)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F6, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Removed an incorrect underground surface type
</commit_message>
<xml_diff>
--- a/InputFiles/DefineScenario.xlsx
+++ b/InputFiles/DefineScenario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERAZA\Documents\Tasking\(4) EPA Stuff\Task 5 Repo\WideAreaDecon\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3397F9-B7B1-49ED-833A-05F609FD7ED4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53721C12-32F1-412B-8A22-DCBC7EEB101D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="649" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="741" uniqueCount="154">
   <si>
     <t>SCWAD</t>
   </si>
@@ -473,9 +473,6 @@
   </si>
   <si>
     <t>The fraction of surface underground which is miscellaneous</t>
-  </si>
-  <si>
-    <t>The fraction of surface underground which is HVAC</t>
   </si>
   <si>
     <t>Area Contaminated</t>
@@ -777,133 +774,7 @@
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="158">
-    <dxf>
-      <font>
-        <i/>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="144">
     <dxf>
       <font>
         <i/>
@@ -3414,192 +3285,192 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{77E3C927-1FC6-443B-87ED-00E2959DD317}" name="Table1568" displayName="Table1568" ref="A1:O33" totalsRowShown="0" tableBorderDxfId="157">
-  <autoFilter ref="A1:O33" xr:uid="{58F00973-C0E2-47D9-9C5E-C7B7F684A0C3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{77E3C927-1FC6-443B-87ED-00E2959DD317}" name="Table1568" displayName="Table1568" ref="A1:O32" totalsRowShown="0" tableBorderDxfId="143">
+  <autoFilter ref="A1:O32" xr:uid="{58F00973-C0E2-47D9-9C5E-C7B7F684A0C3}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{62A6D655-D638-4005-9525-C140421ED9AB}" name="Phase" dataDxfId="156"/>
-    <tableColumn id="1" xr3:uid="{1BC04ADD-0426-4785-9F97-FCE0BCC1E547}" name="Category" dataDxfId="155"/>
-    <tableColumn id="2" xr3:uid="{3089FC2E-257C-4BA5-A9A7-5D0E01D5E6F5}" name="Name" dataDxfId="154"/>
-    <tableColumn id="10" xr3:uid="{E1A27E6E-82E5-4CF6-9164-A680FF7F05A5}" name="Description" dataDxfId="153"/>
-    <tableColumn id="3" xr3:uid="{BA85C23F-8236-43E3-885F-DF8CCDB84F06}" name="Units" dataDxfId="152"/>
-    <tableColumn id="4" xr3:uid="{9121EDDE-A8D8-4E28-AAAC-953CC1A14CB2}" name="Distribution Type" dataDxfId="151"/>
-    <tableColumn id="5" xr3:uid="{67D6DF1C-45B3-456F-B960-B8F495F6867D}" name="Parameter 1" dataDxfId="150"/>
-    <tableColumn id="6" xr3:uid="{A2BB8730-6626-47D8-AABB-90C19B218AFB}" name="Parameter 2" dataDxfId="149"/>
-    <tableColumn id="7" xr3:uid="{B7BC4EB1-7616-4A3A-899A-F01A87DD3B48}" name="Parameter 3" dataDxfId="148"/>
-    <tableColumn id="8" xr3:uid="{32D71C9B-2B39-4A83-9EB0-1934F2F6FC91}" name="Parameter 4" dataDxfId="147"/>
-    <tableColumn id="14" xr3:uid="{31AC778C-1A4A-45DD-8A12-F22858D3CD3A}" name="Parameter 5" dataDxfId="146"/>
-    <tableColumn id="15" xr3:uid="{91C3BDC4-4893-4CF7-9830-76CC4A9BF6F1}" name="Parameter 6" dataDxfId="145"/>
-    <tableColumn id="11" xr3:uid="{6BCEB05C-9FCE-48DE-91F0-D2ACC21C6C3E}" name="Lower Limit" dataDxfId="144"/>
-    <tableColumn id="12" xr3:uid="{CDC89704-43FE-407F-B8B4-079E5E991263}" name="Upper Limit" dataDxfId="143"/>
-    <tableColumn id="13" xr3:uid="{0758CB79-3F38-44D8-B78B-CC33BB1D2C70}" name="Step" dataDxfId="142"/>
+    <tableColumn id="9" xr3:uid="{62A6D655-D638-4005-9525-C140421ED9AB}" name="Phase" dataDxfId="142"/>
+    <tableColumn id="1" xr3:uid="{1BC04ADD-0426-4785-9F97-FCE0BCC1E547}" name="Category" dataDxfId="141"/>
+    <tableColumn id="2" xr3:uid="{3089FC2E-257C-4BA5-A9A7-5D0E01D5E6F5}" name="Name" dataDxfId="140"/>
+    <tableColumn id="10" xr3:uid="{E1A27E6E-82E5-4CF6-9164-A680FF7F05A5}" name="Description" dataDxfId="139"/>
+    <tableColumn id="3" xr3:uid="{BA85C23F-8236-43E3-885F-DF8CCDB84F06}" name="Units" dataDxfId="138"/>
+    <tableColumn id="4" xr3:uid="{9121EDDE-A8D8-4E28-AAAC-953CC1A14CB2}" name="Distribution Type" dataDxfId="137"/>
+    <tableColumn id="5" xr3:uid="{67D6DF1C-45B3-456F-B960-B8F495F6867D}" name="Parameter 1" dataDxfId="136"/>
+    <tableColumn id="6" xr3:uid="{A2BB8730-6626-47D8-AABB-90C19B218AFB}" name="Parameter 2" dataDxfId="135"/>
+    <tableColumn id="7" xr3:uid="{B7BC4EB1-7616-4A3A-899A-F01A87DD3B48}" name="Parameter 3" dataDxfId="134"/>
+    <tableColumn id="8" xr3:uid="{32D71C9B-2B39-4A83-9EB0-1934F2F6FC91}" name="Parameter 4" dataDxfId="133"/>
+    <tableColumn id="14" xr3:uid="{31AC778C-1A4A-45DD-8A12-F22858D3CD3A}" name="Parameter 5" dataDxfId="132"/>
+    <tableColumn id="15" xr3:uid="{91C3BDC4-4893-4CF7-9830-76CC4A9BF6F1}" name="Parameter 6" dataDxfId="131"/>
+    <tableColumn id="11" xr3:uid="{6BCEB05C-9FCE-48DE-91F0-D2ACC21C6C3E}" name="Lower Limit" dataDxfId="130"/>
+    <tableColumn id="12" xr3:uid="{CDC89704-43FE-407F-B8B4-079E5E991263}" name="Upper Limit" dataDxfId="129"/>
+    <tableColumn id="13" xr3:uid="{0758CB79-3F38-44D8-B78B-CC33BB1D2C70}" name="Step" dataDxfId="128"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{72F3CA1E-AAFF-44BC-A114-2AA862291D9E}" name="Table1568102" displayName="Table1568102" ref="A1:O10" totalsRowShown="0" tableBorderDxfId="141">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{72F3CA1E-AAFF-44BC-A114-2AA862291D9E}" name="Table1568102" displayName="Table1568102" ref="A1:O10" totalsRowShown="0" tableBorderDxfId="127">
   <autoFilter ref="A1:O10" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{8FD38CEB-1D1A-41E8-821F-58DD4FBD85EB}" name="Phase" dataDxfId="140"/>
-    <tableColumn id="1" xr3:uid="{574AE483-6154-4EC6-AC18-5FDEBC0931CD}" name="Category" dataDxfId="139"/>
-    <tableColumn id="2" xr3:uid="{EC332146-FEF7-42A1-9698-0FB7656BE557}" name="Name" dataDxfId="138"/>
-    <tableColumn id="10" xr3:uid="{F0942CE2-9658-4EB8-A19F-B3B76B6A5F95}" name="Description" dataDxfId="137"/>
-    <tableColumn id="3" xr3:uid="{B909ADC8-9FD8-4714-A691-8AD0F1933057}" name="Units" dataDxfId="136"/>
-    <tableColumn id="4" xr3:uid="{F8B8B123-0CBC-450A-B098-9FFA08F7FC89}" name="Distribution Type" dataDxfId="135"/>
-    <tableColumn id="5" xr3:uid="{AADB8566-896F-40D4-8181-BB145E678F9B}" name="Parameter 1" dataDxfId="134"/>
-    <tableColumn id="6" xr3:uid="{13B0114C-55D3-4603-92C6-09319B7E315B}" name="Parameter 2" dataDxfId="133"/>
-    <tableColumn id="7" xr3:uid="{7548BB98-B29E-4F39-B198-D6F9994CC04D}" name="Parameter 3" dataDxfId="132"/>
-    <tableColumn id="8" xr3:uid="{355D4B98-B5B0-461B-90E8-3D81112B89E2}" name="Parameter 4" dataDxfId="131"/>
-    <tableColumn id="14" xr3:uid="{14667F24-6EC2-4F8F-8EAA-56B4FF372D98}" name="Parameter 5" dataDxfId="130"/>
-    <tableColumn id="15" xr3:uid="{B058DB6A-9C46-4ED3-9483-5713AD52AE40}" name="Parameter 6" dataDxfId="129"/>
-    <tableColumn id="11" xr3:uid="{0E22E7A3-8506-41E8-AC60-E103665C60A2}" name="Lower Limit" dataDxfId="128"/>
-    <tableColumn id="12" xr3:uid="{479761C6-7DBC-4557-9E7C-984A37ABCB8A}" name="Upper Limit" dataDxfId="127"/>
-    <tableColumn id="13" xr3:uid="{F96695B6-2ADD-458A-A424-B58482082C80}" name="Step" dataDxfId="126"/>
+    <tableColumn id="9" xr3:uid="{8FD38CEB-1D1A-41E8-821F-58DD4FBD85EB}" name="Phase" dataDxfId="126"/>
+    <tableColumn id="1" xr3:uid="{574AE483-6154-4EC6-AC18-5FDEBC0931CD}" name="Category" dataDxfId="125"/>
+    <tableColumn id="2" xr3:uid="{EC332146-FEF7-42A1-9698-0FB7656BE557}" name="Name" dataDxfId="124"/>
+    <tableColumn id="10" xr3:uid="{F0942CE2-9658-4EB8-A19F-B3B76B6A5F95}" name="Description" dataDxfId="123"/>
+    <tableColumn id="3" xr3:uid="{B909ADC8-9FD8-4714-A691-8AD0F1933057}" name="Units" dataDxfId="122"/>
+    <tableColumn id="4" xr3:uid="{F8B8B123-0CBC-450A-B098-9FFA08F7FC89}" name="Distribution Type" dataDxfId="121"/>
+    <tableColumn id="5" xr3:uid="{AADB8566-896F-40D4-8181-BB145E678F9B}" name="Parameter 1" dataDxfId="120"/>
+    <tableColumn id="6" xr3:uid="{13B0114C-55D3-4603-92C6-09319B7E315B}" name="Parameter 2" dataDxfId="119"/>
+    <tableColumn id="7" xr3:uid="{7548BB98-B29E-4F39-B198-D6F9994CC04D}" name="Parameter 3" dataDxfId="118"/>
+    <tableColumn id="8" xr3:uid="{355D4B98-B5B0-461B-90E8-3D81112B89E2}" name="Parameter 4" dataDxfId="117"/>
+    <tableColumn id="14" xr3:uid="{14667F24-6EC2-4F8F-8EAA-56B4FF372D98}" name="Parameter 5" dataDxfId="116"/>
+    <tableColumn id="15" xr3:uid="{B058DB6A-9C46-4ED3-9483-5713AD52AE40}" name="Parameter 6" dataDxfId="115"/>
+    <tableColumn id="11" xr3:uid="{0E22E7A3-8506-41E8-AC60-E103665C60A2}" name="Lower Limit" dataDxfId="114"/>
+    <tableColumn id="12" xr3:uid="{479761C6-7DBC-4557-9E7C-984A37ABCB8A}" name="Upper Limit" dataDxfId="113"/>
+    <tableColumn id="13" xr3:uid="{F96695B6-2ADD-458A-A424-B58482082C80}" name="Step" dataDxfId="112"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{88C3C7FF-7D66-4C1C-A80E-12CD3AFBFB8D}" name="Table156810210" displayName="Table156810210" ref="A1:O10" totalsRowShown="0" tableBorderDxfId="125">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{88C3C7FF-7D66-4C1C-A80E-12CD3AFBFB8D}" name="Table156810210" displayName="Table156810210" ref="A1:O10" totalsRowShown="0" tableBorderDxfId="111">
   <autoFilter ref="A1:O10" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{5AC7EE20-3F52-40E0-87F1-21D82A7C3AA2}" name="Phase" dataDxfId="124"/>
-    <tableColumn id="1" xr3:uid="{9A9754BC-4FF9-4BBA-B750-B911CE430E6A}" name="Category" dataDxfId="123"/>
-    <tableColumn id="2" xr3:uid="{0A114B0A-D97E-4073-8E4E-5B16FB19520E}" name="Name" dataDxfId="122"/>
-    <tableColumn id="10" xr3:uid="{D1A72F97-70A3-4EEB-9316-B31F108E3FD5}" name="Description" dataDxfId="121"/>
-    <tableColumn id="3" xr3:uid="{E8F09B1A-D952-4236-B6AD-8AC480554D73}" name="Units" dataDxfId="120"/>
-    <tableColumn id="4" xr3:uid="{B1DC9551-CBBD-4BF4-B876-9237E0FB121D}" name="Distribution Type" dataDxfId="119"/>
-    <tableColumn id="5" xr3:uid="{72C76302-CA88-4629-BF3A-72DD8971E0B7}" name="Parameter 1" dataDxfId="118"/>
-    <tableColumn id="6" xr3:uid="{C319BB6E-60FD-4F37-B898-C033C52FE070}" name="Parameter 2" dataDxfId="117"/>
-    <tableColumn id="7" xr3:uid="{B370DF9A-4768-49F1-B38B-F65D182A01B4}" name="Parameter 3" dataDxfId="116"/>
-    <tableColumn id="8" xr3:uid="{7BADEC71-6529-4D26-804E-5C9B93DA84E8}" name="Parameter 4" dataDxfId="115"/>
-    <tableColumn id="14" xr3:uid="{125149FE-86DA-4053-8A54-90E57B52F8B0}" name="Parameter 5" dataDxfId="114"/>
-    <tableColumn id="15" xr3:uid="{BAA75930-0A4F-4888-8CAF-A3AFA6F3FF44}" name="Parameter 6" dataDxfId="113"/>
-    <tableColumn id="11" xr3:uid="{7442F6EC-3907-41A8-BBEF-87C9374C67E5}" name="Lower Limit" dataDxfId="112"/>
-    <tableColumn id="12" xr3:uid="{86E2B2CA-B8F0-4FF5-8C59-2D3C44061DFD}" name="Upper Limit" dataDxfId="111"/>
-    <tableColumn id="13" xr3:uid="{C697FE06-06BB-49EC-93BB-FF753593319A}" name="Step" dataDxfId="110"/>
+    <tableColumn id="9" xr3:uid="{5AC7EE20-3F52-40E0-87F1-21D82A7C3AA2}" name="Phase" dataDxfId="110"/>
+    <tableColumn id="1" xr3:uid="{9A9754BC-4FF9-4BBA-B750-B911CE430E6A}" name="Category" dataDxfId="109"/>
+    <tableColumn id="2" xr3:uid="{0A114B0A-D97E-4073-8E4E-5B16FB19520E}" name="Name" dataDxfId="108"/>
+    <tableColumn id="10" xr3:uid="{D1A72F97-70A3-4EEB-9316-B31F108E3FD5}" name="Description" dataDxfId="107"/>
+    <tableColumn id="3" xr3:uid="{E8F09B1A-D952-4236-B6AD-8AC480554D73}" name="Units" dataDxfId="106"/>
+    <tableColumn id="4" xr3:uid="{B1DC9551-CBBD-4BF4-B876-9237E0FB121D}" name="Distribution Type" dataDxfId="105"/>
+    <tableColumn id="5" xr3:uid="{72C76302-CA88-4629-BF3A-72DD8971E0B7}" name="Parameter 1" dataDxfId="104"/>
+    <tableColumn id="6" xr3:uid="{C319BB6E-60FD-4F37-B898-C033C52FE070}" name="Parameter 2" dataDxfId="103"/>
+    <tableColumn id="7" xr3:uid="{B370DF9A-4768-49F1-B38B-F65D182A01B4}" name="Parameter 3" dataDxfId="102"/>
+    <tableColumn id="8" xr3:uid="{7BADEC71-6529-4D26-804E-5C9B93DA84E8}" name="Parameter 4" dataDxfId="101"/>
+    <tableColumn id="14" xr3:uid="{125149FE-86DA-4053-8A54-90E57B52F8B0}" name="Parameter 5" dataDxfId="100"/>
+    <tableColumn id="15" xr3:uid="{BAA75930-0A4F-4888-8CAF-A3AFA6F3FF44}" name="Parameter 6" dataDxfId="99"/>
+    <tableColumn id="11" xr3:uid="{7442F6EC-3907-41A8-BBEF-87C9374C67E5}" name="Lower Limit" dataDxfId="98"/>
+    <tableColumn id="12" xr3:uid="{86E2B2CA-B8F0-4FF5-8C59-2D3C44061DFD}" name="Upper Limit" dataDxfId="97"/>
+    <tableColumn id="13" xr3:uid="{C697FE06-06BB-49EC-93BB-FF753593319A}" name="Step" dataDxfId="96"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6794810C-E49F-4CB0-9B2F-0FA2655BD884}" name="Table15681021011" displayName="Table15681021011" ref="A1:O10" totalsRowShown="0" tableBorderDxfId="109">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6794810C-E49F-4CB0-9B2F-0FA2655BD884}" name="Table15681021011" displayName="Table15681021011" ref="A1:O10" totalsRowShown="0" tableBorderDxfId="95">
   <autoFilter ref="A1:O10" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{5DEAB66E-0CAB-4BF7-B4EA-D8D12FB47328}" name="Phase" dataDxfId="108"/>
-    <tableColumn id="1" xr3:uid="{69C64F5C-9979-4ACA-9A42-C1032E3D98BA}" name="Category" dataDxfId="107"/>
-    <tableColumn id="2" xr3:uid="{D4385687-B64B-46FB-B987-6E74F19DC1AF}" name="Name" dataDxfId="106"/>
-    <tableColumn id="10" xr3:uid="{BE461B66-2B72-42A7-9F3F-5916187828CF}" name="Description" dataDxfId="105"/>
-    <tableColumn id="3" xr3:uid="{9EE711F7-7C5D-4C54-8A9A-D54F8833D434}" name="Units" dataDxfId="104"/>
-    <tableColumn id="4" xr3:uid="{6EAA6194-27E9-4B7C-8A4D-8C0FE7B617F4}" name="Distribution Type" dataDxfId="103"/>
-    <tableColumn id="5" xr3:uid="{75BC5E4C-C28D-4614-8AB6-165A9F7FE7CE}" name="Parameter 1" dataDxfId="102"/>
-    <tableColumn id="6" xr3:uid="{F5AD0C00-9187-4F91-ADA7-5B461FC355CE}" name="Parameter 2" dataDxfId="101"/>
-    <tableColumn id="7" xr3:uid="{34B0A2DF-5607-43F6-AA9E-1106CCB7621B}" name="Parameter 3" dataDxfId="100"/>
-    <tableColumn id="8" xr3:uid="{B0950426-083D-4CE9-A30E-9D71766BA154}" name="Parameter 4" dataDxfId="99"/>
-    <tableColumn id="14" xr3:uid="{88E7A84D-F80D-416C-9037-2E5927AE2697}" name="Parameter 5" dataDxfId="98"/>
-    <tableColumn id="15" xr3:uid="{E3DCF8BA-29B1-4A24-B6E6-DE9435CB3AC9}" name="Parameter 6" dataDxfId="97"/>
-    <tableColumn id="11" xr3:uid="{E8661EBF-62F4-4D4A-BCDC-7C8ABD4866B0}" name="Lower Limit" dataDxfId="96"/>
-    <tableColumn id="12" xr3:uid="{83DA3A0E-E097-4281-9822-6FE3F8FB0CDD}" name="Upper Limit" dataDxfId="95"/>
-    <tableColumn id="13" xr3:uid="{24B0E0E0-CA9C-4655-9B23-EA0BBD517B67}" name="Step" dataDxfId="94"/>
+    <tableColumn id="9" xr3:uid="{5DEAB66E-0CAB-4BF7-B4EA-D8D12FB47328}" name="Phase" dataDxfId="94"/>
+    <tableColumn id="1" xr3:uid="{69C64F5C-9979-4ACA-9A42-C1032E3D98BA}" name="Category" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{D4385687-B64B-46FB-B987-6E74F19DC1AF}" name="Name" dataDxfId="92"/>
+    <tableColumn id="10" xr3:uid="{BE461B66-2B72-42A7-9F3F-5916187828CF}" name="Description" dataDxfId="91"/>
+    <tableColumn id="3" xr3:uid="{9EE711F7-7C5D-4C54-8A9A-D54F8833D434}" name="Units" dataDxfId="90"/>
+    <tableColumn id="4" xr3:uid="{6EAA6194-27E9-4B7C-8A4D-8C0FE7B617F4}" name="Distribution Type" dataDxfId="89"/>
+    <tableColumn id="5" xr3:uid="{75BC5E4C-C28D-4614-8AB6-165A9F7FE7CE}" name="Parameter 1" dataDxfId="88"/>
+    <tableColumn id="6" xr3:uid="{F5AD0C00-9187-4F91-ADA7-5B461FC355CE}" name="Parameter 2" dataDxfId="87"/>
+    <tableColumn id="7" xr3:uid="{34B0A2DF-5607-43F6-AA9E-1106CCB7621B}" name="Parameter 3" dataDxfId="86"/>
+    <tableColumn id="8" xr3:uid="{B0950426-083D-4CE9-A30E-9D71766BA154}" name="Parameter 4" dataDxfId="85"/>
+    <tableColumn id="14" xr3:uid="{88E7A84D-F80D-416C-9037-2E5927AE2697}" name="Parameter 5" dataDxfId="84"/>
+    <tableColumn id="15" xr3:uid="{E3DCF8BA-29B1-4A24-B6E6-DE9435CB3AC9}" name="Parameter 6" dataDxfId="83"/>
+    <tableColumn id="11" xr3:uid="{E8661EBF-62F4-4D4A-BCDC-7C8ABD4866B0}" name="Lower Limit" dataDxfId="82"/>
+    <tableColumn id="12" xr3:uid="{83DA3A0E-E097-4281-9822-6FE3F8FB0CDD}" name="Upper Limit" dataDxfId="81"/>
+    <tableColumn id="13" xr3:uid="{24B0E0E0-CA9C-4655-9B23-EA0BBD517B67}" name="Step" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{81C05191-4139-4D49-BA19-E7D2B74357F9}" name="Table15681021012" displayName="Table15681021012" ref="A1:O10" totalsRowShown="0" tableBorderDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{81C05191-4139-4D49-BA19-E7D2B74357F9}" name="Table15681021012" displayName="Table15681021012" ref="A1:O10" totalsRowShown="0" tableBorderDxfId="79">
   <autoFilter ref="A1:O10" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{64A27C3D-2E18-40E6-9166-742BDA2B413C}" name="Phase" dataDxfId="92"/>
-    <tableColumn id="1" xr3:uid="{0243CFE4-EBE7-4500-A226-23C63BE2FB81}" name="Category" dataDxfId="91"/>
-    <tableColumn id="2" xr3:uid="{69F68BF8-9E6A-4766-AB29-A8B943A84522}" name="Name" dataDxfId="90"/>
-    <tableColumn id="10" xr3:uid="{1E4511F0-B286-4973-A437-9638677030CA}" name="Description" dataDxfId="89"/>
-    <tableColumn id="3" xr3:uid="{B80720A6-55E5-4A17-9FE9-9951AF480E02}" name="Units" dataDxfId="88"/>
-    <tableColumn id="4" xr3:uid="{54B33DED-7F55-4D76-B95F-B7050BBA4BD1}" name="Distribution Type" dataDxfId="87"/>
-    <tableColumn id="5" xr3:uid="{BC7C6514-68B9-48F6-9938-4088DF28B37C}" name="Parameter 1" dataDxfId="86"/>
-    <tableColumn id="6" xr3:uid="{4D372042-F7DE-4E72-A309-C4266E0FA9E8}" name="Parameter 2" dataDxfId="85"/>
-    <tableColumn id="7" xr3:uid="{8D92705D-1A42-46F5-89EA-C4113CC26587}" name="Parameter 3" dataDxfId="84"/>
-    <tableColumn id="8" xr3:uid="{13B56E18-7C36-4950-847A-A7544475E1D1}" name="Parameter 4" dataDxfId="83"/>
-    <tableColumn id="14" xr3:uid="{2649C7B2-1C48-4B13-969D-684D0045538B}" name="Parameter 5" dataDxfId="82"/>
-    <tableColumn id="15" xr3:uid="{5D6C4F8D-D31E-4EED-BABF-A0A688F3A916}" name="Parameter 6" dataDxfId="81"/>
-    <tableColumn id="11" xr3:uid="{1CB1896E-F77C-4DFC-9AB0-D0C102F3F80F}" name="Lower Limit" dataDxfId="80"/>
-    <tableColumn id="12" xr3:uid="{837665AD-748D-4B51-9CCA-780B67A76815}" name="Upper Limit" dataDxfId="79"/>
-    <tableColumn id="13" xr3:uid="{A8F2935C-D451-47EA-A1E1-1E4F0CAE8D87}" name="Step" dataDxfId="78"/>
+    <tableColumn id="9" xr3:uid="{64A27C3D-2E18-40E6-9166-742BDA2B413C}" name="Phase" dataDxfId="78"/>
+    <tableColumn id="1" xr3:uid="{0243CFE4-EBE7-4500-A226-23C63BE2FB81}" name="Category" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{69F68BF8-9E6A-4766-AB29-A8B943A84522}" name="Name" dataDxfId="76"/>
+    <tableColumn id="10" xr3:uid="{1E4511F0-B286-4973-A437-9638677030CA}" name="Description" dataDxfId="75"/>
+    <tableColumn id="3" xr3:uid="{B80720A6-55E5-4A17-9FE9-9951AF480E02}" name="Units" dataDxfId="74"/>
+    <tableColumn id="4" xr3:uid="{54B33DED-7F55-4D76-B95F-B7050BBA4BD1}" name="Distribution Type" dataDxfId="73"/>
+    <tableColumn id="5" xr3:uid="{BC7C6514-68B9-48F6-9938-4088DF28B37C}" name="Parameter 1" dataDxfId="72"/>
+    <tableColumn id="6" xr3:uid="{4D372042-F7DE-4E72-A309-C4266E0FA9E8}" name="Parameter 2" dataDxfId="71"/>
+    <tableColumn id="7" xr3:uid="{8D92705D-1A42-46F5-89EA-C4113CC26587}" name="Parameter 3" dataDxfId="70"/>
+    <tableColumn id="8" xr3:uid="{13B56E18-7C36-4950-847A-A7544475E1D1}" name="Parameter 4" dataDxfId="69"/>
+    <tableColumn id="14" xr3:uid="{2649C7B2-1C48-4B13-969D-684D0045538B}" name="Parameter 5" dataDxfId="68"/>
+    <tableColumn id="15" xr3:uid="{5D6C4F8D-D31E-4EED-BABF-A0A688F3A916}" name="Parameter 6" dataDxfId="67"/>
+    <tableColumn id="11" xr3:uid="{1CB1896E-F77C-4DFC-9AB0-D0C102F3F80F}" name="Lower Limit" dataDxfId="66"/>
+    <tableColumn id="12" xr3:uid="{837665AD-748D-4B51-9CCA-780B67A76815}" name="Upper Limit" dataDxfId="65"/>
+    <tableColumn id="13" xr3:uid="{A8F2935C-D451-47EA-A1E1-1E4F0CAE8D87}" name="Step" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{2EC220FC-5886-477C-8B2C-57082D8749AA}" name="Table1568102101213" displayName="Table1568102101213" ref="A1:O10" totalsRowShown="0" tableBorderDxfId="77">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{2EC220FC-5886-477C-8B2C-57082D8749AA}" name="Table1568102101213" displayName="Table1568102101213" ref="A1:O10" totalsRowShown="0" tableBorderDxfId="63">
   <autoFilter ref="A1:O10" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{525577E1-B46F-47FB-A042-A56D8D45D9AD}" name="Phase" dataDxfId="76"/>
-    <tableColumn id="1" xr3:uid="{30AFC0FE-4503-4A4B-91CA-E5B88AA24F98}" name="Category" dataDxfId="75"/>
-    <tableColumn id="2" xr3:uid="{6333C26F-3D36-4A65-8F1B-CC515ADCE181}" name="Name" dataDxfId="74"/>
-    <tableColumn id="10" xr3:uid="{057A52C2-DED0-48A5-8844-3950CD398F8D}" name="Description" dataDxfId="73"/>
-    <tableColumn id="3" xr3:uid="{EF447B65-8A6A-4F12-ABCB-7BFE84B734A9}" name="Units" dataDxfId="72"/>
-    <tableColumn id="4" xr3:uid="{6E658D46-B4D3-46B1-A15B-9F0095A7EADD}" name="Distribution Type" dataDxfId="71"/>
-    <tableColumn id="5" xr3:uid="{FE235A77-6EFF-4D9A-926F-ACE5D51D4BC8}" name="Parameter 1" dataDxfId="70"/>
-    <tableColumn id="6" xr3:uid="{26694561-3958-440C-BDDC-2DB16EB8A614}" name="Parameter 2" dataDxfId="69"/>
-    <tableColumn id="7" xr3:uid="{DA96F9A2-3DEB-4C42-BECF-B9C30ADA7428}" name="Parameter 3" dataDxfId="68"/>
-    <tableColumn id="8" xr3:uid="{5F8A48E3-9BBF-4210-88D8-F668C1FD845D}" name="Parameter 4" dataDxfId="67"/>
-    <tableColumn id="14" xr3:uid="{21514092-10F7-41E0-B078-A15175C73E93}" name="Parameter 5" dataDxfId="66"/>
-    <tableColumn id="15" xr3:uid="{8BFA8A6A-2BCB-4512-8B77-28D2C28FEEE3}" name="Parameter 6" dataDxfId="65"/>
-    <tableColumn id="11" xr3:uid="{9CB23DDB-2513-48F3-960F-EF0D57CD9724}" name="Lower Limit" dataDxfId="64"/>
-    <tableColumn id="12" xr3:uid="{EDE53E3A-8BAE-4FD6-9C38-CD4B63274C67}" name="Upper Limit" dataDxfId="63"/>
-    <tableColumn id="13" xr3:uid="{980D57FA-1EDD-484A-9D56-BF7EAA580C8D}" name="Step" dataDxfId="62"/>
+    <tableColumn id="9" xr3:uid="{525577E1-B46F-47FB-A042-A56D8D45D9AD}" name="Phase" dataDxfId="62"/>
+    <tableColumn id="1" xr3:uid="{30AFC0FE-4503-4A4B-91CA-E5B88AA24F98}" name="Category" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{6333C26F-3D36-4A65-8F1B-CC515ADCE181}" name="Name" dataDxfId="60"/>
+    <tableColumn id="10" xr3:uid="{057A52C2-DED0-48A5-8844-3950CD398F8D}" name="Description" dataDxfId="59"/>
+    <tableColumn id="3" xr3:uid="{EF447B65-8A6A-4F12-ABCB-7BFE84B734A9}" name="Units" dataDxfId="58"/>
+    <tableColumn id="4" xr3:uid="{6E658D46-B4D3-46B1-A15B-9F0095A7EADD}" name="Distribution Type" dataDxfId="57"/>
+    <tableColumn id="5" xr3:uid="{FE235A77-6EFF-4D9A-926F-ACE5D51D4BC8}" name="Parameter 1" dataDxfId="56"/>
+    <tableColumn id="6" xr3:uid="{26694561-3958-440C-BDDC-2DB16EB8A614}" name="Parameter 2" dataDxfId="55"/>
+    <tableColumn id="7" xr3:uid="{DA96F9A2-3DEB-4C42-BECF-B9C30ADA7428}" name="Parameter 3" dataDxfId="54"/>
+    <tableColumn id="8" xr3:uid="{5F8A48E3-9BBF-4210-88D8-F668C1FD845D}" name="Parameter 4" dataDxfId="53"/>
+    <tableColumn id="14" xr3:uid="{21514092-10F7-41E0-B078-A15175C73E93}" name="Parameter 5" dataDxfId="52"/>
+    <tableColumn id="15" xr3:uid="{8BFA8A6A-2BCB-4512-8B77-28D2C28FEEE3}" name="Parameter 6" dataDxfId="51"/>
+    <tableColumn id="11" xr3:uid="{9CB23DDB-2513-48F3-960F-EF0D57CD9724}" name="Lower Limit" dataDxfId="50"/>
+    <tableColumn id="12" xr3:uid="{EDE53E3A-8BAE-4FD6-9C38-CD4B63274C67}" name="Upper Limit" dataDxfId="49"/>
+    <tableColumn id="13" xr3:uid="{980D57FA-1EDD-484A-9D56-BF7EAA580C8D}" name="Step" dataDxfId="48"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3DDD9CB2-968B-4A43-A20B-C749950155AA}" name="Table156810210121314" displayName="Table156810210121314" ref="A1:O10" totalsRowShown="0" tableBorderDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3DDD9CB2-968B-4A43-A20B-C749950155AA}" name="Table156810210121314" displayName="Table156810210121314" ref="A1:O10" totalsRowShown="0" tableBorderDxfId="47">
   <autoFilter ref="A1:O10" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{6B814874-1824-4E56-A967-04F9F6F3E584}" name="Phase" dataDxfId="60"/>
-    <tableColumn id="1" xr3:uid="{FE1635BE-F6C3-4D5B-B06E-7A92EBAB074D}" name="Category" dataDxfId="59"/>
-    <tableColumn id="2" xr3:uid="{9C16A715-E236-4930-A633-7510E082392C}" name="Name" dataDxfId="58"/>
-    <tableColumn id="10" xr3:uid="{B556C16A-1909-46E7-BC6D-8479761F1F65}" name="Description" dataDxfId="57"/>
-    <tableColumn id="3" xr3:uid="{5EFB6F3C-9894-43AA-AFAC-1013F8F0714B}" name="Units" dataDxfId="56"/>
-    <tableColumn id="4" xr3:uid="{6E3C1049-1D84-4FD5-B7CF-1E130CD32BCA}" name="Distribution Type" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{57E979B1-A630-4AC5-8C4D-CED1A62F587D}" name="Parameter 1" dataDxfId="54"/>
-    <tableColumn id="6" xr3:uid="{C9EF8DDD-DA1F-44E2-AC90-B6993C60CF1F}" name="Parameter 2" dataDxfId="53"/>
-    <tableColumn id="7" xr3:uid="{6FEFD03F-983B-47E2-9525-7EDD875A9C7C}" name="Parameter 3" dataDxfId="52"/>
-    <tableColumn id="8" xr3:uid="{0B661DB2-D286-4AEE-88C3-124B37F1B246}" name="Parameter 4" dataDxfId="51"/>
-    <tableColumn id="14" xr3:uid="{08C4ACC8-5A7B-4864-96E4-CF69FD654892}" name="Parameter 5" dataDxfId="50"/>
-    <tableColumn id="15" xr3:uid="{5505BBCC-5C52-4400-9C19-9ED7DBB490B8}" name="Parameter 6" dataDxfId="49"/>
-    <tableColumn id="11" xr3:uid="{E151AC3B-28ED-4186-A803-48B7F8B7AE5B}" name="Lower Limit" dataDxfId="48"/>
-    <tableColumn id="12" xr3:uid="{223709CC-AD09-4677-85AC-DF8A1619BF81}" name="Upper Limit" dataDxfId="47"/>
-    <tableColumn id="13" xr3:uid="{5FAAB5F5-A70D-4A6B-BE36-5CC1FD787BC5}" name="Step" dataDxfId="46"/>
+    <tableColumn id="9" xr3:uid="{6B814874-1824-4E56-A967-04F9F6F3E584}" name="Phase" dataDxfId="46"/>
+    <tableColumn id="1" xr3:uid="{FE1635BE-F6C3-4D5B-B06E-7A92EBAB074D}" name="Category" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{9C16A715-E236-4930-A633-7510E082392C}" name="Name" dataDxfId="44"/>
+    <tableColumn id="10" xr3:uid="{B556C16A-1909-46E7-BC6D-8479761F1F65}" name="Description" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{5EFB6F3C-9894-43AA-AFAC-1013F8F0714B}" name="Units" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{6E3C1049-1D84-4FD5-B7CF-1E130CD32BCA}" name="Distribution Type" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{57E979B1-A630-4AC5-8C4D-CED1A62F587D}" name="Parameter 1" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{C9EF8DDD-DA1F-44E2-AC90-B6993C60CF1F}" name="Parameter 2" dataDxfId="39"/>
+    <tableColumn id="7" xr3:uid="{6FEFD03F-983B-47E2-9525-7EDD875A9C7C}" name="Parameter 3" dataDxfId="38"/>
+    <tableColumn id="8" xr3:uid="{0B661DB2-D286-4AEE-88C3-124B37F1B246}" name="Parameter 4" dataDxfId="37"/>
+    <tableColumn id="14" xr3:uid="{08C4ACC8-5A7B-4864-96E4-CF69FD654892}" name="Parameter 5" dataDxfId="36"/>
+    <tableColumn id="15" xr3:uid="{5505BBCC-5C52-4400-9C19-9ED7DBB490B8}" name="Parameter 6" dataDxfId="35"/>
+    <tableColumn id="11" xr3:uid="{E151AC3B-28ED-4186-A803-48B7F8B7AE5B}" name="Lower Limit" dataDxfId="34"/>
+    <tableColumn id="12" xr3:uid="{223709CC-AD09-4677-85AC-DF8A1619BF81}" name="Upper Limit" dataDxfId="33"/>
+    <tableColumn id="13" xr3:uid="{5FAAB5F5-A70D-4A6B-BE36-5CC1FD787BC5}" name="Step" dataDxfId="32"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{FBB513AC-2D2B-4552-8740-9D611743FE70}" name="Table15681021012131415" displayName="Table15681021012131415" ref="A1:O10" totalsRowShown="0" tableBorderDxfId="45">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{FBB513AC-2D2B-4552-8740-9D611743FE70}" name="Table15681021012131415" displayName="Table15681021012131415" ref="A1:O10" totalsRowShown="0" tableBorderDxfId="31">
   <autoFilter ref="A1:O10" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{2035FE2F-0A32-497E-B1E0-30D237A0E150}" name="Phase" dataDxfId="44"/>
-    <tableColumn id="1" xr3:uid="{F814DF41-D024-449F-AF42-62D43153FFB7}" name="Category" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{7DC8FB15-5985-4C4F-ADF3-7A17F5076A68}" name="Name" dataDxfId="42"/>
-    <tableColumn id="10" xr3:uid="{614B9103-CB85-46A8-93A4-7DE4EBCB5D2B}" name="Description" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{E1C6CE34-10C1-4516-B6D9-58BC2F148637}" name="Units" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{2DC3C549-6825-4F8C-B404-F2995425599E}" name="Distribution Type" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{805795A1-E0DE-4FCC-9EBD-DDCCA12F0793}" name="Parameter 1" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{8AEEFD06-21CF-4496-9CA8-A505BA5018C8}" name="Parameter 2" dataDxfId="37"/>
-    <tableColumn id="7" xr3:uid="{81F9FC74-65BB-4D24-8C32-944022DBFF45}" name="Parameter 3" dataDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{B80C3AAC-1FDC-42E7-B79C-4A7F876448A4}" name="Parameter 4" dataDxfId="35"/>
-    <tableColumn id="14" xr3:uid="{07C0D5EC-F968-40E1-8F17-889B90B82192}" name="Parameter 5" dataDxfId="34"/>
-    <tableColumn id="15" xr3:uid="{0302BE75-0A0F-489C-99C0-05DCDFC40A44}" name="Parameter 6" dataDxfId="33"/>
-    <tableColumn id="11" xr3:uid="{8B4A7C21-F1CF-4881-A5A6-4163F9C44F88}" name="Lower Limit" dataDxfId="32"/>
-    <tableColumn id="12" xr3:uid="{F4935CE7-6ADF-493E-B887-56BFE62D0ADC}" name="Upper Limit" dataDxfId="31"/>
-    <tableColumn id="13" xr3:uid="{5249EF7A-61B0-47D7-A1ED-48836EF45F76}" name="Step" dataDxfId="30"/>
+    <tableColumn id="9" xr3:uid="{2035FE2F-0A32-497E-B1E0-30D237A0E150}" name="Phase" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{F814DF41-D024-449F-AF42-62D43153FFB7}" name="Category" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{7DC8FB15-5985-4C4F-ADF3-7A17F5076A68}" name="Name" dataDxfId="28"/>
+    <tableColumn id="10" xr3:uid="{614B9103-CB85-46A8-93A4-7DE4EBCB5D2B}" name="Description" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{E1C6CE34-10C1-4516-B6D9-58BC2F148637}" name="Units" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{2DC3C549-6825-4F8C-B404-F2995425599E}" name="Distribution Type" dataDxfId="25"/>
+    <tableColumn id="5" xr3:uid="{805795A1-E0DE-4FCC-9EBD-DDCCA12F0793}" name="Parameter 1" dataDxfId="24"/>
+    <tableColumn id="6" xr3:uid="{8AEEFD06-21CF-4496-9CA8-A505BA5018C8}" name="Parameter 2" dataDxfId="23"/>
+    <tableColumn id="7" xr3:uid="{81F9FC74-65BB-4D24-8C32-944022DBFF45}" name="Parameter 3" dataDxfId="22"/>
+    <tableColumn id="8" xr3:uid="{B80C3AAC-1FDC-42E7-B79C-4A7F876448A4}" name="Parameter 4" dataDxfId="21"/>
+    <tableColumn id="14" xr3:uid="{07C0D5EC-F968-40E1-8F17-889B90B82192}" name="Parameter 5" dataDxfId="20"/>
+    <tableColumn id="15" xr3:uid="{0302BE75-0A0F-489C-99C0-05DCDFC40A44}" name="Parameter 6" dataDxfId="19"/>
+    <tableColumn id="11" xr3:uid="{8B4A7C21-F1CF-4881-A5A6-4163F9C44F88}" name="Lower Limit" dataDxfId="18"/>
+    <tableColumn id="12" xr3:uid="{F4935CE7-6ADF-493E-B887-56BFE62D0ADC}" name="Upper Limit" dataDxfId="17"/>
+    <tableColumn id="13" xr3:uid="{5249EF7A-61B0-47D7-A1ED-48836EF45F76}" name="Step" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5161,10 +5032,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097870CC-1A0F-461E-BDFD-29BDDFDDF05C}">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P32" sqref="P32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5231,7 +5102,7 @@
         <v>70</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>53</v>
@@ -5266,7 +5137,7 @@
         <v>70</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>93</v>
@@ -5301,7 +5172,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>52</v>
@@ -5336,7 +5207,7 @@
         <v>71</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>94</v>
@@ -5371,7 +5242,7 @@
         <v>72</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>73</v>
@@ -5406,7 +5277,7 @@
         <v>72</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>95</v>
@@ -5703,7 +5574,7 @@
         <v>120</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>68</v>
@@ -6101,16 +5972,16 @@
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>68</v>
@@ -6119,7 +5990,7 @@
         <v>3</v>
       </c>
       <c r="G26" s="12">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="H26" s="12"/>
       <c r="I26" s="12"/>
@@ -6141,13 +6012,13 @@
         <v>71</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>68</v>
@@ -6156,7 +6027,7 @@
         <v>3</v>
       </c>
       <c r="G27" s="12">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
@@ -6178,13 +6049,13 @@
         <v>71</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>68</v>
@@ -6193,7 +6064,7 @@
         <v>3</v>
       </c>
       <c r="G28" s="12">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
@@ -6215,10 +6086,10 @@
         <v>71</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D29" s="12" t="s">
         <v>150</v>
@@ -6230,7 +6101,7 @@
         <v>3</v>
       </c>
       <c r="G29" s="12">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
@@ -6252,13 +6123,13 @@
         <v>71</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>68</v>
@@ -6267,7 +6138,7 @@
         <v>3</v>
       </c>
       <c r="G30" s="12">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="H30" s="12"/>
       <c r="I30" s="12"/>
@@ -6289,13 +6160,13 @@
         <v>71</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C31" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="D31" s="12" t="s">
         <v>146</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>149</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>68</v>
@@ -6304,7 +6175,7 @@
         <v>3</v>
       </c>
       <c r="G31" s="12">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
@@ -6326,10 +6197,10 @@
         <v>71</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D32" s="12" t="s">
         <v>147</v>
@@ -6341,7 +6212,7 @@
         <v>3</v>
       </c>
       <c r="G32" s="12">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="H32" s="12"/>
       <c r="I32" s="12"/>
@@ -6358,46 +6229,9 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A33" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>148</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G33" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="16"/>
-      <c r="L33" s="16"/>
-      <c r="M33" s="12">
-        <v>0</v>
-      </c>
-      <c r="N33" s="12">
-        <v>1</v>
-      </c>
-      <c r="O33" s="12">
-        <v>0.01</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A2:L33">
+  <conditionalFormatting sqref="A2:L32">
     <cfRule type="expression" dxfId="15" priority="43">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
@@ -6406,7 +6240,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F33" xr:uid="{330BE9FB-867A-4350-A3CC-F1598E7F7C5E}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F32" xr:uid="{330BE9FB-867A-4350-A3CC-F1598E7F7C5E}">
       <formula1>Validation_Distribution_Types</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Changed pfu label to cfu
</commit_message>
<xml_diff>
--- a/InputFiles/DefineScenario.xlsx
+++ b/InputFiles/DefineScenario.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERAZA\Documents\Tasking\(4) EPA Stuff\Task 5 Repo\WideAreaDecon\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF94E6DA-6E64-47EF-BB5C-D8F87E1638DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE4FE90-1089-49B4-8F1D-E3C95D168FA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="649" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -340,9 +340,6 @@
     <t>Multiplier utilized to determine total loading in a residential building</t>
   </si>
   <si>
-    <t>log(pfu / m^2)</t>
-  </si>
-  <si>
     <t>Building Type Fraction</t>
   </si>
   <si>
@@ -509,6 +506,9 @@
   </si>
   <si>
     <t>The fraction of surface indoors which is building exterior</t>
+  </si>
+  <si>
+    <t>log(cfu / m^2)</t>
   </si>
 </sst>
 </file>
@@ -3905,13 +3905,13 @@
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -3939,13 +3939,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>68</v>
@@ -3976,13 +3976,13 @@
         <v>71</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>68</v>
@@ -4013,13 +4013,13 @@
         <v>71</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>68</v>
@@ -4050,13 +4050,13 @@
         <v>71</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>68</v>
@@ -4087,13 +4087,13 @@
         <v>71</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>68</v>
@@ -4124,13 +4124,13 @@
         <v>71</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>68</v>
@@ -4161,13 +4161,13 @@
         <v>71</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>68</v>
@@ -4321,13 +4321,13 @@
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -4355,13 +4355,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>68</v>
@@ -4392,13 +4392,13 @@
         <v>71</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>68</v>
@@ -4429,13 +4429,13 @@
         <v>71</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>68</v>
@@ -4466,13 +4466,13 @@
         <v>71</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>68</v>
@@ -4503,13 +4503,13 @@
         <v>71</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>68</v>
@@ -4540,13 +4540,13 @@
         <v>71</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>68</v>
@@ -4577,13 +4577,13 @@
         <v>71</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>68</v>
@@ -4874,12 +4874,12 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -5037,8 +5037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097870CC-1A0F-461E-BDFD-29BDDFDDF05C}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5105,7 +5105,7 @@
         <v>70</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>53</v>
@@ -5140,13 +5140,13 @@
         <v>70</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>93</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>98</v>
+        <v>154</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>3</v>
@@ -5175,7 +5175,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>52</v>
@@ -5210,13 +5210,13 @@
         <v>71</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>94</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>98</v>
+        <v>154</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>3</v>
@@ -5245,7 +5245,7 @@
         <v>72</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>73</v>
@@ -5280,13 +5280,13 @@
         <v>72</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>95</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>98</v>
+        <v>154</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>3</v>
@@ -5315,7 +5315,7 @@
         <v>54</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D8" s="9" t="s">
         <v>61</v>
@@ -5352,7 +5352,7 @@
         <v>55</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D9" s="9" t="s">
         <v>62</v>
@@ -5389,7 +5389,7 @@
         <v>56</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D10" s="9" t="s">
         <v>63</v>
@@ -5426,7 +5426,7 @@
         <v>57</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D11" s="9" t="s">
         <v>64</v>
@@ -5463,7 +5463,7 @@
         <v>58</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>65</v>
@@ -5500,7 +5500,7 @@
         <v>59</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>66</v>
@@ -5537,7 +5537,7 @@
         <v>60</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>67</v>
@@ -5571,13 +5571,13 @@
         <v>70</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>68</v>
@@ -5608,13 +5608,13 @@
         <v>70</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>68</v>
@@ -5645,13 +5645,13 @@
         <v>70</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>68</v>
@@ -5682,13 +5682,13 @@
         <v>70</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>68</v>
@@ -5719,13 +5719,13 @@
         <v>70</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>68</v>
@@ -5756,13 +5756,13 @@
         <v>70</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>68</v>
@@ -5793,13 +5793,13 @@
         <v>72</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>68</v>
@@ -5830,13 +5830,13 @@
         <v>72</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>68</v>
@@ -5867,13 +5867,13 @@
         <v>72</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>68</v>
@@ -5904,13 +5904,13 @@
         <v>72</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>68</v>
@@ -5941,13 +5941,13 @@
         <v>72</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>68</v>
@@ -5978,13 +5978,13 @@
         <v>72</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>68</v>
@@ -6015,13 +6015,13 @@
         <v>71</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>68</v>
@@ -6052,13 +6052,13 @@
         <v>71</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>68</v>
@@ -6089,13 +6089,13 @@
         <v>71</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>68</v>
@@ -6126,13 +6126,13 @@
         <v>71</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>68</v>
@@ -6163,13 +6163,13 @@
         <v>71</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>68</v>
@@ -6200,13 +6200,13 @@
         <v>71</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C32" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="D32" s="12" t="s">
         <v>146</v>
-      </c>
-      <c r="D32" s="12" t="s">
-        <v>147</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>68</v>
@@ -6237,13 +6237,13 @@
         <v>71</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E33" s="12" t="s">
         <v>68</v>
@@ -6398,13 +6398,13 @@
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -6432,13 +6432,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>68</v>
@@ -6469,13 +6469,13 @@
         <v>71</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>68</v>
@@ -6506,13 +6506,13 @@
         <v>71</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>68</v>
@@ -6543,13 +6543,13 @@
         <v>71</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>68</v>
@@ -6580,13 +6580,13 @@
         <v>71</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>68</v>
@@ -6617,13 +6617,13 @@
         <v>71</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>68</v>
@@ -6654,13 +6654,13 @@
         <v>71</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>68</v>
@@ -6814,13 +6814,13 @@
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -6848,13 +6848,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>68</v>
@@ -6885,13 +6885,13 @@
         <v>71</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>68</v>
@@ -6922,13 +6922,13 @@
         <v>71</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>68</v>
@@ -6959,13 +6959,13 @@
         <v>71</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>68</v>
@@ -6996,13 +6996,13 @@
         <v>71</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>68</v>
@@ -7033,13 +7033,13 @@
         <v>71</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>68</v>
@@ -7070,13 +7070,13 @@
         <v>71</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>68</v>
@@ -7230,13 +7230,13 @@
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -7264,13 +7264,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>68</v>
@@ -7301,13 +7301,13 @@
         <v>71</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>68</v>
@@ -7338,13 +7338,13 @@
         <v>71</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>68</v>
@@ -7375,13 +7375,13 @@
         <v>71</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>68</v>
@@ -7412,13 +7412,13 @@
         <v>71</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>68</v>
@@ -7449,13 +7449,13 @@
         <v>71</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>68</v>
@@ -7486,13 +7486,13 @@
         <v>71</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>68</v>
@@ -7646,13 +7646,13 @@
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -7680,13 +7680,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>68</v>
@@ -7717,13 +7717,13 @@
         <v>71</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>68</v>
@@ -7754,13 +7754,13 @@
         <v>71</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>68</v>
@@ -7791,13 +7791,13 @@
         <v>71</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>68</v>
@@ -7828,13 +7828,13 @@
         <v>71</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>68</v>
@@ -7865,13 +7865,13 @@
         <v>71</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>68</v>
@@ -7902,13 +7902,13 @@
         <v>71</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>68</v>
@@ -8062,13 +8062,13 @@
       </c>
       <c r="B3" s="11"/>
       <c r="C3" s="12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -8096,13 +8096,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>68</v>
@@ -8133,13 +8133,13 @@
         <v>71</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>68</v>
@@ -8170,13 +8170,13 @@
         <v>71</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>68</v>
@@ -8207,13 +8207,13 @@
         <v>71</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>68</v>
@@ -8244,13 +8244,13 @@
         <v>71</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>68</v>
@@ -8281,13 +8281,13 @@
         <v>71</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>68</v>
@@ -8318,13 +8318,13 @@
         <v>71</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E10" s="12" t="s">
         <v>68</v>

</xml_diff>

<commit_message>
Temporary file changes for model verification using BOTE input files
</commit_message>
<xml_diff>
--- a/InputFiles/DefineScenario.xlsx
+++ b/InputFiles/DefineScenario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERAZA\Documents\Tasking\(4) EPA Stuff\Task 5 Repo\WideAreaDecon\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERAZA\Box\TO 19F0117 Framework for Sampling\Task 5\Deliverables\(14) Verification Cases\BOTE Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204B93E7-23E3-4049-A574-62388FC408A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87BF2BF4-7A5C-4C26-9BFA-1DD32D46C09B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="649" firstSheet="7" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="649" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal - File Info" sheetId="1" r:id="rId1"/>
@@ -391,9 +391,6 @@
     <t>Fraction of residential buildings that are miscellaneous</t>
   </si>
   <si>
-    <t>log(PFU / m^2)</t>
-  </si>
-  <si>
     <t>Outdoor Surface Type Breakout</t>
   </si>
   <si>
@@ -500,6 +497,9 @@
   </si>
   <si>
     <t>Underground Walls</t>
+  </si>
+  <si>
+    <t>log(CFU / m^2)</t>
   </si>
 </sst>
 </file>
@@ -741,7 +741,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -763,12 +763,307 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="144">
+  <dxfs count="156">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <i/>
@@ -806,6 +1101,300 @@
       </fill>
     </dxf>
     <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <i/>
         <strike/>
@@ -842,6 +1431,300 @@
       </fill>
     </dxf>
     <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <i/>
         <strike/>
@@ -878,6 +1761,300 @@
       </fill>
     </dxf>
     <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <i/>
         <strike/>
@@ -1208,6 +2385,42 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border>
         <left style="thin">
           <color indexed="64"/>
@@ -1502,6 +2715,42 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <i/>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border>
         <left style="thin">
           <color indexed="64"/>
@@ -1782,18 +3031,36 @@
     <dxf>
       <border>
         <left style="medium">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </left>
         <right style="medium">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </right>
         <top style="medium">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </top>
         <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <border>
@@ -2076,1194 +3343,36 @@
     <dxf>
       <border>
         <left style="medium">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </left>
         <right style="medium">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </right>
         <top style="medium">
-          <color rgb="FF000000"/>
+          <color indexed="64"/>
         </top>
         <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+        <strike/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3279,72 +3388,72 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{77E3C927-1FC6-443B-87ED-00E2959DD317}" name="Table1568" displayName="Table1568" ref="A1:O32" totalsRowShown="0" tableBorderDxfId="143">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{77E3C927-1FC6-443B-87ED-00E2959DD317}" name="Table1568" displayName="Table1568" ref="A1:O32" totalsRowShown="0" tableBorderDxfId="153">
   <autoFilter ref="A1:O32" xr:uid="{58F00973-C0E2-47D9-9C5E-C7B7F684A0C3}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{62A6D655-D638-4005-9525-C140421ED9AB}" name="Phase" dataDxfId="142"/>
-    <tableColumn id="1" xr3:uid="{1BC04ADD-0426-4785-9F97-FCE0BCC1E547}" name="Category" dataDxfId="141"/>
-    <tableColumn id="2" xr3:uid="{3089FC2E-257C-4BA5-A9A7-5D0E01D5E6F5}" name="Name" dataDxfId="140"/>
-    <tableColumn id="10" xr3:uid="{E1A27E6E-82E5-4CF6-9164-A680FF7F05A5}" name="Description" dataDxfId="139"/>
-    <tableColumn id="3" xr3:uid="{BA85C23F-8236-43E3-885F-DF8CCDB84F06}" name="Units" dataDxfId="138"/>
-    <tableColumn id="4" xr3:uid="{9121EDDE-A8D8-4E28-AAAC-953CC1A14CB2}" name="Distribution Type" dataDxfId="137"/>
-    <tableColumn id="5" xr3:uid="{67D6DF1C-45B3-456F-B960-B8F495F6867D}" name="Parameter 1" dataDxfId="136"/>
-    <tableColumn id="6" xr3:uid="{A2BB8730-6626-47D8-AABB-90C19B218AFB}" name="Parameter 2" dataDxfId="135"/>
-    <tableColumn id="7" xr3:uid="{B7BC4EB1-7616-4A3A-899A-F01A87DD3B48}" name="Parameter 3" dataDxfId="134"/>
-    <tableColumn id="8" xr3:uid="{32D71C9B-2B39-4A83-9EB0-1934F2F6FC91}" name="Parameter 4" dataDxfId="133"/>
-    <tableColumn id="14" xr3:uid="{31AC778C-1A4A-45DD-8A12-F22858D3CD3A}" name="Parameter 5" dataDxfId="132"/>
-    <tableColumn id="15" xr3:uid="{91C3BDC4-4893-4CF7-9830-76CC4A9BF6F1}" name="Parameter 6" dataDxfId="131"/>
-    <tableColumn id="11" xr3:uid="{6BCEB05C-9FCE-48DE-91F0-D2ACC21C6C3E}" name="Lower Limit" dataDxfId="130"/>
-    <tableColumn id="12" xr3:uid="{CDC89704-43FE-407F-B8B4-079E5E991263}" name="Upper Limit" dataDxfId="129"/>
-    <tableColumn id="13" xr3:uid="{0758CB79-3F38-44D8-B78B-CC33BB1D2C70}" name="Step" dataDxfId="128"/>
+    <tableColumn id="9" xr3:uid="{62A6D655-D638-4005-9525-C140421ED9AB}" name="Phase" dataDxfId="152"/>
+    <tableColumn id="1" xr3:uid="{1BC04ADD-0426-4785-9F97-FCE0BCC1E547}" name="Category" dataDxfId="151"/>
+    <tableColumn id="2" xr3:uid="{3089FC2E-257C-4BA5-A9A7-5D0E01D5E6F5}" name="Name" dataDxfId="150"/>
+    <tableColumn id="10" xr3:uid="{E1A27E6E-82E5-4CF6-9164-A680FF7F05A5}" name="Description" dataDxfId="149"/>
+    <tableColumn id="3" xr3:uid="{BA85C23F-8236-43E3-885F-DF8CCDB84F06}" name="Units" dataDxfId="148"/>
+    <tableColumn id="4" xr3:uid="{9121EDDE-A8D8-4E28-AAAC-953CC1A14CB2}" name="Distribution Type" dataDxfId="147"/>
+    <tableColumn id="5" xr3:uid="{67D6DF1C-45B3-456F-B960-B8F495F6867D}" name="Parameter 1" dataDxfId="146"/>
+    <tableColumn id="6" xr3:uid="{A2BB8730-6626-47D8-AABB-90C19B218AFB}" name="Parameter 2" dataDxfId="145"/>
+    <tableColumn id="7" xr3:uid="{B7BC4EB1-7616-4A3A-899A-F01A87DD3B48}" name="Parameter 3" dataDxfId="144"/>
+    <tableColumn id="8" xr3:uid="{32D71C9B-2B39-4A83-9EB0-1934F2F6FC91}" name="Parameter 4" dataDxfId="143"/>
+    <tableColumn id="14" xr3:uid="{31AC778C-1A4A-45DD-8A12-F22858D3CD3A}" name="Parameter 5" dataDxfId="142"/>
+    <tableColumn id="15" xr3:uid="{91C3BDC4-4893-4CF7-9830-76CC4A9BF6F1}" name="Parameter 6" dataDxfId="141"/>
+    <tableColumn id="11" xr3:uid="{6BCEB05C-9FCE-48DE-91F0-D2ACC21C6C3E}" name="Lower Limit" dataDxfId="140"/>
+    <tableColumn id="12" xr3:uid="{CDC89704-43FE-407F-B8B4-079E5E991263}" name="Upper Limit" dataDxfId="139"/>
+    <tableColumn id="13" xr3:uid="{0758CB79-3F38-44D8-B78B-CC33BB1D2C70}" name="Step" dataDxfId="138"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{72F3CA1E-AAFF-44BC-A114-2AA862291D9E}" name="Table1568102" displayName="Table1568102" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="127">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{72F3CA1E-AAFF-44BC-A114-2AA862291D9E}" name="Table1568102" displayName="Table1568102" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="135">
   <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{8FD38CEB-1D1A-41E8-821F-58DD4FBD85EB}" name="Phase" dataDxfId="126"/>
-    <tableColumn id="1" xr3:uid="{574AE483-6154-4EC6-AC18-5FDEBC0931CD}" name="Category" dataDxfId="125"/>
-    <tableColumn id="2" xr3:uid="{EC332146-FEF7-42A1-9698-0FB7656BE557}" name="Name" dataDxfId="124"/>
-    <tableColumn id="10" xr3:uid="{F0942CE2-9658-4EB8-A19F-B3B76B6A5F95}" name="Description" dataDxfId="123"/>
-    <tableColumn id="3" xr3:uid="{B909ADC8-9FD8-4714-A691-8AD0F1933057}" name="Units" dataDxfId="122"/>
-    <tableColumn id="4" xr3:uid="{F8B8B123-0CBC-450A-B098-9FFA08F7FC89}" name="Distribution Type" dataDxfId="121"/>
-    <tableColumn id="5" xr3:uid="{AADB8566-896F-40D4-8181-BB145E678F9B}" name="Parameter 1" dataDxfId="120"/>
-    <tableColumn id="6" xr3:uid="{13B0114C-55D3-4603-92C6-09319B7E315B}" name="Parameter 2" dataDxfId="119"/>
-    <tableColumn id="7" xr3:uid="{7548BB98-B29E-4F39-B198-D6F9994CC04D}" name="Parameter 3" dataDxfId="118"/>
-    <tableColumn id="8" xr3:uid="{355D4B98-B5B0-461B-90E8-3D81112B89E2}" name="Parameter 4" dataDxfId="117"/>
-    <tableColumn id="14" xr3:uid="{14667F24-6EC2-4F8F-8EAA-56B4FF372D98}" name="Parameter 5" dataDxfId="116"/>
-    <tableColumn id="15" xr3:uid="{B058DB6A-9C46-4ED3-9483-5713AD52AE40}" name="Parameter 6" dataDxfId="115"/>
-    <tableColumn id="11" xr3:uid="{0E22E7A3-8506-41E8-AC60-E103665C60A2}" name="Lower Limit" dataDxfId="114"/>
-    <tableColumn id="12" xr3:uid="{479761C6-7DBC-4557-9E7C-984A37ABCB8A}" name="Upper Limit" dataDxfId="113"/>
-    <tableColumn id="13" xr3:uid="{F96695B6-2ADD-458A-A424-B58482082C80}" name="Step" dataDxfId="112"/>
+    <tableColumn id="9" xr3:uid="{8FD38CEB-1D1A-41E8-821F-58DD4FBD85EB}" name="Phase" dataDxfId="134"/>
+    <tableColumn id="1" xr3:uid="{574AE483-6154-4EC6-AC18-5FDEBC0931CD}" name="Category" dataDxfId="133"/>
+    <tableColumn id="2" xr3:uid="{EC332146-FEF7-42A1-9698-0FB7656BE557}" name="Name" dataDxfId="132"/>
+    <tableColumn id="10" xr3:uid="{F0942CE2-9658-4EB8-A19F-B3B76B6A5F95}" name="Description" dataDxfId="131"/>
+    <tableColumn id="3" xr3:uid="{B909ADC8-9FD8-4714-A691-8AD0F1933057}" name="Units" dataDxfId="130"/>
+    <tableColumn id="4" xr3:uid="{F8B8B123-0CBC-450A-B098-9FFA08F7FC89}" name="Distribution Type" dataDxfId="129"/>
+    <tableColumn id="5" xr3:uid="{AADB8566-896F-40D4-8181-BB145E678F9B}" name="Parameter 1" dataDxfId="128"/>
+    <tableColumn id="6" xr3:uid="{13B0114C-55D3-4603-92C6-09319B7E315B}" name="Parameter 2" dataDxfId="127"/>
+    <tableColumn id="7" xr3:uid="{7548BB98-B29E-4F39-B198-D6F9994CC04D}" name="Parameter 3" dataDxfId="126"/>
+    <tableColumn id="8" xr3:uid="{355D4B98-B5B0-461B-90E8-3D81112B89E2}" name="Parameter 4" dataDxfId="125"/>
+    <tableColumn id="14" xr3:uid="{14667F24-6EC2-4F8F-8EAA-56B4FF372D98}" name="Parameter 5" dataDxfId="124"/>
+    <tableColumn id="15" xr3:uid="{B058DB6A-9C46-4ED3-9483-5713AD52AE40}" name="Parameter 6" dataDxfId="123"/>
+    <tableColumn id="11" xr3:uid="{0E22E7A3-8506-41E8-AC60-E103665C60A2}" name="Lower Limit" dataDxfId="122"/>
+    <tableColumn id="12" xr3:uid="{479761C6-7DBC-4557-9E7C-984A37ABCB8A}" name="Upper Limit" dataDxfId="121"/>
+    <tableColumn id="13" xr3:uid="{F96695B6-2ADD-458A-A424-B58482082C80}" name="Step" dataDxfId="120"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{88C3C7FF-7D66-4C1C-A80E-12CD3AFBFB8D}" name="Table156810210" displayName="Table156810210" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="111">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{88C3C7FF-7D66-4C1C-A80E-12CD3AFBFB8D}" name="Table156810210" displayName="Table156810210" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="115">
   <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{5AC7EE20-3F52-40E0-87F1-21D82A7C3AA2}" name="Phase" dataDxfId="110"/>
-    <tableColumn id="1" xr3:uid="{9A9754BC-4FF9-4BBA-B750-B911CE430E6A}" name="Category" dataDxfId="109"/>
-    <tableColumn id="2" xr3:uid="{0A114B0A-D97E-4073-8E4E-5B16FB19520E}" name="Name" dataDxfId="108"/>
-    <tableColumn id="10" xr3:uid="{D1A72F97-70A3-4EEB-9316-B31F108E3FD5}" name="Description" dataDxfId="107"/>
-    <tableColumn id="3" xr3:uid="{E8F09B1A-D952-4236-B6AD-8AC480554D73}" name="Units" dataDxfId="106"/>
-    <tableColumn id="4" xr3:uid="{B1DC9551-CBBD-4BF4-B876-9237E0FB121D}" name="Distribution Type" dataDxfId="105"/>
-    <tableColumn id="5" xr3:uid="{72C76302-CA88-4629-BF3A-72DD8971E0B7}" name="Parameter 1" dataDxfId="104"/>
-    <tableColumn id="6" xr3:uid="{C319BB6E-60FD-4F37-B898-C033C52FE070}" name="Parameter 2" dataDxfId="103"/>
-    <tableColumn id="7" xr3:uid="{B370DF9A-4768-49F1-B38B-F65D182A01B4}" name="Parameter 3" dataDxfId="102"/>
-    <tableColumn id="8" xr3:uid="{7BADEC71-6529-4D26-804E-5C9B93DA84E8}" name="Parameter 4" dataDxfId="101"/>
-    <tableColumn id="14" xr3:uid="{125149FE-86DA-4053-8A54-90E57B52F8B0}" name="Parameter 5" dataDxfId="100"/>
-    <tableColumn id="15" xr3:uid="{BAA75930-0A4F-4888-8CAF-A3AFA6F3FF44}" name="Parameter 6" dataDxfId="99"/>
-    <tableColumn id="11" xr3:uid="{7442F6EC-3907-41A8-BBEF-87C9374C67E5}" name="Lower Limit" dataDxfId="98"/>
-    <tableColumn id="12" xr3:uid="{86E2B2CA-B8F0-4FF5-8C59-2D3C44061DFD}" name="Upper Limit" dataDxfId="97"/>
-    <tableColumn id="13" xr3:uid="{C697FE06-06BB-49EC-93BB-FF753593319A}" name="Step" dataDxfId="96"/>
+    <tableColumn id="9" xr3:uid="{5AC7EE20-3F52-40E0-87F1-21D82A7C3AA2}" name="Phase" dataDxfId="114"/>
+    <tableColumn id="1" xr3:uid="{9A9754BC-4FF9-4BBA-B750-B911CE430E6A}" name="Category" dataDxfId="113"/>
+    <tableColumn id="2" xr3:uid="{0A114B0A-D97E-4073-8E4E-5B16FB19520E}" name="Name" dataDxfId="112"/>
+    <tableColumn id="10" xr3:uid="{D1A72F97-70A3-4EEB-9316-B31F108E3FD5}" name="Description" dataDxfId="111"/>
+    <tableColumn id="3" xr3:uid="{E8F09B1A-D952-4236-B6AD-8AC480554D73}" name="Units" dataDxfId="110"/>
+    <tableColumn id="4" xr3:uid="{B1DC9551-CBBD-4BF4-B876-9237E0FB121D}" name="Distribution Type" dataDxfId="109"/>
+    <tableColumn id="5" xr3:uid="{72C76302-CA88-4629-BF3A-72DD8971E0B7}" name="Parameter 1" dataDxfId="108"/>
+    <tableColumn id="6" xr3:uid="{C319BB6E-60FD-4F37-B898-C033C52FE070}" name="Parameter 2" dataDxfId="107"/>
+    <tableColumn id="7" xr3:uid="{B370DF9A-4768-49F1-B38B-F65D182A01B4}" name="Parameter 3" dataDxfId="106"/>
+    <tableColumn id="8" xr3:uid="{7BADEC71-6529-4D26-804E-5C9B93DA84E8}" name="Parameter 4" dataDxfId="105"/>
+    <tableColumn id="14" xr3:uid="{125149FE-86DA-4053-8A54-90E57B52F8B0}" name="Parameter 5" dataDxfId="104"/>
+    <tableColumn id="15" xr3:uid="{BAA75930-0A4F-4888-8CAF-A3AFA6F3FF44}" name="Parameter 6" dataDxfId="103"/>
+    <tableColumn id="11" xr3:uid="{7442F6EC-3907-41A8-BBEF-87C9374C67E5}" name="Lower Limit" dataDxfId="102"/>
+    <tableColumn id="12" xr3:uid="{86E2B2CA-B8F0-4FF5-8C59-2D3C44061DFD}" name="Upper Limit" dataDxfId="101"/>
+    <tableColumn id="13" xr3:uid="{C697FE06-06BB-49EC-93BB-FF753593319A}" name="Step" dataDxfId="100"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3375,96 +3484,96 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{81C05191-4139-4D49-BA19-E7D2B74357F9}" name="Table15681021012" displayName="Table15681021012" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="79">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{81C05191-4139-4D49-BA19-E7D2B74357F9}" name="Table15681021012" displayName="Table15681021012" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="75">
   <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{64A27C3D-2E18-40E6-9166-742BDA2B413C}" name="Phase" dataDxfId="78"/>
-    <tableColumn id="1" xr3:uid="{0243CFE4-EBE7-4500-A226-23C63BE2FB81}" name="Category" dataDxfId="77"/>
-    <tableColumn id="2" xr3:uid="{69F68BF8-9E6A-4766-AB29-A8B943A84522}" name="Name" dataDxfId="76"/>
-    <tableColumn id="10" xr3:uid="{1E4511F0-B286-4973-A437-9638677030CA}" name="Description" dataDxfId="75"/>
-    <tableColumn id="3" xr3:uid="{B80720A6-55E5-4A17-9FE9-9951AF480E02}" name="Units" dataDxfId="74"/>
-    <tableColumn id="4" xr3:uid="{54B33DED-7F55-4D76-B95F-B7050BBA4BD1}" name="Distribution Type" dataDxfId="73"/>
-    <tableColumn id="5" xr3:uid="{BC7C6514-68B9-48F6-9938-4088DF28B37C}" name="Parameter 1" dataDxfId="72"/>
-    <tableColumn id="6" xr3:uid="{4D372042-F7DE-4E72-A309-C4266E0FA9E8}" name="Parameter 2" dataDxfId="71"/>
-    <tableColumn id="7" xr3:uid="{8D92705D-1A42-46F5-89EA-C4113CC26587}" name="Parameter 3" dataDxfId="70"/>
-    <tableColumn id="8" xr3:uid="{13B56E18-7C36-4950-847A-A7544475E1D1}" name="Parameter 4" dataDxfId="69"/>
-    <tableColumn id="14" xr3:uid="{2649C7B2-1C48-4B13-969D-684D0045538B}" name="Parameter 5" dataDxfId="68"/>
-    <tableColumn id="15" xr3:uid="{5D6C4F8D-D31E-4EED-BABF-A0A688F3A916}" name="Parameter 6" dataDxfId="67"/>
-    <tableColumn id="11" xr3:uid="{1CB1896E-F77C-4DFC-9AB0-D0C102F3F80F}" name="Lower Limit" dataDxfId="66"/>
-    <tableColumn id="12" xr3:uid="{837665AD-748D-4B51-9CCA-780B67A76815}" name="Upper Limit" dataDxfId="65"/>
-    <tableColumn id="13" xr3:uid="{A8F2935C-D451-47EA-A1E1-1E4F0CAE8D87}" name="Step" dataDxfId="64"/>
+    <tableColumn id="9" xr3:uid="{64A27C3D-2E18-40E6-9166-742BDA2B413C}" name="Phase" dataDxfId="74"/>
+    <tableColumn id="1" xr3:uid="{0243CFE4-EBE7-4500-A226-23C63BE2FB81}" name="Category" dataDxfId="73"/>
+    <tableColumn id="2" xr3:uid="{69F68BF8-9E6A-4766-AB29-A8B943A84522}" name="Name" dataDxfId="72"/>
+    <tableColumn id="10" xr3:uid="{1E4511F0-B286-4973-A437-9638677030CA}" name="Description" dataDxfId="71"/>
+    <tableColumn id="3" xr3:uid="{B80720A6-55E5-4A17-9FE9-9951AF480E02}" name="Units" dataDxfId="70"/>
+    <tableColumn id="4" xr3:uid="{54B33DED-7F55-4D76-B95F-B7050BBA4BD1}" name="Distribution Type" dataDxfId="69"/>
+    <tableColumn id="5" xr3:uid="{BC7C6514-68B9-48F6-9938-4088DF28B37C}" name="Parameter 1" dataDxfId="68"/>
+    <tableColumn id="6" xr3:uid="{4D372042-F7DE-4E72-A309-C4266E0FA9E8}" name="Parameter 2" dataDxfId="67"/>
+    <tableColumn id="7" xr3:uid="{8D92705D-1A42-46F5-89EA-C4113CC26587}" name="Parameter 3" dataDxfId="66"/>
+    <tableColumn id="8" xr3:uid="{13B56E18-7C36-4950-847A-A7544475E1D1}" name="Parameter 4" dataDxfId="65"/>
+    <tableColumn id="14" xr3:uid="{2649C7B2-1C48-4B13-969D-684D0045538B}" name="Parameter 5" dataDxfId="64"/>
+    <tableColumn id="15" xr3:uid="{5D6C4F8D-D31E-4EED-BABF-A0A688F3A916}" name="Parameter 6" dataDxfId="63"/>
+    <tableColumn id="11" xr3:uid="{1CB1896E-F77C-4DFC-9AB0-D0C102F3F80F}" name="Lower Limit" dataDxfId="62"/>
+    <tableColumn id="12" xr3:uid="{837665AD-748D-4B51-9CCA-780B67A76815}" name="Upper Limit" dataDxfId="61"/>
+    <tableColumn id="13" xr3:uid="{A8F2935C-D451-47EA-A1E1-1E4F0CAE8D87}" name="Step" dataDxfId="60"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{2EC220FC-5886-477C-8B2C-57082D8749AA}" name="Table1568102101213" displayName="Table1568102101213" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{2EC220FC-5886-477C-8B2C-57082D8749AA}" name="Table1568102101213" displayName="Table1568102101213" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="55">
   <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{525577E1-B46F-47FB-A042-A56D8D45D9AD}" name="Phase" dataDxfId="62"/>
-    <tableColumn id="1" xr3:uid="{30AFC0FE-4503-4A4B-91CA-E5B88AA24F98}" name="Category" dataDxfId="61"/>
-    <tableColumn id="2" xr3:uid="{6333C26F-3D36-4A65-8F1B-CC515ADCE181}" name="Name" dataDxfId="60"/>
-    <tableColumn id="10" xr3:uid="{057A52C2-DED0-48A5-8844-3950CD398F8D}" name="Description" dataDxfId="59"/>
-    <tableColumn id="3" xr3:uid="{EF447B65-8A6A-4F12-ABCB-7BFE84B734A9}" name="Units" dataDxfId="58"/>
-    <tableColumn id="4" xr3:uid="{6E658D46-B4D3-46B1-A15B-9F0095A7EADD}" name="Distribution Type" dataDxfId="57"/>
-    <tableColumn id="5" xr3:uid="{FE235A77-6EFF-4D9A-926F-ACE5D51D4BC8}" name="Parameter 1" dataDxfId="56"/>
-    <tableColumn id="6" xr3:uid="{26694561-3958-440C-BDDC-2DB16EB8A614}" name="Parameter 2" dataDxfId="55"/>
-    <tableColumn id="7" xr3:uid="{DA96F9A2-3DEB-4C42-BECF-B9C30ADA7428}" name="Parameter 3" dataDxfId="54"/>
-    <tableColumn id="8" xr3:uid="{5F8A48E3-9BBF-4210-88D8-F668C1FD845D}" name="Parameter 4" dataDxfId="53"/>
-    <tableColumn id="14" xr3:uid="{21514092-10F7-41E0-B078-A15175C73E93}" name="Parameter 5" dataDxfId="52"/>
-    <tableColumn id="15" xr3:uid="{8BFA8A6A-2BCB-4512-8B77-28D2C28FEEE3}" name="Parameter 6" dataDxfId="51"/>
-    <tableColumn id="11" xr3:uid="{9CB23DDB-2513-48F3-960F-EF0D57CD9724}" name="Lower Limit" dataDxfId="50"/>
-    <tableColumn id="12" xr3:uid="{EDE53E3A-8BAE-4FD6-9C38-CD4B63274C67}" name="Upper Limit" dataDxfId="49"/>
-    <tableColumn id="13" xr3:uid="{980D57FA-1EDD-484A-9D56-BF7EAA580C8D}" name="Step" dataDxfId="48"/>
+    <tableColumn id="9" xr3:uid="{525577E1-B46F-47FB-A042-A56D8D45D9AD}" name="Phase" dataDxfId="54"/>
+    <tableColumn id="1" xr3:uid="{30AFC0FE-4503-4A4B-91CA-E5B88AA24F98}" name="Category" dataDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{6333C26F-3D36-4A65-8F1B-CC515ADCE181}" name="Name" dataDxfId="52"/>
+    <tableColumn id="10" xr3:uid="{057A52C2-DED0-48A5-8844-3950CD398F8D}" name="Description" dataDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{EF447B65-8A6A-4F12-ABCB-7BFE84B734A9}" name="Units" dataDxfId="50"/>
+    <tableColumn id="4" xr3:uid="{6E658D46-B4D3-46B1-A15B-9F0095A7EADD}" name="Distribution Type" dataDxfId="49"/>
+    <tableColumn id="5" xr3:uid="{FE235A77-6EFF-4D9A-926F-ACE5D51D4BC8}" name="Parameter 1" dataDxfId="48"/>
+    <tableColumn id="6" xr3:uid="{26694561-3958-440C-BDDC-2DB16EB8A614}" name="Parameter 2" dataDxfId="47"/>
+    <tableColumn id="7" xr3:uid="{DA96F9A2-3DEB-4C42-BECF-B9C30ADA7428}" name="Parameter 3" dataDxfId="46"/>
+    <tableColumn id="8" xr3:uid="{5F8A48E3-9BBF-4210-88D8-F668C1FD845D}" name="Parameter 4" dataDxfId="45"/>
+    <tableColumn id="14" xr3:uid="{21514092-10F7-41E0-B078-A15175C73E93}" name="Parameter 5" dataDxfId="44"/>
+    <tableColumn id="15" xr3:uid="{8BFA8A6A-2BCB-4512-8B77-28D2C28FEEE3}" name="Parameter 6" dataDxfId="43"/>
+    <tableColumn id="11" xr3:uid="{9CB23DDB-2513-48F3-960F-EF0D57CD9724}" name="Lower Limit" dataDxfId="42"/>
+    <tableColumn id="12" xr3:uid="{EDE53E3A-8BAE-4FD6-9C38-CD4B63274C67}" name="Upper Limit" dataDxfId="41"/>
+    <tableColumn id="13" xr3:uid="{980D57FA-1EDD-484A-9D56-BF7EAA580C8D}" name="Step" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3DDD9CB2-968B-4A43-A20B-C749950155AA}" name="Table156810210121314" displayName="Table156810210121314" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3DDD9CB2-968B-4A43-A20B-C749950155AA}" name="Table156810210121314" displayName="Table156810210121314" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="35">
   <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{6B814874-1824-4E56-A967-04F9F6F3E584}" name="Phase" dataDxfId="46"/>
-    <tableColumn id="1" xr3:uid="{FE1635BE-F6C3-4D5B-B06E-7A92EBAB074D}" name="Category" dataDxfId="45"/>
-    <tableColumn id="2" xr3:uid="{9C16A715-E236-4930-A633-7510E082392C}" name="Name" dataDxfId="44"/>
-    <tableColumn id="10" xr3:uid="{B556C16A-1909-46E7-BC6D-8479761F1F65}" name="Description" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{5EFB6F3C-9894-43AA-AFAC-1013F8F0714B}" name="Units" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{6E3C1049-1D84-4FD5-B7CF-1E130CD32BCA}" name="Distribution Type" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{57E979B1-A630-4AC5-8C4D-CED1A62F587D}" name="Parameter 1" dataDxfId="40"/>
-    <tableColumn id="6" xr3:uid="{C9EF8DDD-DA1F-44E2-AC90-B6993C60CF1F}" name="Parameter 2" dataDxfId="39"/>
-    <tableColumn id="7" xr3:uid="{6FEFD03F-983B-47E2-9525-7EDD875A9C7C}" name="Parameter 3" dataDxfId="38"/>
-    <tableColumn id="8" xr3:uid="{0B661DB2-D286-4AEE-88C3-124B37F1B246}" name="Parameter 4" dataDxfId="37"/>
-    <tableColumn id="14" xr3:uid="{08C4ACC8-5A7B-4864-96E4-CF69FD654892}" name="Parameter 5" dataDxfId="36"/>
-    <tableColumn id="15" xr3:uid="{5505BBCC-5C52-4400-9C19-9ED7DBB490B8}" name="Parameter 6" dataDxfId="35"/>
-    <tableColumn id="11" xr3:uid="{E151AC3B-28ED-4186-A803-48B7F8B7AE5B}" name="Lower Limit" dataDxfId="34"/>
-    <tableColumn id="12" xr3:uid="{223709CC-AD09-4677-85AC-DF8A1619BF81}" name="Upper Limit" dataDxfId="33"/>
-    <tableColumn id="13" xr3:uid="{5FAAB5F5-A70D-4A6B-BE36-5CC1FD787BC5}" name="Step" dataDxfId="32"/>
+    <tableColumn id="9" xr3:uid="{6B814874-1824-4E56-A967-04F9F6F3E584}" name="Phase" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{FE1635BE-F6C3-4D5B-B06E-7A92EBAB074D}" name="Category" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{9C16A715-E236-4930-A633-7510E082392C}" name="Name" dataDxfId="32"/>
+    <tableColumn id="10" xr3:uid="{B556C16A-1909-46E7-BC6D-8479761F1F65}" name="Description" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{5EFB6F3C-9894-43AA-AFAC-1013F8F0714B}" name="Units" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{6E3C1049-1D84-4FD5-B7CF-1E130CD32BCA}" name="Distribution Type" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{57E979B1-A630-4AC5-8C4D-CED1A62F587D}" name="Parameter 1" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{C9EF8DDD-DA1F-44E2-AC90-B6993C60CF1F}" name="Parameter 2" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{6FEFD03F-983B-47E2-9525-7EDD875A9C7C}" name="Parameter 3" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{0B661DB2-D286-4AEE-88C3-124B37F1B246}" name="Parameter 4" dataDxfId="25"/>
+    <tableColumn id="14" xr3:uid="{08C4ACC8-5A7B-4864-96E4-CF69FD654892}" name="Parameter 5" dataDxfId="24"/>
+    <tableColumn id="15" xr3:uid="{5505BBCC-5C52-4400-9C19-9ED7DBB490B8}" name="Parameter 6" dataDxfId="23"/>
+    <tableColumn id="11" xr3:uid="{E151AC3B-28ED-4186-A803-48B7F8B7AE5B}" name="Lower Limit" dataDxfId="22"/>
+    <tableColumn id="12" xr3:uid="{223709CC-AD09-4677-85AC-DF8A1619BF81}" name="Upper Limit" dataDxfId="21"/>
+    <tableColumn id="13" xr3:uid="{5FAAB5F5-A70D-4A6B-BE36-5CC1FD787BC5}" name="Step" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{FBB513AC-2D2B-4552-8740-9D611743FE70}" name="Table15681021012131415" displayName="Table15681021012131415" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{FBB513AC-2D2B-4552-8740-9D611743FE70}" name="Table15681021012131415" displayName="Table15681021012131415" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="15">
   <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{2035FE2F-0A32-497E-B1E0-30D237A0E150}" name="Phase" dataDxfId="30"/>
-    <tableColumn id="1" xr3:uid="{F814DF41-D024-449F-AF42-62D43153FFB7}" name="Category" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{7DC8FB15-5985-4C4F-ADF3-7A17F5076A68}" name="Name" dataDxfId="28"/>
-    <tableColumn id="10" xr3:uid="{614B9103-CB85-46A8-93A4-7DE4EBCB5D2B}" name="Description" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{E1C6CE34-10C1-4516-B6D9-58BC2F148637}" name="Units" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{2DC3C549-6825-4F8C-B404-F2995425599E}" name="Distribution Type" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{805795A1-E0DE-4FCC-9EBD-DDCCA12F0793}" name="Parameter 1" dataDxfId="24"/>
-    <tableColumn id="6" xr3:uid="{8AEEFD06-21CF-4496-9CA8-A505BA5018C8}" name="Parameter 2" dataDxfId="23"/>
-    <tableColumn id="7" xr3:uid="{81F9FC74-65BB-4D24-8C32-944022DBFF45}" name="Parameter 3" dataDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{B80C3AAC-1FDC-42E7-B79C-4A7F876448A4}" name="Parameter 4" dataDxfId="21"/>
-    <tableColumn id="14" xr3:uid="{07C0D5EC-F968-40E1-8F17-889B90B82192}" name="Parameter 5" dataDxfId="20"/>
-    <tableColumn id="15" xr3:uid="{0302BE75-0A0F-489C-99C0-05DCDFC40A44}" name="Parameter 6" dataDxfId="19"/>
-    <tableColumn id="11" xr3:uid="{8B4A7C21-F1CF-4881-A5A6-4163F9C44F88}" name="Lower Limit" dataDxfId="18"/>
-    <tableColumn id="12" xr3:uid="{F4935CE7-6ADF-493E-B887-56BFE62D0ADC}" name="Upper Limit" dataDxfId="17"/>
-    <tableColumn id="13" xr3:uid="{5249EF7A-61B0-47D7-A1ED-48836EF45F76}" name="Step" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{2035FE2F-0A32-497E-B1E0-30D237A0E150}" name="Phase" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{F814DF41-D024-449F-AF42-62D43153FFB7}" name="Category" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{7DC8FB15-5985-4C4F-ADF3-7A17F5076A68}" name="Name" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{614B9103-CB85-46A8-93A4-7DE4EBCB5D2B}" name="Description" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{E1C6CE34-10C1-4516-B6D9-58BC2F148637}" name="Units" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{2DC3C549-6825-4F8C-B404-F2995425599E}" name="Distribution Type" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{805795A1-E0DE-4FCC-9EBD-DDCCA12F0793}" name="Parameter 1" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{8AEEFD06-21CF-4496-9CA8-A505BA5018C8}" name="Parameter 2" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{81F9FC74-65BB-4D24-8C32-944022DBFF45}" name="Parameter 3" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{B80C3AAC-1FDC-42E7-B79C-4A7F876448A4}" name="Parameter 4" dataDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{07C0D5EC-F968-40E1-8F17-889B90B82192}" name="Parameter 5" dataDxfId="4"/>
+    <tableColumn id="15" xr3:uid="{0302BE75-0A0F-489C-99C0-05DCDFC40A44}" name="Parameter 6" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{8B4A7C21-F1CF-4881-A5A6-4163F9C44F88}" name="Lower Limit" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{F4935CE7-6ADF-493E-B887-56BFE62D0ADC}" name="Upper Limit" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{5249EF7A-61B0-47D7-A1ED-48836EF45F76}" name="Step" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3794,7 +3903,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3902,7 +4011,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -3930,7 +4039,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
@@ -4148,12 +4257,20 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L9">
-    <cfRule type="expression" dxfId="3" priority="1">
+  <conditionalFormatting sqref="A2:L2 A4:L9 A3:D3 F3:L3">
+    <cfRule type="expression" dxfId="39" priority="3">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="38" priority="4">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="expression" dxfId="37" priority="1">
+      <formula>ISBLANK($F3)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="36" priority="2">
+      <formula>NOT((COLUMN(E3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -4172,8 +4289,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07EF9366-5AFF-4F5A-9471-F50914749AD6}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4281,7 +4398,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -4309,7 +4426,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
@@ -4527,12 +4644,20 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L9">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="A2:L2 A4:L9 A3:D3 F3:L3">
+    <cfRule type="expression" dxfId="19" priority="3">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="18" priority="4">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="expression" dxfId="17" priority="1">
+      <formula>ISBLANK($F3)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="2">
+      <formula>NOT((COLUMN(E3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -4952,10 +5077,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097870CC-1A0F-461E-BDFD-29BDDFDDF05C}">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4967,7 +5092,7 @@
     <col min="5" max="15" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -5014,7 +5139,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>70</v>
       </c>
@@ -5022,7 +5147,7 @@
         <v>70</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>53</v>
@@ -5033,14 +5158,16 @@
       <c r="F2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="G2" s="5">
+        <v>0</v>
+      </c>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="6"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="17">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="N2" s="17">
         <v>50000000</v>
@@ -5049,7 +5176,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>70</v>
       </c>
@@ -5057,18 +5184,20 @@
         <v>70</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>93</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="9"/>
+      <c r="G3" s="9">
+        <v>-1</v>
+      </c>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="10"/>
@@ -5084,7 +5213,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -5092,7 +5221,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>52</v>
@@ -5103,23 +5232,25 @@
       <c r="F4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="12"/>
+      <c r="G4" s="12">
+        <v>747.86950000000002</v>
+      </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
       <c r="M4" s="18">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="N4" s="18">
         <v>50000000</v>
       </c>
       <c r="O4" s="18">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+        <v>1.0000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>71</v>
       </c>
@@ -5127,19 +5258,23 @@
         <v>71</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>94</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
+        <v>4</v>
+      </c>
+      <c r="G5" s="9">
+        <v>3.0319702616531905</v>
+      </c>
+      <c r="H5" s="9">
+        <v>8.0319702616531909</v>
+      </c>
       <c r="I5" s="9"/>
       <c r="J5" s="10"/>
       <c r="K5" s="2"/>
@@ -5150,11 +5285,12 @@
       <c r="N5" s="19">
         <v>10</v>
       </c>
-      <c r="O5" s="19">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O5" s="18">
+        <v>1.0000000000000001E-9</v>
+      </c>
+      <c r="Q5" s="21"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>72</v>
       </c>
@@ -5162,7 +5298,7 @@
         <v>72</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>73</v>
@@ -5173,14 +5309,16 @@
       <c r="F6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="12"/>
+      <c r="G6" s="12">
+        <v>0</v>
+      </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="13"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
       <c r="M6" s="18">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="N6" s="18">
         <v>50000000</v>
@@ -5189,7 +5327,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>72</v>
       </c>
@@ -5197,18 +5335,20 @@
         <v>72</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>95</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="12"/>
+      <c r="G7" s="12">
+        <v>-1</v>
+      </c>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="13"/>
@@ -5224,7 +5364,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>71</v>
       </c>
@@ -5244,7 +5384,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="9">
-        <v>0</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -5257,11 +5397,11 @@
       <c r="N8" s="9">
         <v>1</v>
       </c>
-      <c r="O8" s="9">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O8" s="18">
+        <v>1.0000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>71</v>
       </c>
@@ -5281,7 +5421,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="9">
-        <v>0.5</v>
+        <v>0.55555555555555558</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -5294,11 +5434,11 @@
       <c r="N9" s="9">
         <v>1</v>
       </c>
-      <c r="O9" s="9">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O9" s="18">
+        <v>1.0000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>71</v>
       </c>
@@ -5318,7 +5458,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="9">
-        <v>0.5</v>
+        <v>0.1111111111111111</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -5331,11 +5471,11 @@
       <c r="N10" s="9">
         <v>1</v>
       </c>
-      <c r="O10" s="9">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O10" s="18">
+        <v>1.0000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>71</v>
       </c>
@@ -5372,7 +5512,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>71</v>
       </c>
@@ -5409,7 +5549,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>71</v>
       </c>
@@ -5446,7 +5586,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>71</v>
       </c>
@@ -5483,18 +5623,18 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>70</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>68</v>
@@ -5503,7 +5643,7 @@
         <v>3</v>
       </c>
       <c r="G15" s="12">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
@@ -5520,18 +5660,18 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>70</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>68</v>
@@ -5540,7 +5680,7 @@
         <v>3</v>
       </c>
       <c r="G16" s="12">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
@@ -5562,13 +5702,13 @@
         <v>70</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>68</v>
@@ -5577,7 +5717,7 @@
         <v>3</v>
       </c>
       <c r="G17" s="12">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
@@ -5599,13 +5739,13 @@
         <v>70</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>68</v>
@@ -5614,7 +5754,7 @@
         <v>3</v>
       </c>
       <c r="G18" s="12">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
@@ -5636,13 +5776,13 @@
         <v>70</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>68</v>
@@ -5651,7 +5791,7 @@
         <v>3</v>
       </c>
       <c r="G19" s="12">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
@@ -5673,13 +5813,13 @@
         <v>70</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>68</v>
@@ -5688,7 +5828,7 @@
         <v>3</v>
       </c>
       <c r="G20" s="12">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
@@ -5710,13 +5850,13 @@
         <v>72</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>68</v>
@@ -5725,7 +5865,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="12">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
@@ -5747,13 +5887,13 @@
         <v>72</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>68</v>
@@ -5762,7 +5902,7 @@
         <v>3</v>
       </c>
       <c r="G22" s="12">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
@@ -5784,13 +5924,13 @@
         <v>72</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>68</v>
@@ -5799,7 +5939,7 @@
         <v>3</v>
       </c>
       <c r="G23" s="12">
-        <v>0.1</v>
+        <v>0</v>
       </c>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
@@ -5821,13 +5961,13 @@
         <v>72</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>68</v>
@@ -5836,7 +5976,7 @@
         <v>3</v>
       </c>
       <c r="G24" s="12">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
@@ -5858,13 +5998,13 @@
         <v>72</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>68</v>
@@ -5873,7 +6013,7 @@
         <v>3</v>
       </c>
       <c r="G25" s="12">
-        <v>0.3</v>
+        <v>0</v>
       </c>
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
@@ -5898,10 +6038,10 @@
         <v>107</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>68</v>
@@ -5910,7 +6050,7 @@
         <v>3</v>
       </c>
       <c r="G26" s="12">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="H26" s="12"/>
       <c r="I26" s="12"/>
@@ -5932,13 +6072,13 @@
         <v>71</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>68</v>
@@ -5947,7 +6087,7 @@
         <v>3</v>
       </c>
       <c r="G27" s="12">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
@@ -5972,10 +6112,10 @@
         <v>104</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>68</v>
@@ -5984,7 +6124,7 @@
         <v>3</v>
       </c>
       <c r="G28" s="12">
-        <v>0.1</v>
+        <v>0.125</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
@@ -5998,7 +6138,7 @@
         <v>1</v>
       </c>
       <c r="O28" s="12">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -6009,10 +6149,10 @@
         <v>105</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>68</v>
@@ -6021,7 +6161,7 @@
         <v>3</v>
       </c>
       <c r="G29" s="12">
-        <v>0.05</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
@@ -6035,7 +6175,7 @@
         <v>1</v>
       </c>
       <c r="O29" s="12">
-        <v>0.01</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -6046,10 +6186,10 @@
         <v>106</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>68</v>
@@ -6058,7 +6198,7 @@
         <v>3</v>
       </c>
       <c r="G30" s="12">
-        <v>0.3</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H30" s="12"/>
       <c r="I30" s="12"/>
@@ -6072,7 +6212,7 @@
         <v>1</v>
       </c>
       <c r="O30" s="12">
-        <v>0.01</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
@@ -6083,10 +6223,10 @@
         <v>107</v>
       </c>
       <c r="C31" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="D31" s="12" t="s">
         <v>141</v>
-      </c>
-      <c r="D31" s="12" t="s">
-        <v>142</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>68</v>
@@ -6095,7 +6235,7 @@
         <v>3</v>
       </c>
       <c r="G31" s="12">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
@@ -6120,10 +6260,10 @@
         <v>108</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>68</v>
@@ -6132,7 +6272,7 @@
         <v>3</v>
       </c>
       <c r="G32" s="12">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="H32" s="12"/>
       <c r="I32" s="12"/>
@@ -6152,10 +6292,10 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A2:L32">
-    <cfRule type="expression" dxfId="15" priority="43">
+    <cfRule type="expression" dxfId="155" priority="43">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="44">
+    <cfRule type="expression" dxfId="154" priority="44">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6176,7 +6316,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6284,7 +6424,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -6312,7 +6452,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
@@ -6531,10 +6671,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:L9">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="137" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="136" priority="2">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6555,7 +6695,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:G4"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6663,7 +6803,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -6691,7 +6831,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
@@ -6909,12 +7049,20 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L9">
-    <cfRule type="expression" dxfId="11" priority="1">
+  <conditionalFormatting sqref="A2:L2 A4:L9 A3:D3 F3:L3">
+    <cfRule type="expression" dxfId="119" priority="3">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="118" priority="4">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="expression" dxfId="117" priority="1">
+      <formula>ISBLANK($F3)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="116" priority="2">
+      <formula>NOT((COLUMN(E3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -6934,7 +7082,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7042,7 +7190,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -7070,7 +7218,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
@@ -7288,12 +7436,20 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L9">
-    <cfRule type="expression" dxfId="9" priority="3">
+  <conditionalFormatting sqref="A2:L2 A4:L9 A3:D3 F3:L3">
+    <cfRule type="expression" dxfId="99" priority="5">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="4">
+    <cfRule type="expression" dxfId="98" priority="6">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="expression" dxfId="97" priority="1">
+      <formula>ISBLANK($F3)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="96" priority="2">
+      <formula>NOT((COLUMN(E3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -7313,7 +7469,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7421,7 +7577,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -7449,7 +7605,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
@@ -7667,12 +7823,20 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L9">
-    <cfRule type="expression" dxfId="7" priority="1">
+  <conditionalFormatting sqref="A2:L2 A4:L9 A3:D3 F3:L3">
+    <cfRule type="expression" dxfId="79" priority="3">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="78" priority="4">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="expression" dxfId="77" priority="1">
+      <formula>ISBLANK($F3)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="76" priority="2">
+      <formula>NOT((COLUMN(E3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -7692,7 +7856,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7800,7 +7964,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>115</v>
+        <v>151</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -7828,7 +7992,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
@@ -8046,12 +8210,20 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L9">
-    <cfRule type="expression" dxfId="5" priority="1">
+  <conditionalFormatting sqref="A2:L2 A4:L9 A3:D3 F3:L3">
+    <cfRule type="expression" dxfId="59" priority="3">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="58" priority="4">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="expression" dxfId="57" priority="1">
+      <formula>ISBLANK($F3)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="56" priority="2">
+      <formula>NOT((COLUMN(E3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Edited BOTE input files
</commit_message>
<xml_diff>
--- a/InputFiles/DefineScenario.xlsx
+++ b/InputFiles/DefineScenario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peraza\Documents\Tasking\(4) EPA Stuff\Task 5 Repo\WideAreaDecon\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE9BDC5B-54EC-4D60-B3FE-47FC64B71D76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEBDF50-20E1-4D9F-B43A-DD28720E6792}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="649" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5086,7 +5086,7 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6241,7 +6241,7 @@
         <v>3</v>
       </c>
       <c r="G31" s="12">
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
@@ -6278,7 +6278,7 @@
         <v>3</v>
       </c>
       <c r="G32" s="12">
-        <v>0.25</v>
+        <v>0.125</v>
       </c>
       <c r="H32" s="12"/>
       <c r="I32" s="12"/>

</xml_diff>

<commit_message>
Replaced original input files with updated files
</commit_message>
<xml_diff>
--- a/InputFiles/DefineScenario.xlsx
+++ b/InputFiles/DefineScenario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peraza\Documents\Tasking\(4) EPA Stuff\Task 5 Repo\WideAreaDecon\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERAZA\Documents\Tasking\(4) EPA Stuff\Task 5 Repo\WideAreaDecon\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEBDF50-20E1-4D9F-B43A-DD28720E6792}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9F6AF9-D8C7-4947-8663-BAC9963E88A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="649" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="649" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal - File Info" sheetId="1" r:id="rId1"/>
@@ -391,6 +391,9 @@
     <t>Fraction of residential buildings that are miscellaneous</t>
   </si>
   <si>
+    <t>log(PFU / m^2)</t>
+  </si>
+  <si>
     <t>Outdoor Surface Type Breakout</t>
   </si>
   <si>
@@ -497,9 +500,6 @@
   </si>
   <si>
     <t>Underground Walls</t>
-  </si>
-  <si>
-    <t>log(CFU / m^2)</t>
   </si>
   <si>
     <t>Underground HVAC</t>
@@ -747,7 +747,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -769,13 +769,12 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="156">
+  <dxfs count="144">
     <dxf>
       <border>
         <left style="thin">
@@ -1089,6 +1088,300 @@
       </fill>
     </dxf>
     <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <i/>
         <strike/>
@@ -1419,6 +1712,300 @@
       </fill>
     </dxf>
     <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <i/>
         <strike/>
@@ -1749,24 +2336,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <i/>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color indexed="64"/>
@@ -2059,684 +2628,6 @@
           <color rgb="FF000000"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3394,168 +3285,168 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{77E3C927-1FC6-443B-87ED-00E2959DD317}" name="Table1568" displayName="Table1568" ref="A1:O32" totalsRowShown="0" tableBorderDxfId="153">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{77E3C927-1FC6-443B-87ED-00E2959DD317}" name="Table1568" displayName="Table1568" ref="A1:O32" totalsRowShown="0" tableBorderDxfId="141">
   <autoFilter ref="A1:O32" xr:uid="{58F00973-C0E2-47D9-9C5E-C7B7F684A0C3}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{62A6D655-D638-4005-9525-C140421ED9AB}" name="Phase" dataDxfId="152"/>
-    <tableColumn id="1" xr3:uid="{1BC04ADD-0426-4785-9F97-FCE0BCC1E547}" name="Category" dataDxfId="151"/>
-    <tableColumn id="2" xr3:uid="{3089FC2E-257C-4BA5-A9A7-5D0E01D5E6F5}" name="Name" dataDxfId="150"/>
-    <tableColumn id="10" xr3:uid="{E1A27E6E-82E5-4CF6-9164-A680FF7F05A5}" name="Description" dataDxfId="149"/>
-    <tableColumn id="3" xr3:uid="{BA85C23F-8236-43E3-885F-DF8CCDB84F06}" name="Units" dataDxfId="148"/>
-    <tableColumn id="4" xr3:uid="{9121EDDE-A8D8-4E28-AAAC-953CC1A14CB2}" name="Distribution Type" dataDxfId="147"/>
-    <tableColumn id="5" xr3:uid="{67D6DF1C-45B3-456F-B960-B8F495F6867D}" name="Parameter 1" dataDxfId="146"/>
-    <tableColumn id="6" xr3:uid="{A2BB8730-6626-47D8-AABB-90C19B218AFB}" name="Parameter 2" dataDxfId="145"/>
-    <tableColumn id="7" xr3:uid="{B7BC4EB1-7616-4A3A-899A-F01A87DD3B48}" name="Parameter 3" dataDxfId="144"/>
-    <tableColumn id="8" xr3:uid="{32D71C9B-2B39-4A83-9EB0-1934F2F6FC91}" name="Parameter 4" dataDxfId="143"/>
-    <tableColumn id="14" xr3:uid="{31AC778C-1A4A-45DD-8A12-F22858D3CD3A}" name="Parameter 5" dataDxfId="142"/>
-    <tableColumn id="15" xr3:uid="{91C3BDC4-4893-4CF7-9830-76CC4A9BF6F1}" name="Parameter 6" dataDxfId="141"/>
-    <tableColumn id="11" xr3:uid="{6BCEB05C-9FCE-48DE-91F0-D2ACC21C6C3E}" name="Lower Limit" dataDxfId="140"/>
-    <tableColumn id="12" xr3:uid="{CDC89704-43FE-407F-B8B4-079E5E991263}" name="Upper Limit" dataDxfId="139"/>
-    <tableColumn id="13" xr3:uid="{0758CB79-3F38-44D8-B78B-CC33BB1D2C70}" name="Step" dataDxfId="138"/>
+    <tableColumn id="9" xr3:uid="{62A6D655-D638-4005-9525-C140421ED9AB}" name="Phase" dataDxfId="140"/>
+    <tableColumn id="1" xr3:uid="{1BC04ADD-0426-4785-9F97-FCE0BCC1E547}" name="Category" dataDxfId="139"/>
+    <tableColumn id="2" xr3:uid="{3089FC2E-257C-4BA5-A9A7-5D0E01D5E6F5}" name="Name" dataDxfId="138"/>
+    <tableColumn id="10" xr3:uid="{E1A27E6E-82E5-4CF6-9164-A680FF7F05A5}" name="Description" dataDxfId="137"/>
+    <tableColumn id="3" xr3:uid="{BA85C23F-8236-43E3-885F-DF8CCDB84F06}" name="Units" dataDxfId="136"/>
+    <tableColumn id="4" xr3:uid="{9121EDDE-A8D8-4E28-AAAC-953CC1A14CB2}" name="Distribution Type" dataDxfId="135"/>
+    <tableColumn id="5" xr3:uid="{67D6DF1C-45B3-456F-B960-B8F495F6867D}" name="Parameter 1" dataDxfId="134"/>
+    <tableColumn id="6" xr3:uid="{A2BB8730-6626-47D8-AABB-90C19B218AFB}" name="Parameter 2" dataDxfId="133"/>
+    <tableColumn id="7" xr3:uid="{B7BC4EB1-7616-4A3A-899A-F01A87DD3B48}" name="Parameter 3" dataDxfId="132"/>
+    <tableColumn id="8" xr3:uid="{32D71C9B-2B39-4A83-9EB0-1934F2F6FC91}" name="Parameter 4" dataDxfId="131"/>
+    <tableColumn id="14" xr3:uid="{31AC778C-1A4A-45DD-8A12-F22858D3CD3A}" name="Parameter 5" dataDxfId="130"/>
+    <tableColumn id="15" xr3:uid="{91C3BDC4-4893-4CF7-9830-76CC4A9BF6F1}" name="Parameter 6" dataDxfId="129"/>
+    <tableColumn id="11" xr3:uid="{6BCEB05C-9FCE-48DE-91F0-D2ACC21C6C3E}" name="Lower Limit" dataDxfId="128"/>
+    <tableColumn id="12" xr3:uid="{CDC89704-43FE-407F-B8B4-079E5E991263}" name="Upper Limit" dataDxfId="127"/>
+    <tableColumn id="13" xr3:uid="{0758CB79-3F38-44D8-B78B-CC33BB1D2C70}" name="Step" dataDxfId="126"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{72F3CA1E-AAFF-44BC-A114-2AA862291D9E}" name="Table1568102" displayName="Table1568102" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="135">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{72F3CA1E-AAFF-44BC-A114-2AA862291D9E}" name="Table1568102" displayName="Table1568102" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="123">
   <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{8FD38CEB-1D1A-41E8-821F-58DD4FBD85EB}" name="Phase" dataDxfId="134"/>
-    <tableColumn id="1" xr3:uid="{574AE483-6154-4EC6-AC18-5FDEBC0931CD}" name="Category" dataDxfId="133"/>
-    <tableColumn id="2" xr3:uid="{EC332146-FEF7-42A1-9698-0FB7656BE557}" name="Name" dataDxfId="132"/>
-    <tableColumn id="10" xr3:uid="{F0942CE2-9658-4EB8-A19F-B3B76B6A5F95}" name="Description" dataDxfId="131"/>
-    <tableColumn id="3" xr3:uid="{B909ADC8-9FD8-4714-A691-8AD0F1933057}" name="Units" dataDxfId="130"/>
-    <tableColumn id="4" xr3:uid="{F8B8B123-0CBC-450A-B098-9FFA08F7FC89}" name="Distribution Type" dataDxfId="129"/>
-    <tableColumn id="5" xr3:uid="{AADB8566-896F-40D4-8181-BB145E678F9B}" name="Parameter 1" dataDxfId="128"/>
-    <tableColumn id="6" xr3:uid="{13B0114C-55D3-4603-92C6-09319B7E315B}" name="Parameter 2" dataDxfId="127"/>
-    <tableColumn id="7" xr3:uid="{7548BB98-B29E-4F39-B198-D6F9994CC04D}" name="Parameter 3" dataDxfId="126"/>
-    <tableColumn id="8" xr3:uid="{355D4B98-B5B0-461B-90E8-3D81112B89E2}" name="Parameter 4" dataDxfId="125"/>
-    <tableColumn id="14" xr3:uid="{14667F24-6EC2-4F8F-8EAA-56B4FF372D98}" name="Parameter 5" dataDxfId="124"/>
-    <tableColumn id="15" xr3:uid="{B058DB6A-9C46-4ED3-9483-5713AD52AE40}" name="Parameter 6" dataDxfId="123"/>
-    <tableColumn id="11" xr3:uid="{0E22E7A3-8506-41E8-AC60-E103665C60A2}" name="Lower Limit" dataDxfId="122"/>
-    <tableColumn id="12" xr3:uid="{479761C6-7DBC-4557-9E7C-984A37ABCB8A}" name="Upper Limit" dataDxfId="121"/>
-    <tableColumn id="13" xr3:uid="{F96695B6-2ADD-458A-A424-B58482082C80}" name="Step" dataDxfId="120"/>
+    <tableColumn id="9" xr3:uid="{8FD38CEB-1D1A-41E8-821F-58DD4FBD85EB}" name="Phase" dataDxfId="122"/>
+    <tableColumn id="1" xr3:uid="{574AE483-6154-4EC6-AC18-5FDEBC0931CD}" name="Category" dataDxfId="121"/>
+    <tableColumn id="2" xr3:uid="{EC332146-FEF7-42A1-9698-0FB7656BE557}" name="Name" dataDxfId="120"/>
+    <tableColumn id="10" xr3:uid="{F0942CE2-9658-4EB8-A19F-B3B76B6A5F95}" name="Description" dataDxfId="119"/>
+    <tableColumn id="3" xr3:uid="{B909ADC8-9FD8-4714-A691-8AD0F1933057}" name="Units" dataDxfId="118"/>
+    <tableColumn id="4" xr3:uid="{F8B8B123-0CBC-450A-B098-9FFA08F7FC89}" name="Distribution Type" dataDxfId="117"/>
+    <tableColumn id="5" xr3:uid="{AADB8566-896F-40D4-8181-BB145E678F9B}" name="Parameter 1" dataDxfId="116"/>
+    <tableColumn id="6" xr3:uid="{13B0114C-55D3-4603-92C6-09319B7E315B}" name="Parameter 2" dataDxfId="115"/>
+    <tableColumn id="7" xr3:uid="{7548BB98-B29E-4F39-B198-D6F9994CC04D}" name="Parameter 3" dataDxfId="114"/>
+    <tableColumn id="8" xr3:uid="{355D4B98-B5B0-461B-90E8-3D81112B89E2}" name="Parameter 4" dataDxfId="113"/>
+    <tableColumn id="14" xr3:uid="{14667F24-6EC2-4F8F-8EAA-56B4FF372D98}" name="Parameter 5" dataDxfId="112"/>
+    <tableColumn id="15" xr3:uid="{B058DB6A-9C46-4ED3-9483-5713AD52AE40}" name="Parameter 6" dataDxfId="111"/>
+    <tableColumn id="11" xr3:uid="{0E22E7A3-8506-41E8-AC60-E103665C60A2}" name="Lower Limit" dataDxfId="110"/>
+    <tableColumn id="12" xr3:uid="{479761C6-7DBC-4557-9E7C-984A37ABCB8A}" name="Upper Limit" dataDxfId="109"/>
+    <tableColumn id="13" xr3:uid="{F96695B6-2ADD-458A-A424-B58482082C80}" name="Step" dataDxfId="108"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{88C3C7FF-7D66-4C1C-A80E-12CD3AFBFB8D}" name="Table156810210" displayName="Table156810210" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="115">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{88C3C7FF-7D66-4C1C-A80E-12CD3AFBFB8D}" name="Table156810210" displayName="Table156810210" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="105">
   <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{5AC7EE20-3F52-40E0-87F1-21D82A7C3AA2}" name="Phase" dataDxfId="114"/>
-    <tableColumn id="1" xr3:uid="{9A9754BC-4FF9-4BBA-B750-B911CE430E6A}" name="Category" dataDxfId="113"/>
-    <tableColumn id="2" xr3:uid="{0A114B0A-D97E-4073-8E4E-5B16FB19520E}" name="Name" dataDxfId="112"/>
-    <tableColumn id="10" xr3:uid="{D1A72F97-70A3-4EEB-9316-B31F108E3FD5}" name="Description" dataDxfId="111"/>
-    <tableColumn id="3" xr3:uid="{E8F09B1A-D952-4236-B6AD-8AC480554D73}" name="Units" dataDxfId="110"/>
-    <tableColumn id="4" xr3:uid="{B1DC9551-CBBD-4BF4-B876-9237E0FB121D}" name="Distribution Type" dataDxfId="109"/>
-    <tableColumn id="5" xr3:uid="{72C76302-CA88-4629-BF3A-72DD8971E0B7}" name="Parameter 1" dataDxfId="108"/>
-    <tableColumn id="6" xr3:uid="{C319BB6E-60FD-4F37-B898-C033C52FE070}" name="Parameter 2" dataDxfId="107"/>
-    <tableColumn id="7" xr3:uid="{B370DF9A-4768-49F1-B38B-F65D182A01B4}" name="Parameter 3" dataDxfId="106"/>
-    <tableColumn id="8" xr3:uid="{7BADEC71-6529-4D26-804E-5C9B93DA84E8}" name="Parameter 4" dataDxfId="105"/>
-    <tableColumn id="14" xr3:uid="{125149FE-86DA-4053-8A54-90E57B52F8B0}" name="Parameter 5" dataDxfId="104"/>
-    <tableColumn id="15" xr3:uid="{BAA75930-0A4F-4888-8CAF-A3AFA6F3FF44}" name="Parameter 6" dataDxfId="103"/>
-    <tableColumn id="11" xr3:uid="{7442F6EC-3907-41A8-BBEF-87C9374C67E5}" name="Lower Limit" dataDxfId="102"/>
-    <tableColumn id="12" xr3:uid="{86E2B2CA-B8F0-4FF5-8C59-2D3C44061DFD}" name="Upper Limit" dataDxfId="101"/>
-    <tableColumn id="13" xr3:uid="{C697FE06-06BB-49EC-93BB-FF753593319A}" name="Step" dataDxfId="100"/>
+    <tableColumn id="9" xr3:uid="{5AC7EE20-3F52-40E0-87F1-21D82A7C3AA2}" name="Phase" dataDxfId="104"/>
+    <tableColumn id="1" xr3:uid="{9A9754BC-4FF9-4BBA-B750-B911CE430E6A}" name="Category" dataDxfId="103"/>
+    <tableColumn id="2" xr3:uid="{0A114B0A-D97E-4073-8E4E-5B16FB19520E}" name="Name" dataDxfId="102"/>
+    <tableColumn id="10" xr3:uid="{D1A72F97-70A3-4EEB-9316-B31F108E3FD5}" name="Description" dataDxfId="101"/>
+    <tableColumn id="3" xr3:uid="{E8F09B1A-D952-4236-B6AD-8AC480554D73}" name="Units" dataDxfId="100"/>
+    <tableColumn id="4" xr3:uid="{B1DC9551-CBBD-4BF4-B876-9237E0FB121D}" name="Distribution Type" dataDxfId="99"/>
+    <tableColumn id="5" xr3:uid="{72C76302-CA88-4629-BF3A-72DD8971E0B7}" name="Parameter 1" dataDxfId="98"/>
+    <tableColumn id="6" xr3:uid="{C319BB6E-60FD-4F37-B898-C033C52FE070}" name="Parameter 2" dataDxfId="97"/>
+    <tableColumn id="7" xr3:uid="{B370DF9A-4768-49F1-B38B-F65D182A01B4}" name="Parameter 3" dataDxfId="96"/>
+    <tableColumn id="8" xr3:uid="{7BADEC71-6529-4D26-804E-5C9B93DA84E8}" name="Parameter 4" dataDxfId="95"/>
+    <tableColumn id="14" xr3:uid="{125149FE-86DA-4053-8A54-90E57B52F8B0}" name="Parameter 5" dataDxfId="94"/>
+    <tableColumn id="15" xr3:uid="{BAA75930-0A4F-4888-8CAF-A3AFA6F3FF44}" name="Parameter 6" dataDxfId="93"/>
+    <tableColumn id="11" xr3:uid="{7442F6EC-3907-41A8-BBEF-87C9374C67E5}" name="Lower Limit" dataDxfId="92"/>
+    <tableColumn id="12" xr3:uid="{86E2B2CA-B8F0-4FF5-8C59-2D3C44061DFD}" name="Upper Limit" dataDxfId="91"/>
+    <tableColumn id="13" xr3:uid="{C697FE06-06BB-49EC-93BB-FF753593319A}" name="Step" dataDxfId="90"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6794810C-E49F-4CB0-9B2F-0FA2655BD884}" name="Table15681021011" displayName="Table15681021011" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6794810C-E49F-4CB0-9B2F-0FA2655BD884}" name="Table15681021011" displayName="Table15681021011" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="87">
   <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{5DEAB66E-0CAB-4BF7-B4EA-D8D12FB47328}" name="Phase" dataDxfId="94"/>
-    <tableColumn id="1" xr3:uid="{69C64F5C-9979-4ACA-9A42-C1032E3D98BA}" name="Category" dataDxfId="93"/>
-    <tableColumn id="2" xr3:uid="{D4385687-B64B-46FB-B987-6E74F19DC1AF}" name="Name" dataDxfId="92"/>
-    <tableColumn id="10" xr3:uid="{BE461B66-2B72-42A7-9F3F-5916187828CF}" name="Description" dataDxfId="91"/>
-    <tableColumn id="3" xr3:uid="{9EE711F7-7C5D-4C54-8A9A-D54F8833D434}" name="Units" dataDxfId="90"/>
-    <tableColumn id="4" xr3:uid="{6EAA6194-27E9-4B7C-8A4D-8C0FE7B617F4}" name="Distribution Type" dataDxfId="89"/>
-    <tableColumn id="5" xr3:uid="{75BC5E4C-C28D-4614-8AB6-165A9F7FE7CE}" name="Parameter 1" dataDxfId="88"/>
-    <tableColumn id="6" xr3:uid="{F5AD0C00-9187-4F91-ADA7-5B461FC355CE}" name="Parameter 2" dataDxfId="87"/>
-    <tableColumn id="7" xr3:uid="{34B0A2DF-5607-43F6-AA9E-1106CCB7621B}" name="Parameter 3" dataDxfId="86"/>
-    <tableColumn id="8" xr3:uid="{B0950426-083D-4CE9-A30E-9D71766BA154}" name="Parameter 4" dataDxfId="85"/>
-    <tableColumn id="14" xr3:uid="{88E7A84D-F80D-416C-9037-2E5927AE2697}" name="Parameter 5" dataDxfId="84"/>
-    <tableColumn id="15" xr3:uid="{E3DCF8BA-29B1-4A24-B6E6-DE9435CB3AC9}" name="Parameter 6" dataDxfId="83"/>
-    <tableColumn id="11" xr3:uid="{E8661EBF-62F4-4D4A-BCDC-7C8ABD4866B0}" name="Lower Limit" dataDxfId="82"/>
-    <tableColumn id="12" xr3:uid="{83DA3A0E-E097-4281-9822-6FE3F8FB0CDD}" name="Upper Limit" dataDxfId="81"/>
-    <tableColumn id="13" xr3:uid="{24B0E0E0-CA9C-4655-9B23-EA0BBD517B67}" name="Step" dataDxfId="80"/>
+    <tableColumn id="9" xr3:uid="{5DEAB66E-0CAB-4BF7-B4EA-D8D12FB47328}" name="Phase" dataDxfId="86"/>
+    <tableColumn id="1" xr3:uid="{69C64F5C-9979-4ACA-9A42-C1032E3D98BA}" name="Category" dataDxfId="85"/>
+    <tableColumn id="2" xr3:uid="{D4385687-B64B-46FB-B987-6E74F19DC1AF}" name="Name" dataDxfId="84"/>
+    <tableColumn id="10" xr3:uid="{BE461B66-2B72-42A7-9F3F-5916187828CF}" name="Description" dataDxfId="83"/>
+    <tableColumn id="3" xr3:uid="{9EE711F7-7C5D-4C54-8A9A-D54F8833D434}" name="Units" dataDxfId="82"/>
+    <tableColumn id="4" xr3:uid="{6EAA6194-27E9-4B7C-8A4D-8C0FE7B617F4}" name="Distribution Type" dataDxfId="81"/>
+    <tableColumn id="5" xr3:uid="{75BC5E4C-C28D-4614-8AB6-165A9F7FE7CE}" name="Parameter 1" dataDxfId="80"/>
+    <tableColumn id="6" xr3:uid="{F5AD0C00-9187-4F91-ADA7-5B461FC355CE}" name="Parameter 2" dataDxfId="79"/>
+    <tableColumn id="7" xr3:uid="{34B0A2DF-5607-43F6-AA9E-1106CCB7621B}" name="Parameter 3" dataDxfId="78"/>
+    <tableColumn id="8" xr3:uid="{B0950426-083D-4CE9-A30E-9D71766BA154}" name="Parameter 4" dataDxfId="77"/>
+    <tableColumn id="14" xr3:uid="{88E7A84D-F80D-416C-9037-2E5927AE2697}" name="Parameter 5" dataDxfId="76"/>
+    <tableColumn id="15" xr3:uid="{E3DCF8BA-29B1-4A24-B6E6-DE9435CB3AC9}" name="Parameter 6" dataDxfId="75"/>
+    <tableColumn id="11" xr3:uid="{E8661EBF-62F4-4D4A-BCDC-7C8ABD4866B0}" name="Lower Limit" dataDxfId="74"/>
+    <tableColumn id="12" xr3:uid="{83DA3A0E-E097-4281-9822-6FE3F8FB0CDD}" name="Upper Limit" dataDxfId="73"/>
+    <tableColumn id="13" xr3:uid="{24B0E0E0-CA9C-4655-9B23-EA0BBD517B67}" name="Step" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{81C05191-4139-4D49-BA19-E7D2B74357F9}" name="Table15681021012" displayName="Table15681021012" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{81C05191-4139-4D49-BA19-E7D2B74357F9}" name="Table15681021012" displayName="Table15681021012" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="69">
   <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{64A27C3D-2E18-40E6-9166-742BDA2B413C}" name="Phase" dataDxfId="74"/>
-    <tableColumn id="1" xr3:uid="{0243CFE4-EBE7-4500-A226-23C63BE2FB81}" name="Category" dataDxfId="73"/>
-    <tableColumn id="2" xr3:uid="{69F68BF8-9E6A-4766-AB29-A8B943A84522}" name="Name" dataDxfId="72"/>
-    <tableColumn id="10" xr3:uid="{1E4511F0-B286-4973-A437-9638677030CA}" name="Description" dataDxfId="71"/>
-    <tableColumn id="3" xr3:uid="{B80720A6-55E5-4A17-9FE9-9951AF480E02}" name="Units" dataDxfId="70"/>
-    <tableColumn id="4" xr3:uid="{54B33DED-7F55-4D76-B95F-B7050BBA4BD1}" name="Distribution Type" dataDxfId="69"/>
-    <tableColumn id="5" xr3:uid="{BC7C6514-68B9-48F6-9938-4088DF28B37C}" name="Parameter 1" dataDxfId="68"/>
-    <tableColumn id="6" xr3:uid="{4D372042-F7DE-4E72-A309-C4266E0FA9E8}" name="Parameter 2" dataDxfId="67"/>
-    <tableColumn id="7" xr3:uid="{8D92705D-1A42-46F5-89EA-C4113CC26587}" name="Parameter 3" dataDxfId="66"/>
-    <tableColumn id="8" xr3:uid="{13B56E18-7C36-4950-847A-A7544475E1D1}" name="Parameter 4" dataDxfId="65"/>
-    <tableColumn id="14" xr3:uid="{2649C7B2-1C48-4B13-969D-684D0045538B}" name="Parameter 5" dataDxfId="64"/>
-    <tableColumn id="15" xr3:uid="{5D6C4F8D-D31E-4EED-BABF-A0A688F3A916}" name="Parameter 6" dataDxfId="63"/>
-    <tableColumn id="11" xr3:uid="{1CB1896E-F77C-4DFC-9AB0-D0C102F3F80F}" name="Lower Limit" dataDxfId="62"/>
-    <tableColumn id="12" xr3:uid="{837665AD-748D-4B51-9CCA-780B67A76815}" name="Upper Limit" dataDxfId="61"/>
-    <tableColumn id="13" xr3:uid="{A8F2935C-D451-47EA-A1E1-1E4F0CAE8D87}" name="Step" dataDxfId="60"/>
+    <tableColumn id="9" xr3:uid="{64A27C3D-2E18-40E6-9166-742BDA2B413C}" name="Phase" dataDxfId="68"/>
+    <tableColumn id="1" xr3:uid="{0243CFE4-EBE7-4500-A226-23C63BE2FB81}" name="Category" dataDxfId="67"/>
+    <tableColumn id="2" xr3:uid="{69F68BF8-9E6A-4766-AB29-A8B943A84522}" name="Name" dataDxfId="66"/>
+    <tableColumn id="10" xr3:uid="{1E4511F0-B286-4973-A437-9638677030CA}" name="Description" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{B80720A6-55E5-4A17-9FE9-9951AF480E02}" name="Units" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{54B33DED-7F55-4D76-B95F-B7050BBA4BD1}" name="Distribution Type" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{BC7C6514-68B9-48F6-9938-4088DF28B37C}" name="Parameter 1" dataDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{4D372042-F7DE-4E72-A309-C4266E0FA9E8}" name="Parameter 2" dataDxfId="61"/>
+    <tableColumn id="7" xr3:uid="{8D92705D-1A42-46F5-89EA-C4113CC26587}" name="Parameter 3" dataDxfId="60"/>
+    <tableColumn id="8" xr3:uid="{13B56E18-7C36-4950-847A-A7544475E1D1}" name="Parameter 4" dataDxfId="59"/>
+    <tableColumn id="14" xr3:uid="{2649C7B2-1C48-4B13-969D-684D0045538B}" name="Parameter 5" dataDxfId="58"/>
+    <tableColumn id="15" xr3:uid="{5D6C4F8D-D31E-4EED-BABF-A0A688F3A916}" name="Parameter 6" dataDxfId="57"/>
+    <tableColumn id="11" xr3:uid="{1CB1896E-F77C-4DFC-9AB0-D0C102F3F80F}" name="Lower Limit" dataDxfId="56"/>
+    <tableColumn id="12" xr3:uid="{837665AD-748D-4B51-9CCA-780B67A76815}" name="Upper Limit" dataDxfId="55"/>
+    <tableColumn id="13" xr3:uid="{A8F2935C-D451-47EA-A1E1-1E4F0CAE8D87}" name="Step" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{2EC220FC-5886-477C-8B2C-57082D8749AA}" name="Table1568102101213" displayName="Table1568102101213" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{2EC220FC-5886-477C-8B2C-57082D8749AA}" name="Table1568102101213" displayName="Table1568102101213" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="51">
   <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{525577E1-B46F-47FB-A042-A56D8D45D9AD}" name="Phase" dataDxfId="54"/>
-    <tableColumn id="1" xr3:uid="{30AFC0FE-4503-4A4B-91CA-E5B88AA24F98}" name="Category" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{6333C26F-3D36-4A65-8F1B-CC515ADCE181}" name="Name" dataDxfId="52"/>
-    <tableColumn id="10" xr3:uid="{057A52C2-DED0-48A5-8844-3950CD398F8D}" name="Description" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{EF447B65-8A6A-4F12-ABCB-7BFE84B734A9}" name="Units" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{6E658D46-B4D3-46B1-A15B-9F0095A7EADD}" name="Distribution Type" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{FE235A77-6EFF-4D9A-926F-ACE5D51D4BC8}" name="Parameter 1" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{26694561-3958-440C-BDDC-2DB16EB8A614}" name="Parameter 2" dataDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{DA96F9A2-3DEB-4C42-BECF-B9C30ADA7428}" name="Parameter 3" dataDxfId="46"/>
-    <tableColumn id="8" xr3:uid="{5F8A48E3-9BBF-4210-88D8-F668C1FD845D}" name="Parameter 4" dataDxfId="45"/>
-    <tableColumn id="14" xr3:uid="{21514092-10F7-41E0-B078-A15175C73E93}" name="Parameter 5" dataDxfId="44"/>
-    <tableColumn id="15" xr3:uid="{8BFA8A6A-2BCB-4512-8B77-28D2C28FEEE3}" name="Parameter 6" dataDxfId="43"/>
-    <tableColumn id="11" xr3:uid="{9CB23DDB-2513-48F3-960F-EF0D57CD9724}" name="Lower Limit" dataDxfId="42"/>
-    <tableColumn id="12" xr3:uid="{EDE53E3A-8BAE-4FD6-9C38-CD4B63274C67}" name="Upper Limit" dataDxfId="41"/>
-    <tableColumn id="13" xr3:uid="{980D57FA-1EDD-484A-9D56-BF7EAA580C8D}" name="Step" dataDxfId="40"/>
+    <tableColumn id="9" xr3:uid="{525577E1-B46F-47FB-A042-A56D8D45D9AD}" name="Phase" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{30AFC0FE-4503-4A4B-91CA-E5B88AA24F98}" name="Category" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{6333C26F-3D36-4A65-8F1B-CC515ADCE181}" name="Name" dataDxfId="48"/>
+    <tableColumn id="10" xr3:uid="{057A52C2-DED0-48A5-8844-3950CD398F8D}" name="Description" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{EF447B65-8A6A-4F12-ABCB-7BFE84B734A9}" name="Units" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{6E658D46-B4D3-46B1-A15B-9F0095A7EADD}" name="Distribution Type" dataDxfId="45"/>
+    <tableColumn id="5" xr3:uid="{FE235A77-6EFF-4D9A-926F-ACE5D51D4BC8}" name="Parameter 1" dataDxfId="44"/>
+    <tableColumn id="6" xr3:uid="{26694561-3958-440C-BDDC-2DB16EB8A614}" name="Parameter 2" dataDxfId="43"/>
+    <tableColumn id="7" xr3:uid="{DA96F9A2-3DEB-4C42-BECF-B9C30ADA7428}" name="Parameter 3" dataDxfId="42"/>
+    <tableColumn id="8" xr3:uid="{5F8A48E3-9BBF-4210-88D8-F668C1FD845D}" name="Parameter 4" dataDxfId="41"/>
+    <tableColumn id="14" xr3:uid="{21514092-10F7-41E0-B078-A15175C73E93}" name="Parameter 5" dataDxfId="40"/>
+    <tableColumn id="15" xr3:uid="{8BFA8A6A-2BCB-4512-8B77-28D2C28FEEE3}" name="Parameter 6" dataDxfId="39"/>
+    <tableColumn id="11" xr3:uid="{9CB23DDB-2513-48F3-960F-EF0D57CD9724}" name="Lower Limit" dataDxfId="38"/>
+    <tableColumn id="12" xr3:uid="{EDE53E3A-8BAE-4FD6-9C38-CD4B63274C67}" name="Upper Limit" dataDxfId="37"/>
+    <tableColumn id="13" xr3:uid="{980D57FA-1EDD-484A-9D56-BF7EAA580C8D}" name="Step" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3DDD9CB2-968B-4A43-A20B-C749950155AA}" name="Table156810210121314" displayName="Table156810210121314" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3DDD9CB2-968B-4A43-A20B-C749950155AA}" name="Table156810210121314" displayName="Table156810210121314" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="33">
   <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{6B814874-1824-4E56-A967-04F9F6F3E584}" name="Phase" dataDxfId="34"/>
-    <tableColumn id="1" xr3:uid="{FE1635BE-F6C3-4D5B-B06E-7A92EBAB074D}" name="Category" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{9C16A715-E236-4930-A633-7510E082392C}" name="Name" dataDxfId="32"/>
-    <tableColumn id="10" xr3:uid="{B556C16A-1909-46E7-BC6D-8479761F1F65}" name="Description" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{5EFB6F3C-9894-43AA-AFAC-1013F8F0714B}" name="Units" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{6E3C1049-1D84-4FD5-B7CF-1E130CD32BCA}" name="Distribution Type" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{57E979B1-A630-4AC5-8C4D-CED1A62F587D}" name="Parameter 1" dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{C9EF8DDD-DA1F-44E2-AC90-B6993C60CF1F}" name="Parameter 2" dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{6FEFD03F-983B-47E2-9525-7EDD875A9C7C}" name="Parameter 3" dataDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{0B661DB2-D286-4AEE-88C3-124B37F1B246}" name="Parameter 4" dataDxfId="25"/>
-    <tableColumn id="14" xr3:uid="{08C4ACC8-5A7B-4864-96E4-CF69FD654892}" name="Parameter 5" dataDxfId="24"/>
-    <tableColumn id="15" xr3:uid="{5505BBCC-5C52-4400-9C19-9ED7DBB490B8}" name="Parameter 6" dataDxfId="23"/>
-    <tableColumn id="11" xr3:uid="{E151AC3B-28ED-4186-A803-48B7F8B7AE5B}" name="Lower Limit" dataDxfId="22"/>
-    <tableColumn id="12" xr3:uid="{223709CC-AD09-4677-85AC-DF8A1619BF81}" name="Upper Limit" dataDxfId="21"/>
-    <tableColumn id="13" xr3:uid="{5FAAB5F5-A70D-4A6B-BE36-5CC1FD787BC5}" name="Step" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{6B814874-1824-4E56-A967-04F9F6F3E584}" name="Phase" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{FE1635BE-F6C3-4D5B-B06E-7A92EBAB074D}" name="Category" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{9C16A715-E236-4930-A633-7510E082392C}" name="Name" dataDxfId="30"/>
+    <tableColumn id="10" xr3:uid="{B556C16A-1909-46E7-BC6D-8479761F1F65}" name="Description" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{5EFB6F3C-9894-43AA-AFAC-1013F8F0714B}" name="Units" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{6E3C1049-1D84-4FD5-B7CF-1E130CD32BCA}" name="Distribution Type" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{57E979B1-A630-4AC5-8C4D-CED1A62F587D}" name="Parameter 1" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{C9EF8DDD-DA1F-44E2-AC90-B6993C60CF1F}" name="Parameter 2" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{6FEFD03F-983B-47E2-9525-7EDD875A9C7C}" name="Parameter 3" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{0B661DB2-D286-4AEE-88C3-124B37F1B246}" name="Parameter 4" dataDxfId="23"/>
+    <tableColumn id="14" xr3:uid="{08C4ACC8-5A7B-4864-96E4-CF69FD654892}" name="Parameter 5" dataDxfId="22"/>
+    <tableColumn id="15" xr3:uid="{5505BBCC-5C52-4400-9C19-9ED7DBB490B8}" name="Parameter 6" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{E151AC3B-28ED-4186-A803-48B7F8B7AE5B}" name="Lower Limit" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{223709CC-AD09-4677-85AC-DF8A1619BF81}" name="Upper Limit" dataDxfId="19"/>
+    <tableColumn id="13" xr3:uid="{5FAAB5F5-A70D-4A6B-BE36-5CC1FD787BC5}" name="Step" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3909,7 +3800,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4017,7 +3908,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -4045,7 +3936,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
@@ -4263,20 +4154,12 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L2 A4:L9 A3:D3 F3:L3">
-    <cfRule type="expression" dxfId="39" priority="3">
+  <conditionalFormatting sqref="A2:L9">
+    <cfRule type="expression" dxfId="35" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="4">
+    <cfRule type="expression" dxfId="34" priority="2">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="37" priority="1">
-      <formula>ISBLANK($F3)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="2">
-      <formula>NOT((COLUMN(E3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -4296,7 +4179,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4404,7 +4287,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -4432,7 +4315,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
@@ -4650,20 +4533,12 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L2 A4:L9 A3:D3 F3:L3">
-    <cfRule type="expression" dxfId="19" priority="3">
+  <conditionalFormatting sqref="A2:L9">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="4">
+    <cfRule type="expression" dxfId="16" priority="2">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="17" priority="1">
-      <formula>ISBLANK($F3)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="2">
-      <formula>NOT((COLUMN(E3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -5083,10 +4958,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097870CC-1A0F-461E-BDFD-29BDDFDDF05C}">
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5098,7 +4973,7 @@
     <col min="5" max="15" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -5145,7 +5020,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>70</v>
       </c>
@@ -5153,7 +5028,7 @@
         <v>70</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>53</v>
@@ -5164,16 +5039,14 @@
       <c r="F2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="5">
-        <v>0</v>
-      </c>
+      <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="6"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="17">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="N2" s="17">
         <v>50000000</v>
@@ -5182,7 +5055,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>70</v>
       </c>
@@ -5190,20 +5063,18 @@
         <v>70</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>93</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="9">
-        <v>-1</v>
-      </c>
+      <c r="G3" s="9"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="10"/>
@@ -5219,7 +5090,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -5227,7 +5098,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>52</v>
@@ -5238,25 +5109,23 @@
       <c r="F4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="12">
-        <v>747.86950000000002</v>
-      </c>
+      <c r="G4" s="12"/>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
-      <c r="M4" s="17">
-        <v>0</v>
+      <c r="M4" s="18">
+        <v>10000</v>
       </c>
       <c r="N4" s="18">
         <v>50000000</v>
       </c>
       <c r="O4" s="18">
-        <v>1.0000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>71</v>
       </c>
@@ -5264,23 +5133,19 @@
         <v>71</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>94</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="9">
-        <v>3.0319702616531905</v>
-      </c>
-      <c r="H5" s="9">
-        <v>8.0319702616531909</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="10"/>
       <c r="K5" s="2"/>
@@ -5291,12 +5156,11 @@
       <c r="N5" s="19">
         <v>10</v>
       </c>
-      <c r="O5" s="18">
-        <v>1.0000000000000001E-9</v>
-      </c>
-      <c r="Q5" s="21"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O5" s="19">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>72</v>
       </c>
@@ -5304,7 +5168,7 @@
         <v>72</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>73</v>
@@ -5315,16 +5179,14 @@
       <c r="F6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="12">
-        <v>0</v>
-      </c>
+      <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="13"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
       <c r="M6" s="18">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="N6" s="18">
         <v>50000000</v>
@@ -5333,7 +5195,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>72</v>
       </c>
@@ -5341,20 +5203,18 @@
         <v>72</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>95</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="12">
-        <v>-1</v>
-      </c>
+      <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="13"/>
@@ -5370,7 +5230,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>71</v>
       </c>
@@ -5390,7 +5250,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="9">
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -5403,11 +5263,11 @@
       <c r="N8" s="9">
         <v>1</v>
       </c>
-      <c r="O8" s="18">
-        <v>1.0000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O8" s="9">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>71</v>
       </c>
@@ -5427,7 +5287,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="9">
-        <v>0.55555555555555558</v>
+        <v>0.5</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -5440,11 +5300,11 @@
       <c r="N9" s="9">
         <v>1</v>
       </c>
-      <c r="O9" s="18">
-        <v>1.0000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O9" s="9">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>71</v>
       </c>
@@ -5464,7 +5324,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="9">
-        <v>0.1111111111111111</v>
+        <v>0.5</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -5477,11 +5337,11 @@
       <c r="N10" s="9">
         <v>1</v>
       </c>
-      <c r="O10" s="18">
-        <v>1.0000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O10" s="9">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>71</v>
       </c>
@@ -5518,7 +5378,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>71</v>
       </c>
@@ -5555,7 +5415,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>71</v>
       </c>
@@ -5592,7 +5452,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>71</v>
       </c>
@@ -5629,18 +5489,18 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>70</v>
       </c>
       <c r="B15" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>115</v>
-      </c>
       <c r="D15" s="12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>68</v>
@@ -5649,7 +5509,7 @@
         <v>3</v>
       </c>
       <c r="G15" s="12">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
@@ -5666,18 +5526,18 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>70</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>68</v>
@@ -5686,7 +5546,7 @@
         <v>3</v>
       </c>
       <c r="G16" s="12">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
@@ -5708,13 +5568,13 @@
         <v>70</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>68</v>
@@ -5723,7 +5583,7 @@
         <v>3</v>
       </c>
       <c r="G17" s="12">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
@@ -5745,13 +5605,13 @@
         <v>70</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>68</v>
@@ -5760,7 +5620,7 @@
         <v>3</v>
       </c>
       <c r="G18" s="12">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
@@ -5782,13 +5642,13 @@
         <v>70</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>68</v>
@@ -5797,7 +5657,7 @@
         <v>3</v>
       </c>
       <c r="G19" s="12">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
@@ -5819,13 +5679,13 @@
         <v>70</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>68</v>
@@ -5834,7 +5694,7 @@
         <v>3</v>
       </c>
       <c r="G20" s="12">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
@@ -5856,13 +5716,13 @@
         <v>72</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>68</v>
@@ -5871,7 +5731,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="12">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
@@ -5893,13 +5753,13 @@
         <v>72</v>
       </c>
       <c r="B22" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>127</v>
-      </c>
       <c r="D22" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>68</v>
@@ -5908,7 +5768,7 @@
         <v>3</v>
       </c>
       <c r="G22" s="12">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
@@ -5930,13 +5790,13 @@
         <v>72</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>68</v>
@@ -5945,7 +5805,7 @@
         <v>3</v>
       </c>
       <c r="G23" s="12">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
@@ -5967,13 +5827,13 @@
         <v>72</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>68</v>
@@ -5982,7 +5842,7 @@
         <v>3</v>
       </c>
       <c r="G24" s="12">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
@@ -6004,13 +5864,13 @@
         <v>72</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>68</v>
@@ -6019,7 +5879,7 @@
         <v>3</v>
       </c>
       <c r="G25" s="12">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
@@ -6044,10 +5904,10 @@
         <v>152</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>68</v>
@@ -6056,7 +5916,7 @@
         <v>3</v>
       </c>
       <c r="G26" s="12">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="H26" s="12"/>
       <c r="I26" s="12"/>
@@ -6078,13 +5938,13 @@
         <v>71</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>68</v>
@@ -6093,7 +5953,7 @@
         <v>3</v>
       </c>
       <c r="G27" s="12">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
@@ -6118,10 +5978,10 @@
         <v>104</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>68</v>
@@ -6130,7 +5990,7 @@
         <v>3</v>
       </c>
       <c r="G28" s="12">
-        <v>0.125</v>
+        <v>0.1</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
@@ -6144,7 +6004,7 @@
         <v>1</v>
       </c>
       <c r="O28" s="12">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -6155,10 +6015,10 @@
         <v>105</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>68</v>
@@ -6167,7 +6027,7 @@
         <v>3</v>
       </c>
       <c r="G29" s="12">
-        <v>6.25E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
@@ -6181,7 +6041,7 @@
         <v>1</v>
       </c>
       <c r="O29" s="12">
-        <v>1E-4</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -6192,10 +6052,10 @@
         <v>106</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>68</v>
@@ -6204,7 +6064,7 @@
         <v>3</v>
       </c>
       <c r="G30" s="12">
-        <v>6.25E-2</v>
+        <v>0.3</v>
       </c>
       <c r="H30" s="12"/>
       <c r="I30" s="12"/>
@@ -6218,7 +6078,7 @@
         <v>1</v>
       </c>
       <c r="O30" s="12">
-        <v>1E-4</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
@@ -6229,10 +6089,10 @@
         <v>153</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>68</v>
@@ -6241,7 +6101,7 @@
         <v>3</v>
       </c>
       <c r="G31" s="12">
-        <v>0.125</v>
+        <v>0.15</v>
       </c>
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
@@ -6266,10 +6126,10 @@
         <v>108</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>68</v>
@@ -6278,7 +6138,7 @@
         <v>3</v>
       </c>
       <c r="G32" s="12">
-        <v>0.125</v>
+        <v>0.1</v>
       </c>
       <c r="H32" s="12"/>
       <c r="I32" s="12"/>
@@ -6298,10 +6158,10 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A2:L32">
-    <cfRule type="expression" dxfId="155" priority="43">
+    <cfRule type="expression" dxfId="143" priority="43">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="154" priority="44">
+    <cfRule type="expression" dxfId="142" priority="44">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6322,7 +6182,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6430,7 +6290,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -6458,7 +6318,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
@@ -6677,10 +6537,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:L9">
-    <cfRule type="expression" dxfId="137" priority="1">
+    <cfRule type="expression" dxfId="125" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="136" priority="2">
+    <cfRule type="expression" dxfId="124" priority="2">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6701,7 +6561,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B4" sqref="B4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6809,7 +6669,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -6837,7 +6697,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
@@ -7055,20 +6915,12 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L2 A4:L9 A3:D3 F3:L3">
-    <cfRule type="expression" dxfId="119" priority="3">
+  <conditionalFormatting sqref="A2:L9">
+    <cfRule type="expression" dxfId="107" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="4">
+    <cfRule type="expression" dxfId="106" priority="2">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="117" priority="1">
-      <formula>ISBLANK($F3)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="116" priority="2">
-      <formula>NOT((COLUMN(E3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -7088,7 +6940,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7196,7 +7048,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -7224,7 +7076,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
@@ -7442,20 +7294,12 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L2 A4:L9 A3:D3 F3:L3">
-    <cfRule type="expression" dxfId="99" priority="5">
+  <conditionalFormatting sqref="A2:L9">
+    <cfRule type="expression" dxfId="89" priority="3">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="6">
+    <cfRule type="expression" dxfId="88" priority="4">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="97" priority="1">
-      <formula>ISBLANK($F3)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="96" priority="2">
-      <formula>NOT((COLUMN(E3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -7475,7 +7319,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7583,7 +7427,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -7611,7 +7455,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
@@ -7829,20 +7673,12 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L2 A4:L9 A3:D3 F3:L3">
-    <cfRule type="expression" dxfId="79" priority="3">
+  <conditionalFormatting sqref="A2:L9">
+    <cfRule type="expression" dxfId="71" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="4">
+    <cfRule type="expression" dxfId="70" priority="2">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="77" priority="1">
-      <formula>ISBLANK($F3)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="76" priority="2">
-      <formula>NOT((COLUMN(E3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -7862,7 +7698,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7970,7 +7806,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -7998,7 +7834,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
@@ -8216,20 +8052,12 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L2 A4:L9 A3:D3 F3:L3">
-    <cfRule type="expression" dxfId="59" priority="3">
+  <conditionalFormatting sqref="A2:L9">
+    <cfRule type="expression" dxfId="53" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="4">
+    <cfRule type="expression" dxfId="52" priority="2">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="57" priority="1">
-      <formula>ISBLANK($F3)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="56" priority="2">
-      <formula>NOT((COLUMN(E3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Merged PR 45: Updating from master_dev
</commit_message>
<xml_diff>
--- a/InputFiles/DefineScenario.xlsx
+++ b/InputFiles/DefineScenario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERAZA\Documents\Tasking\(4) EPA Stuff\Task 5 Repo\WideAreaDecon\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE4FE90-1089-49B4-8F1D-E3C95D168FA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9F6AF9-D8C7-4947-8663-BAC9963E88A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="649" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="649" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal - File Info" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="154">
   <si>
     <t>SCWAD</t>
   </si>
@@ -358,12 +358,6 @@
     <t>Surface Type Breakout</t>
   </si>
   <si>
-    <t>Indoor Interior</t>
-  </si>
-  <si>
-    <t>Indoor Exterior</t>
-  </si>
-  <si>
     <t>Indoor Ceilings</t>
   </si>
   <si>
@@ -382,9 +376,6 @@
     <t>Fraction of residential buildings that are interior walls</t>
   </si>
   <si>
-    <t>Fraction of residential buildings that are exterior walls</t>
-  </si>
-  <si>
     <t>Fraction of residential buildings that are ceilings walls</t>
   </si>
   <si>
@@ -442,9 +433,6 @@
     <t>Underground Surface Type Breakout</t>
   </si>
   <si>
-    <t>Underground Interior</t>
-  </si>
-  <si>
     <t>Underground Ceilings</t>
   </si>
   <si>
@@ -505,10 +493,19 @@
     <t>The fraction of surface outdoors which is building exterior</t>
   </si>
   <si>
-    <t>The fraction of surface indoors which is building exterior</t>
-  </si>
-  <si>
     <t>log(cfu / m^2)</t>
+  </si>
+  <si>
+    <t>Indoor Walls</t>
+  </si>
+  <si>
+    <t>Underground Walls</t>
+  </si>
+  <si>
+    <t>Underground HVAC</t>
+  </si>
+  <si>
+    <t>Indoor HVAC</t>
   </si>
 </sst>
 </file>
@@ -3288,8 +3285,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{77E3C927-1FC6-443B-87ED-00E2959DD317}" name="Table1568" displayName="Table1568" ref="A1:O33" totalsRowShown="0" tableBorderDxfId="141">
-  <autoFilter ref="A1:O33" xr:uid="{58F00973-C0E2-47D9-9C5E-C7B7F684A0C3}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{77E3C927-1FC6-443B-87ED-00E2959DD317}" name="Table1568" displayName="Table1568" ref="A1:O32" totalsRowShown="0" tableBorderDxfId="141">
+  <autoFilter ref="A1:O32" xr:uid="{58F00973-C0E2-47D9-9C5E-C7B7F684A0C3}"/>
   <tableColumns count="15">
     <tableColumn id="9" xr3:uid="{62A6D655-D638-4005-9525-C140421ED9AB}" name="Phase" dataDxfId="140"/>
     <tableColumn id="1" xr3:uid="{1BC04ADD-0426-4785-9F97-FCE0BCC1E547}" name="Category" dataDxfId="139"/>
@@ -3312,8 +3309,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{72F3CA1E-AAFF-44BC-A114-2AA862291D9E}" name="Table1568102" displayName="Table1568102" ref="A1:O10" totalsRowShown="0" tableBorderDxfId="123">
-  <autoFilter ref="A1:O10" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{72F3CA1E-AAFF-44BC-A114-2AA862291D9E}" name="Table1568102" displayName="Table1568102" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="123">
+  <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
     <tableColumn id="9" xr3:uid="{8FD38CEB-1D1A-41E8-821F-58DD4FBD85EB}" name="Phase" dataDxfId="122"/>
     <tableColumn id="1" xr3:uid="{574AE483-6154-4EC6-AC18-5FDEBC0931CD}" name="Category" dataDxfId="121"/>
@@ -3336,8 +3333,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{88C3C7FF-7D66-4C1C-A80E-12CD3AFBFB8D}" name="Table156810210" displayName="Table156810210" ref="A1:O10" totalsRowShown="0" tableBorderDxfId="105">
-  <autoFilter ref="A1:O10" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{88C3C7FF-7D66-4C1C-A80E-12CD3AFBFB8D}" name="Table156810210" displayName="Table156810210" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="105">
+  <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
     <tableColumn id="9" xr3:uid="{5AC7EE20-3F52-40E0-87F1-21D82A7C3AA2}" name="Phase" dataDxfId="104"/>
     <tableColumn id="1" xr3:uid="{9A9754BC-4FF9-4BBA-B750-B911CE430E6A}" name="Category" dataDxfId="103"/>
@@ -3360,8 +3357,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6794810C-E49F-4CB0-9B2F-0FA2655BD884}" name="Table15681021011" displayName="Table15681021011" ref="A1:O10" totalsRowShown="0" tableBorderDxfId="87">
-  <autoFilter ref="A1:O10" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6794810C-E49F-4CB0-9B2F-0FA2655BD884}" name="Table15681021011" displayName="Table15681021011" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="87">
+  <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
     <tableColumn id="9" xr3:uid="{5DEAB66E-0CAB-4BF7-B4EA-D8D12FB47328}" name="Phase" dataDxfId="86"/>
     <tableColumn id="1" xr3:uid="{69C64F5C-9979-4ACA-9A42-C1032E3D98BA}" name="Category" dataDxfId="85"/>
@@ -3384,8 +3381,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{81C05191-4139-4D49-BA19-E7D2B74357F9}" name="Table15681021012" displayName="Table15681021012" ref="A1:O10" totalsRowShown="0" tableBorderDxfId="69">
-  <autoFilter ref="A1:O10" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{81C05191-4139-4D49-BA19-E7D2B74357F9}" name="Table15681021012" displayName="Table15681021012" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="69">
+  <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
     <tableColumn id="9" xr3:uid="{64A27C3D-2E18-40E6-9166-742BDA2B413C}" name="Phase" dataDxfId="68"/>
     <tableColumn id="1" xr3:uid="{0243CFE4-EBE7-4500-A226-23C63BE2FB81}" name="Category" dataDxfId="67"/>
@@ -3408,8 +3405,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{2EC220FC-5886-477C-8B2C-57082D8749AA}" name="Table1568102101213" displayName="Table1568102101213" ref="A1:O10" totalsRowShown="0" tableBorderDxfId="51">
-  <autoFilter ref="A1:O10" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{2EC220FC-5886-477C-8B2C-57082D8749AA}" name="Table1568102101213" displayName="Table1568102101213" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="51">
+  <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
     <tableColumn id="9" xr3:uid="{525577E1-B46F-47FB-A042-A56D8D45D9AD}" name="Phase" dataDxfId="50"/>
     <tableColumn id="1" xr3:uid="{30AFC0FE-4503-4A4B-91CA-E5B88AA24F98}" name="Category" dataDxfId="49"/>
@@ -3432,8 +3429,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3DDD9CB2-968B-4A43-A20B-C749950155AA}" name="Table156810210121314" displayName="Table156810210121314" ref="A1:O10" totalsRowShown="0" tableBorderDxfId="33">
-  <autoFilter ref="A1:O10" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3DDD9CB2-968B-4A43-A20B-C749950155AA}" name="Table156810210121314" displayName="Table156810210121314" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="33">
+  <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
     <tableColumn id="9" xr3:uid="{6B814874-1824-4E56-A967-04F9F6F3E584}" name="Phase" dataDxfId="32"/>
     <tableColumn id="1" xr3:uid="{FE1635BE-F6C3-4D5B-B06E-7A92EBAB074D}" name="Category" dataDxfId="31"/>
@@ -3456,8 +3453,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{FBB513AC-2D2B-4552-8740-9D611743FE70}" name="Table15681021012131415" displayName="Table15681021012131415" ref="A1:O10" totalsRowShown="0" tableBorderDxfId="15">
-  <autoFilter ref="A1:O10" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{FBB513AC-2D2B-4552-8740-9D611743FE70}" name="Table15681021012131415" displayName="Table15681021012131415" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="15">
+  <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
     <tableColumn id="9" xr3:uid="{2035FE2F-0A32-497E-B1E0-30D237A0E150}" name="Phase" dataDxfId="14"/>
     <tableColumn id="1" xr3:uid="{F814DF41-D024-449F-AF42-62D43153FFB7}" name="Category" dataDxfId="13"/>
@@ -3800,10 +3797,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E43DD9-157B-49FC-9197-883D6786BB87}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3911,7 +3908,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -3939,13 +3936,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>104</v>
+        <v>150</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>68</v>
@@ -3954,7 +3951,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="12">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -3976,13 +3973,13 @@
         <v>71</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>68</v>
@@ -3991,7 +3988,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="12">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
@@ -4013,13 +4010,13 @@
         <v>71</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>68</v>
@@ -4028,7 +4025,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="12">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
@@ -4050,13 +4047,13 @@
         <v>71</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>68</v>
@@ -4065,7 +4062,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="12">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
@@ -4087,13 +4084,13 @@
         <v>71</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>68</v>
@@ -4124,13 +4121,13 @@
         <v>71</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>68</v>
@@ -4139,7 +4136,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="12">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
@@ -4156,45 +4153,8 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="12">
-        <v>0</v>
-      </c>
-      <c r="N10" s="12">
-        <v>1</v>
-      </c>
-      <c r="O10" s="12">
-        <v>0.01</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L10">
+  <conditionalFormatting sqref="A2:L9">
     <cfRule type="expression" dxfId="35" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
@@ -4203,7 +4163,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F10" xr:uid="{31A8EBC6-6F05-479C-82BC-9274F3B72E56}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F9" xr:uid="{31A8EBC6-6F05-479C-82BC-9274F3B72E56}">
       <formula1>Validation_Distribution_Types</formula1>
     </dataValidation>
   </dataValidations>
@@ -4216,10 +4176,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07EF9366-5AFF-4F5A-9471-F50914749AD6}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4327,7 +4287,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -4355,13 +4315,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>104</v>
+        <v>150</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>68</v>
@@ -4370,7 +4330,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="12">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -4392,13 +4352,13 @@
         <v>71</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>68</v>
@@ -4407,7 +4367,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="12">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
@@ -4429,13 +4389,13 @@
         <v>71</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>68</v>
@@ -4444,7 +4404,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="12">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
@@ -4466,13 +4426,13 @@
         <v>71</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>68</v>
@@ -4481,7 +4441,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="12">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
@@ -4503,13 +4463,13 @@
         <v>71</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>68</v>
@@ -4540,13 +4500,13 @@
         <v>71</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>68</v>
@@ -4555,7 +4515,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="12">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
@@ -4572,45 +4532,8 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="12">
-        <v>0</v>
-      </c>
-      <c r="N10" s="12">
-        <v>1</v>
-      </c>
-      <c r="O10" s="12">
-        <v>0.01</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L10">
+  <conditionalFormatting sqref="A2:L9">
     <cfRule type="expression" dxfId="17" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
@@ -4619,7 +4542,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F10" xr:uid="{FB9861EC-C1B9-4BC7-96DE-3903141525C5}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F9" xr:uid="{FB9861EC-C1B9-4BC7-96DE-3903141525C5}">
       <formula1>Validation_Distribution_Types</formula1>
     </dataValidation>
   </dataValidations>
@@ -5035,10 +4958,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097870CC-1A0F-461E-BDFD-29BDDFDDF05C}">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5105,7 +5028,7 @@
         <v>70</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>53</v>
@@ -5140,13 +5063,13 @@
         <v>70</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>93</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>3</v>
@@ -5175,7 +5098,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>52</v>
@@ -5210,13 +5133,13 @@
         <v>71</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>94</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>3</v>
@@ -5245,7 +5168,7 @@
         <v>72</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>73</v>
@@ -5280,13 +5203,13 @@
         <v>72</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>95</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>3</v>
@@ -5571,13 +5494,13 @@
         <v>70</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>68</v>
@@ -5608,13 +5531,13 @@
         <v>70</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>68</v>
@@ -5645,13 +5568,13 @@
         <v>70</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>68</v>
@@ -5682,13 +5605,13 @@
         <v>70</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>68</v>
@@ -5719,13 +5642,13 @@
         <v>70</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>68</v>
@@ -5756,13 +5679,13 @@
         <v>70</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>68</v>
@@ -5793,13 +5716,13 @@
         <v>72</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>68</v>
@@ -5830,13 +5753,13 @@
         <v>72</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>68</v>
@@ -5867,13 +5790,13 @@
         <v>72</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>68</v>
@@ -5904,13 +5827,13 @@
         <v>72</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>68</v>
@@ -5941,13 +5864,13 @@
         <v>72</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>68</v>
@@ -5978,13 +5901,13 @@
         <v>72</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>109</v>
+        <v>152</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>68</v>
@@ -6015,13 +5938,13 @@
         <v>71</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>104</v>
+        <v>150</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>68</v>
@@ -6030,7 +5953,7 @@
         <v>3</v>
       </c>
       <c r="G27" s="12">
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
@@ -6052,13 +5975,13 @@
         <v>71</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C28" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="D28" s="12" t="s">
         <v>145</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>153</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>68</v>
@@ -6067,7 +5990,7 @@
         <v>3</v>
       </c>
       <c r="G28" s="12">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
@@ -6089,13 +6012,13 @@
         <v>71</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>68</v>
@@ -6104,7 +6027,7 @@
         <v>3</v>
       </c>
       <c r="G29" s="12">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
@@ -6126,13 +6049,13 @@
         <v>71</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>68</v>
@@ -6141,7 +6064,7 @@
         <v>3</v>
       </c>
       <c r="G30" s="12">
-        <v>0.05</v>
+        <v>0.3</v>
       </c>
       <c r="H30" s="12"/>
       <c r="I30" s="12"/>
@@ -6163,13 +6086,13 @@
         <v>71</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>108</v>
+        <v>153</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>68</v>
@@ -6178,7 +6101,7 @@
         <v>3</v>
       </c>
       <c r="G31" s="12">
-        <v>0.3</v>
+        <v>0.15</v>
       </c>
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
@@ -6200,13 +6123,13 @@
         <v>71</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>68</v>
@@ -6215,7 +6138,7 @@
         <v>3</v>
       </c>
       <c r="G32" s="12">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="H32" s="12"/>
       <c r="I32" s="12"/>
@@ -6232,46 +6155,9 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A33" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B33" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="E33" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G33" s="12">
-        <v>0.1</v>
-      </c>
-      <c r="H33" s="12"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="16"/>
-      <c r="L33" s="16"/>
-      <c r="M33" s="12">
-        <v>0</v>
-      </c>
-      <c r="N33" s="12">
-        <v>1</v>
-      </c>
-      <c r="O33" s="12">
-        <v>0.01</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A2:L33">
+  <conditionalFormatting sqref="A2:L32">
     <cfRule type="expression" dxfId="143" priority="43">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
@@ -6280,7 +6166,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F33" xr:uid="{330BE9FB-867A-4350-A3CC-F1598E7F7C5E}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F32" xr:uid="{330BE9FB-867A-4350-A3CC-F1598E7F7C5E}">
       <formula1>Validation_Distribution_Types</formula1>
     </dataValidation>
   </dataValidations>
@@ -6293,10 +6179,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2CC74AC-9C8A-4982-AAA7-A84AB700668C}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6404,7 +6290,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -6432,13 +6318,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>104</v>
+        <v>150</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>68</v>
@@ -6447,7 +6333,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="12">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -6469,13 +6355,13 @@
         <v>71</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>68</v>
@@ -6484,7 +6370,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="12">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
@@ -6506,13 +6392,13 @@
         <v>71</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>68</v>
@@ -6521,7 +6407,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="12">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
@@ -6543,13 +6429,13 @@
         <v>71</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>68</v>
@@ -6558,7 +6444,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="12">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
@@ -6580,13 +6466,13 @@
         <v>71</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>68</v>
@@ -6617,13 +6503,13 @@
         <v>71</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>68</v>
@@ -6632,7 +6518,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="12">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
@@ -6649,45 +6535,8 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="12">
-        <v>0</v>
-      </c>
-      <c r="N10" s="12">
-        <v>1</v>
-      </c>
-      <c r="O10" s="12">
-        <v>0.01</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L10">
+  <conditionalFormatting sqref="A2:L9">
     <cfRule type="expression" dxfId="125" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
@@ -6696,7 +6545,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F10" xr:uid="{715A25B3-8A34-4C57-B072-9E97752CB3B7}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F9" xr:uid="{715A25B3-8A34-4C57-B072-9E97752CB3B7}">
       <formula1>Validation_Distribution_Types</formula1>
     </dataValidation>
   </dataValidations>
@@ -6709,10 +6558,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7042F79-A311-45CE-9A65-4502414AAE8E}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="B4" sqref="B4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6820,7 +6669,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -6848,13 +6697,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>104</v>
+        <v>150</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>68</v>
@@ -6863,7 +6712,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="12">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -6885,13 +6734,13 @@
         <v>71</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>68</v>
@@ -6900,7 +6749,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="12">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
@@ -6922,13 +6771,13 @@
         <v>71</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>68</v>
@@ -6937,7 +6786,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="12">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
@@ -6959,13 +6808,13 @@
         <v>71</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>68</v>
@@ -6974,7 +6823,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="12">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
@@ -6996,13 +6845,13 @@
         <v>71</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>68</v>
@@ -7033,13 +6882,13 @@
         <v>71</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>68</v>
@@ -7048,7 +6897,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="12">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
@@ -7065,45 +6914,8 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="12">
-        <v>0</v>
-      </c>
-      <c r="N10" s="12">
-        <v>1</v>
-      </c>
-      <c r="O10" s="12">
-        <v>0.01</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L10">
+  <conditionalFormatting sqref="A2:L9">
     <cfRule type="expression" dxfId="107" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
@@ -7112,7 +6924,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F10" xr:uid="{DA5A1EE8-224D-4BF6-A924-4AB90DE068C4}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F9" xr:uid="{DA5A1EE8-224D-4BF6-A924-4AB90DE068C4}">
       <formula1>Validation_Distribution_Types</formula1>
     </dataValidation>
   </dataValidations>
@@ -7125,10 +6937,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333733AB-F5E6-46AE-8B18-F38FE91E5E0A}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7236,7 +7048,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -7264,13 +7076,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>104</v>
+        <v>150</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>68</v>
@@ -7279,7 +7091,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="12">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -7301,13 +7113,13 @@
         <v>71</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>68</v>
@@ -7316,7 +7128,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="12">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
@@ -7338,13 +7150,13 @@
         <v>71</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>68</v>
@@ -7353,7 +7165,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="12">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
@@ -7375,13 +7187,13 @@
         <v>71</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>68</v>
@@ -7390,7 +7202,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="12">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
@@ -7412,13 +7224,13 @@
         <v>71</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>68</v>
@@ -7449,13 +7261,13 @@
         <v>71</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>68</v>
@@ -7464,7 +7276,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="12">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
@@ -7481,54 +7293,17 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="12">
-        <v>0</v>
-      </c>
-      <c r="N10" s="12">
-        <v>1</v>
-      </c>
-      <c r="O10" s="12">
-        <v>0.01</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L10">
-    <cfRule type="expression" dxfId="89" priority="1">
+  <conditionalFormatting sqref="A2:L9">
+    <cfRule type="expression" dxfId="89" priority="3">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="88" priority="2">
+    <cfRule type="expression" dxfId="88" priority="4">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F10" xr:uid="{BEA4092A-E6CF-486D-B7C9-E43ADA763306}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F9" xr:uid="{BEA4092A-E6CF-486D-B7C9-E43ADA763306}">
       <formula1>Validation_Distribution_Types</formula1>
     </dataValidation>
   </dataValidations>
@@ -7541,10 +7316,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{550F5AA7-2C47-4C71-A36F-C83AF51A7B16}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7652,7 +7427,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -7680,13 +7455,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>104</v>
+        <v>150</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>68</v>
@@ -7695,7 +7470,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="12">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -7717,13 +7492,13 @@
         <v>71</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>68</v>
@@ -7732,7 +7507,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="12">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
@@ -7754,13 +7529,13 @@
         <v>71</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>68</v>
@@ -7769,7 +7544,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="12">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
@@ -7791,13 +7566,13 @@
         <v>71</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>68</v>
@@ -7806,7 +7581,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="12">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
@@ -7828,13 +7603,13 @@
         <v>71</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>68</v>
@@ -7865,13 +7640,13 @@
         <v>71</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>68</v>
@@ -7880,7 +7655,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="12">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
@@ -7897,45 +7672,8 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="12">
-        <v>0</v>
-      </c>
-      <c r="N10" s="12">
-        <v>1</v>
-      </c>
-      <c r="O10" s="12">
-        <v>0.01</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L10">
+  <conditionalFormatting sqref="A2:L9">
     <cfRule type="expression" dxfId="71" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
@@ -7944,7 +7682,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F10" xr:uid="{30BC8E04-688C-4141-80C9-C8E8CC43E159}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F9" xr:uid="{30BC8E04-688C-4141-80C9-C8E8CC43E159}">
       <formula1>Validation_Distribution_Types</formula1>
     </dataValidation>
   </dataValidations>
@@ -7957,10 +7695,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{069E8A85-F700-42D5-83B0-8B7D70A63994}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8068,7 +7806,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -8096,13 +7834,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>104</v>
+        <v>150</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>68</v>
@@ -8111,7 +7849,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="12">
-        <v>0.25</v>
+        <v>0.35</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -8133,13 +7871,13 @@
         <v>71</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>68</v>
@@ -8148,7 +7886,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="12">
-        <v>0.1</v>
+        <v>0.25</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="12"/>
@@ -8170,13 +7908,13 @@
         <v>71</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>68</v>
@@ -8185,7 +7923,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="12">
-        <v>0.25</v>
+        <v>0.15</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
@@ -8207,13 +7945,13 @@
         <v>71</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>68</v>
@@ -8222,7 +7960,7 @@
         <v>3</v>
       </c>
       <c r="G7" s="12">
-        <v>0.15</v>
+        <v>0.1</v>
       </c>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
@@ -8244,13 +7982,13 @@
         <v>71</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>68</v>
@@ -8281,13 +8019,13 @@
         <v>71</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>103</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>68</v>
@@ -8296,7 +8034,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="12">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="12"/>
@@ -8313,45 +8051,8 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G10" s="12">
-        <v>0.05</v>
-      </c>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="16"/>
-      <c r="L10" s="16"/>
-      <c r="M10" s="12">
-        <v>0</v>
-      </c>
-      <c r="N10" s="12">
-        <v>1</v>
-      </c>
-      <c r="O10" s="12">
-        <v>0.01</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L10">
+  <conditionalFormatting sqref="A2:L9">
     <cfRule type="expression" dxfId="53" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
@@ -8360,7 +8061,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F10" xr:uid="{9D0136A2-A837-4385-ABB0-9D7AA0D4314C}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:F9" xr:uid="{9D0136A2-A837-4385-ABB0-9D7AA0D4314C}">
       <formula1>Validation_Distribution_Types</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
UTR OTD input files
</commit_message>
<xml_diff>
--- a/InputFiles/DefineScenario.xlsx
+++ b/InputFiles/DefineScenario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peraza\Documents\Tasking\(4) EPA Stuff\Task 5 Repo\WideAreaDecon\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEBDF50-20E1-4D9F-B43A-DD28720E6792}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF364F9C-4F3E-4FBB-82D9-D67167E4FBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="649" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="649" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal - File Info" sheetId="1" r:id="rId1"/>
@@ -3889,9 +3889,9 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3912,16 +3912,16 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="67.5546875" customWidth="1"/>
-    <col min="5" max="15" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="67.5703125" customWidth="1"/>
+    <col min="5" max="15" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -3968,7 +3968,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -4005,7 +4005,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -4077,7 +4077,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>71</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>71</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>71</v>
       </c>
@@ -4188,7 +4188,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>71</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>71</v>
       </c>
@@ -4299,16 +4299,16 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="67.5546875" customWidth="1"/>
-    <col min="5" max="15" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="67.5703125" customWidth="1"/>
+    <col min="5" max="15" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -4355,7 +4355,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -4392,7 +4392,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -4427,7 +4427,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -4464,7 +4464,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>71</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>71</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>71</v>
       </c>
@@ -4575,7 +4575,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>71</v>
       </c>
@@ -4612,7 +4612,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>71</v>
       </c>
@@ -4687,14 +4687,14 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
@@ -4736,7 +4736,7 @@
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
@@ -4754,7 +4754,7 @@
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>85</v>
       </c>
@@ -4776,7 +4776,7 @@
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>86</v>
       </c>
@@ -4796,7 +4796,7 @@
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>87</v>
       </c>
@@ -4814,7 +4814,7 @@
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>88</v>
       </c>
@@ -4836,7 +4836,7 @@
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>89</v>
       </c>
@@ -4854,7 +4854,7 @@
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>90</v>
       </c>
@@ -4872,7 +4872,7 @@
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>91</v>
       </c>
@@ -4894,7 +4894,7 @@
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>92</v>
       </c>
@@ -4920,12 +4920,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="20" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="20" t="s">
         <v>99</v>
       </c>
@@ -4945,34 +4945,34 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <f>ROWS($A$10:A10)</f>
         <v>1</v>
@@ -4981,7 +4981,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <f>ROWS($A$10:A11)</f>
         <v>2</v>
@@ -4990,7 +4990,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <f>ROWS($A$10:A12)</f>
         <v>3</v>
@@ -4999,7 +4999,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <f>ROWS($A$10:A13)</f>
         <v>4</v>
@@ -5008,7 +5008,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <f>ROWS($A$10:A14)</f>
         <v>5</v>
@@ -5017,7 +5017,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>6</v>
       </c>
@@ -5025,12 +5025,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
@@ -5038,17 +5038,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2</v>
       </c>
@@ -5056,22 +5056,22 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D27" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
         <v>24</v>
       </c>
@@ -5085,20 +5085,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097870CC-1A0F-461E-BDFD-29BDDFDDF05C}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="45.6640625" customWidth="1"/>
-    <col min="5" max="15" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" customWidth="1"/>
+    <col min="5" max="15" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -5145,7 +5145,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>70</v>
       </c>
@@ -5182,7 +5182,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>70</v>
       </c>
@@ -5219,7 +5219,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -5239,7 +5239,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="12">
-        <v>747.86950000000002</v>
+        <v>0</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -5256,7 +5256,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>71</v>
       </c>
@@ -5272,15 +5272,13 @@
       <c r="E5" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="F5" s="9" t="s">
-        <v>4</v>
+      <c r="F5" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="G5" s="9">
-        <v>3.0319702616531905</v>
-      </c>
-      <c r="H5" s="9">
-        <v>8.0319702616531909</v>
-      </c>
+        <v>-1</v>
+      </c>
+      <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="10"/>
       <c r="K5" s="2"/>
@@ -5296,7 +5294,7 @@
       </c>
       <c r="Q5" s="21"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>72</v>
       </c>
@@ -5316,7 +5314,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="12">
-        <v>0</v>
+        <v>2682.8539999999998</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
@@ -5333,7 +5331,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>72</v>
       </c>
@@ -5350,12 +5348,14 @@
         <v>148</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="12">
-        <v>-1</v>
-      </c>
-      <c r="H7" s="12"/>
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>5.6318533337268804</v>
+      </c>
+      <c r="H7" s="12">
+        <v>6.1323408067707499</v>
+      </c>
       <c r="I7" s="12"/>
       <c r="J7" s="13"/>
       <c r="K7" s="16"/>
@@ -5370,7 +5370,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>71</v>
       </c>
@@ -5390,7 +5390,7 @@
         <v>3</v>
       </c>
       <c r="G8" s="9">
-        <v>0.33333333333333331</v>
+        <v>0</v>
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
@@ -5407,7 +5407,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>71</v>
       </c>
@@ -5427,7 +5427,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="9">
-        <v>0.55555555555555558</v>
+        <v>0</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -5444,7 +5444,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>71</v>
       </c>
@@ -5464,7 +5464,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="9">
-        <v>0.1111111111111111</v>
+        <v>0</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -5481,7 +5481,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>71</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>71</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>71</v>
       </c>
@@ -5592,7 +5592,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>71</v>
       </c>
@@ -5629,7 +5629,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>70</v>
       </c>
@@ -5666,7 +5666,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>70</v>
       </c>
@@ -5703,7 +5703,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>70</v>
       </c>
@@ -5740,7 +5740,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>70</v>
       </c>
@@ -5777,7 +5777,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>70</v>
       </c>
@@ -5814,7 +5814,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>70</v>
       </c>
@@ -5851,7 +5851,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>72</v>
       </c>
@@ -5871,7 +5871,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
@@ -5888,7 +5888,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>72</v>
       </c>
@@ -5908,7 +5908,7 @@
         <v>3</v>
       </c>
       <c r="G22" s="12">
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
@@ -5925,7 +5925,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>72</v>
       </c>
@@ -5962,7 +5962,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>72</v>
       </c>
@@ -5982,7 +5982,7 @@
         <v>3</v>
       </c>
       <c r="G24" s="12">
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
@@ -5999,7 +5999,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>72</v>
       </c>
@@ -6019,7 +6019,7 @@
         <v>3</v>
       </c>
       <c r="G25" s="12">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
@@ -6036,7 +6036,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>72</v>
       </c>
@@ -6073,7 +6073,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>71</v>
       </c>
@@ -6093,7 +6093,7 @@
         <v>3</v>
       </c>
       <c r="G27" s="12">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
@@ -6110,7 +6110,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>71</v>
       </c>
@@ -6130,7 +6130,7 @@
         <v>3</v>
       </c>
       <c r="G28" s="12">
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
@@ -6147,7 +6147,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>71</v>
       </c>
@@ -6167,7 +6167,7 @@
         <v>3</v>
       </c>
       <c r="G29" s="12">
-        <v>6.25E-2</v>
+        <v>0</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
@@ -6184,7 +6184,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>71</v>
       </c>
@@ -6204,7 +6204,7 @@
         <v>3</v>
       </c>
       <c r="G30" s="12">
-        <v>6.25E-2</v>
+        <v>0</v>
       </c>
       <c r="H30" s="12"/>
       <c r="I30" s="12"/>
@@ -6221,7 +6221,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>71</v>
       </c>
@@ -6241,7 +6241,7 @@
         <v>3</v>
       </c>
       <c r="G31" s="12">
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
@@ -6258,7 +6258,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>71</v>
       </c>
@@ -6278,7 +6278,7 @@
         <v>3</v>
       </c>
       <c r="G32" s="12">
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="H32" s="12"/>
       <c r="I32" s="12"/>
@@ -6297,7 +6297,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A2:L32">
+  <conditionalFormatting sqref="A2:L6 A8:L32 A7:F7 H7:L7">
     <cfRule type="expression" dxfId="155" priority="43">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
@@ -6325,16 +6325,16 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="67.5546875" customWidth="1"/>
-    <col min="5" max="15" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="67.5703125" customWidth="1"/>
+    <col min="5" max="15" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -6381,7 +6381,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -6418,7 +6418,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -6453,7 +6453,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -6490,7 +6490,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>71</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>71</v>
       </c>
@@ -6564,7 +6564,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>71</v>
       </c>
@@ -6601,7 +6601,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>71</v>
       </c>
@@ -6638,7 +6638,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>71</v>
       </c>
@@ -6704,16 +6704,16 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="67.5546875" customWidth="1"/>
-    <col min="5" max="15" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="67.5703125" customWidth="1"/>
+    <col min="5" max="15" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -6760,7 +6760,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -6797,7 +6797,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -6832,7 +6832,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -6869,7 +6869,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>71</v>
       </c>
@@ -6906,7 +6906,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>71</v>
       </c>
@@ -6943,7 +6943,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>71</v>
       </c>
@@ -6980,7 +6980,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>71</v>
       </c>
@@ -7017,7 +7017,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>71</v>
       </c>
@@ -7091,16 +7091,16 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="67.5546875" customWidth="1"/>
-    <col min="5" max="15" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="67.5703125" customWidth="1"/>
+    <col min="5" max="15" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -7147,7 +7147,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -7184,7 +7184,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -7219,7 +7219,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -7256,7 +7256,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>71</v>
       </c>
@@ -7293,7 +7293,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>71</v>
       </c>
@@ -7330,7 +7330,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>71</v>
       </c>
@@ -7367,7 +7367,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>71</v>
       </c>
@@ -7404,7 +7404,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>71</v>
       </c>
@@ -7478,16 +7478,16 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="67.5546875" customWidth="1"/>
-    <col min="5" max="15" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="67.5703125" customWidth="1"/>
+    <col min="5" max="15" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -7534,7 +7534,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -7571,7 +7571,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -7606,7 +7606,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -7643,7 +7643,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>71</v>
       </c>
@@ -7680,7 +7680,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>71</v>
       </c>
@@ -7717,7 +7717,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>71</v>
       </c>
@@ -7754,7 +7754,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>71</v>
       </c>
@@ -7791,7 +7791,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>71</v>
       </c>
@@ -7865,16 +7865,16 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" customWidth="1"/>
-    <col min="2" max="2" width="22.5546875" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1"/>
-    <col min="4" max="4" width="67.5546875" customWidth="1"/>
-    <col min="5" max="15" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1"/>
+    <col min="4" max="4" width="67.5703125" customWidth="1"/>
+    <col min="5" max="15" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -7921,7 +7921,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -7958,7 +7958,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -7993,7 +7993,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -8030,7 +8030,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>71</v>
       </c>
@@ -8067,7 +8067,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>71</v>
       </c>
@@ -8104,7 +8104,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>71</v>
       </c>
@@ -8141,7 +8141,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>71</v>
       </c>
@@ -8178,7 +8178,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>71</v>
       </c>

</xml_diff>

<commit_message>
Updated UTR OTD input files
</commit_message>
<xml_diff>
--- a/InputFiles/DefineScenario.xlsx
+++ b/InputFiles/DefineScenario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peraza\Documents\Tasking\(4) EPA Stuff\Task 5 Repo\WideAreaDecon\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peraza\Box\TO 19F0117 Framework for Sampling\Task 5\Deliverables\(14) Verification Cases\BOTE Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF364F9C-4F3E-4FBB-82D9-D67167E4FBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DCC5AD-F1BD-4628-9535-E630E15D3625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="649" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="649" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal - File Info" sheetId="1" r:id="rId1"/>
@@ -3889,9 +3889,9 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3912,16 +3912,16 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="67.5703125" customWidth="1"/>
-    <col min="5" max="15" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="67.5546875" customWidth="1"/>
+    <col min="5" max="15" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -3968,7 +3968,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -4005,7 +4005,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -4077,7 +4077,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>71</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>71</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>71</v>
       </c>
@@ -4188,7 +4188,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>71</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>71</v>
       </c>
@@ -4299,16 +4299,16 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="67.5703125" customWidth="1"/>
-    <col min="5" max="15" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="67.5546875" customWidth="1"/>
+    <col min="5" max="15" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -4355,7 +4355,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -4392,7 +4392,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -4427,7 +4427,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -4464,7 +4464,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>71</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>71</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>71</v>
       </c>
@@ -4575,7 +4575,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>71</v>
       </c>
@@ -4612,7 +4612,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>71</v>
       </c>
@@ -4687,14 +4687,14 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
@@ -4736,7 +4736,7 @@
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
@@ -4754,7 +4754,7 @@
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>85</v>
       </c>
@@ -4776,7 +4776,7 @@
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>86</v>
       </c>
@@ -4796,7 +4796,7 @@
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>87</v>
       </c>
@@ -4814,7 +4814,7 @@
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>88</v>
       </c>
@@ -4836,7 +4836,7 @@
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>89</v>
       </c>
@@ -4854,7 +4854,7 @@
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>90</v>
       </c>
@@ -4872,7 +4872,7 @@
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>91</v>
       </c>
@@ -4894,7 +4894,7 @@
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>92</v>
       </c>
@@ -4920,12 +4920,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>99</v>
       </c>
@@ -4945,34 +4945,34 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <f>ROWS($A$10:A10)</f>
         <v>1</v>
@@ -4981,7 +4981,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>ROWS($A$10:A11)</f>
         <v>2</v>
@@ -4990,7 +4990,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>ROWS($A$10:A12)</f>
         <v>3</v>
@@ -4999,7 +4999,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <f>ROWS($A$10:A13)</f>
         <v>4</v>
@@ -5008,7 +5008,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <f>ROWS($A$10:A14)</f>
         <v>5</v>
@@ -5017,7 +5017,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>6</v>
       </c>
@@ -5025,12 +5025,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -5038,17 +5038,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2</v>
       </c>
@@ -5056,22 +5056,22 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E29" t="s">
         <v>24</v>
       </c>
@@ -5086,19 +5086,19 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="45.7109375" customWidth="1"/>
-    <col min="5" max="15" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="45.6640625" customWidth="1"/>
+    <col min="5" max="15" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -5145,7 +5145,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>70</v>
       </c>
@@ -5182,7 +5182,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>70</v>
       </c>
@@ -5219,7 +5219,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -5239,7 +5239,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="12">
-        <v>0</v>
+        <v>747.86950000000002</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -5256,7 +5256,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>71</v>
       </c>
@@ -5272,13 +5272,15 @@
       <c r="E5" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>3</v>
+      <c r="F5" s="9" t="s">
+        <v>4</v>
       </c>
       <c r="G5" s="9">
-        <v>-1</v>
-      </c>
-      <c r="H5" s="9"/>
+        <v>3.0319702616531905</v>
+      </c>
+      <c r="H5" s="9">
+        <v>8.0319702616531909</v>
+      </c>
       <c r="I5" s="9"/>
       <c r="J5" s="10"/>
       <c r="K5" s="2"/>
@@ -5294,7 +5296,7 @@
       </c>
       <c r="Q5" s="21"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>72</v>
       </c>
@@ -5314,7 +5316,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="12">
-        <v>2682.8539999999998</v>
+        <v>0</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
@@ -5331,7 +5333,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>72</v>
       </c>
@@ -5348,14 +5350,12 @@
         <v>148</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7">
-        <v>5.6318533337268804</v>
-      </c>
-      <c r="H7" s="12">
-        <v>6.1323408067707499</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="G7" s="12">
+        <v>-1</v>
+      </c>
+      <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="13"/>
       <c r="K7" s="16"/>
@@ -5370,7 +5370,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>71</v>
       </c>
@@ -5407,7 +5407,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>71</v>
       </c>
@@ -5427,7 +5427,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -5444,7 +5444,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>71</v>
       </c>
@@ -5481,7 +5481,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>71</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>71</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>71</v>
       </c>
@@ -5592,7 +5592,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>71</v>
       </c>
@@ -5629,7 +5629,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>70</v>
       </c>
@@ -5666,7 +5666,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>70</v>
       </c>
@@ -5703,7 +5703,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>70</v>
       </c>
@@ -5740,7 +5740,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>70</v>
       </c>
@@ -5777,7 +5777,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>70</v>
       </c>
@@ -5814,7 +5814,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>70</v>
       </c>
@@ -5851,7 +5851,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>72</v>
       </c>
@@ -5871,7 +5871,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="12">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
@@ -5888,7 +5888,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>72</v>
       </c>
@@ -5908,7 +5908,7 @@
         <v>3</v>
       </c>
       <c r="G22" s="12">
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
@@ -5925,7 +5925,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>72</v>
       </c>
@@ -5962,7 +5962,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>72</v>
       </c>
@@ -5982,7 +5982,7 @@
         <v>3</v>
       </c>
       <c r="G24" s="12">
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
@@ -5999,7 +5999,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>72</v>
       </c>
@@ -6019,7 +6019,7 @@
         <v>3</v>
       </c>
       <c r="G25" s="12">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
@@ -6036,7 +6036,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>72</v>
       </c>
@@ -6073,7 +6073,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>71</v>
       </c>
@@ -6093,7 +6093,7 @@
         <v>3</v>
       </c>
       <c r="G27" s="12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
@@ -6110,7 +6110,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>71</v>
       </c>
@@ -6130,7 +6130,7 @@
         <v>3</v>
       </c>
       <c r="G28" s="12">
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
@@ -6147,7 +6147,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>71</v>
       </c>
@@ -6167,7 +6167,7 @@
         <v>3</v>
       </c>
       <c r="G29" s="12">
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
@@ -6184,7 +6184,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>71</v>
       </c>
@@ -6204,7 +6204,7 @@
         <v>3</v>
       </c>
       <c r="G30" s="12">
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H30" s="12"/>
       <c r="I30" s="12"/>
@@ -6221,7 +6221,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>71</v>
       </c>
@@ -6241,7 +6241,7 @@
         <v>3</v>
       </c>
       <c r="G31" s="12">
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
@@ -6258,7 +6258,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>71</v>
       </c>
@@ -6278,7 +6278,7 @@
         <v>3</v>
       </c>
       <c r="G32" s="12">
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="H32" s="12"/>
       <c r="I32" s="12"/>
@@ -6297,7 +6297,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A2:L6 A8:L32 A7:F7 H7:L7">
+  <conditionalFormatting sqref="A2:L32">
     <cfRule type="expression" dxfId="155" priority="43">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
@@ -6325,16 +6325,16 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="67.5703125" customWidth="1"/>
-    <col min="5" max="15" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="67.5546875" customWidth="1"/>
+    <col min="5" max="15" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -6381,7 +6381,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -6418,7 +6418,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -6453,7 +6453,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -6490,7 +6490,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>71</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>71</v>
       </c>
@@ -6564,7 +6564,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>71</v>
       </c>
@@ -6601,7 +6601,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>71</v>
       </c>
@@ -6638,7 +6638,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>71</v>
       </c>
@@ -6704,16 +6704,16 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="67.5703125" customWidth="1"/>
-    <col min="5" max="15" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="67.5546875" customWidth="1"/>
+    <col min="5" max="15" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -6760,7 +6760,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -6797,7 +6797,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -6832,7 +6832,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -6869,7 +6869,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>71</v>
       </c>
@@ -6906,7 +6906,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>71</v>
       </c>
@@ -6943,7 +6943,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>71</v>
       </c>
@@ -6980,7 +6980,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>71</v>
       </c>
@@ -7017,7 +7017,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>71</v>
       </c>
@@ -7091,16 +7091,16 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="67.5703125" customWidth="1"/>
-    <col min="5" max="15" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="67.5546875" customWidth="1"/>
+    <col min="5" max="15" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -7147,7 +7147,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -7184,7 +7184,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -7219,7 +7219,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -7256,7 +7256,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>71</v>
       </c>
@@ -7293,7 +7293,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>71</v>
       </c>
@@ -7330,7 +7330,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>71</v>
       </c>
@@ -7367,7 +7367,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>71</v>
       </c>
@@ -7404,7 +7404,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>71</v>
       </c>
@@ -7478,16 +7478,16 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="67.5703125" customWidth="1"/>
-    <col min="5" max="15" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="67.5546875" customWidth="1"/>
+    <col min="5" max="15" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -7534,7 +7534,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -7571,7 +7571,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -7606,7 +7606,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -7643,7 +7643,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>71</v>
       </c>
@@ -7680,7 +7680,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>71</v>
       </c>
@@ -7717,7 +7717,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>71</v>
       </c>
@@ -7754,7 +7754,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>71</v>
       </c>
@@ -7791,7 +7791,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>71</v>
       </c>
@@ -7865,16 +7865,16 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="67.5703125" customWidth="1"/>
-    <col min="5" max="15" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="67.5546875" customWidth="1"/>
+    <col min="5" max="15" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -7921,7 +7921,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -7958,7 +7958,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -7993,7 +7993,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -8030,7 +8030,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>71</v>
       </c>
@@ -8067,7 +8067,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>71</v>
       </c>
@@ -8104,7 +8104,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>71</v>
       </c>
@@ -8141,7 +8141,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>71</v>
       </c>
@@ -8178,7 +8178,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>71</v>
       </c>

</xml_diff>

<commit_message>
Updated BOTE input files
</commit_message>
<xml_diff>
--- a/InputFiles/DefineScenario.xlsx
+++ b/InputFiles/DefineScenario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peraza\Documents\Tasking\(4) EPA Stuff\Task 5 Repo\WideAreaDecon\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peraza\Box\TO 19F0117 Framework for Sampling\Task 5\Deliverables\(14) Verification Cases\BOTE Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF364F9C-4F3E-4FBB-82D9-D67167E4FBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DCC5AD-F1BD-4628-9535-E630E15D3625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="649" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="649" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal - File Info" sheetId="1" r:id="rId1"/>
@@ -3889,9 +3889,9 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3912,16 +3912,16 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="67.5703125" customWidth="1"/>
-    <col min="5" max="15" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="67.5546875" customWidth="1"/>
+    <col min="5" max="15" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -3968,7 +3968,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -4005,7 +4005,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -4077,7 +4077,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>71</v>
       </c>
@@ -4114,7 +4114,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>71</v>
       </c>
@@ -4151,7 +4151,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>71</v>
       </c>
@@ -4188,7 +4188,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>71</v>
       </c>
@@ -4225,7 +4225,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>71</v>
       </c>
@@ -4299,16 +4299,16 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="67.5703125" customWidth="1"/>
-    <col min="5" max="15" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="67.5546875" customWidth="1"/>
+    <col min="5" max="15" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -4355,7 +4355,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -4392,7 +4392,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -4427,7 +4427,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -4464,7 +4464,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>71</v>
       </c>
@@ -4501,7 +4501,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>71</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>71</v>
       </c>
@@ -4575,7 +4575,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>71</v>
       </c>
@@ -4612,7 +4612,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>71</v>
       </c>
@@ -4687,14 +4687,14 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="8" width="17.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
@@ -4720,7 +4720,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
@@ -4736,7 +4736,7 @@
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>4</v>
       </c>
@@ -4754,7 +4754,7 @@
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>85</v>
       </c>
@@ -4776,7 +4776,7 @@
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>86</v>
       </c>
@@ -4796,7 +4796,7 @@
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>87</v>
       </c>
@@ -4814,7 +4814,7 @@
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
         <v>88</v>
       </c>
@@ -4836,7 +4836,7 @@
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
         <v>89</v>
       </c>
@@ -4854,7 +4854,7 @@
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
         <v>90</v>
       </c>
@@ -4872,7 +4872,7 @@
       <c r="G9" s="15"/>
       <c r="H9" s="15"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
         <v>91</v>
       </c>
@@ -4894,7 +4894,7 @@
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
         <v>92</v>
       </c>
@@ -4920,12 +4920,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
         <v>99</v>
       </c>
@@ -4945,34 +4945,34 @@
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <f>ROWS($A$10:A10)</f>
         <v>1</v>
@@ -4981,7 +4981,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>ROWS($A$10:A11)</f>
         <v>2</v>
@@ -4990,7 +4990,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>ROWS($A$10:A12)</f>
         <v>3</v>
@@ -4999,7 +4999,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
         <f>ROWS($A$10:A13)</f>
         <v>4</v>
@@ -5008,7 +5008,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
         <f>ROWS($A$10:A14)</f>
         <v>5</v>
@@ -5017,7 +5017,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>6</v>
       </c>
@@ -5025,12 +5025,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
@@ -5038,17 +5038,17 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>2</v>
       </c>
@@ -5056,22 +5056,22 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="C26" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D27" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="D28" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="E29" t="s">
         <v>24</v>
       </c>
@@ -5086,19 +5086,19 @@
   <dimension ref="A1:Q32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="28.140625" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="45.7109375" customWidth="1"/>
-    <col min="5" max="15" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="28.109375" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="45.6640625" customWidth="1"/>
+    <col min="5" max="15" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -5145,7 +5145,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>70</v>
       </c>
@@ -5182,7 +5182,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>70</v>
       </c>
@@ -5219,7 +5219,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -5239,7 +5239,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="12">
-        <v>0</v>
+        <v>747.86950000000002</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -5256,7 +5256,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>71</v>
       </c>
@@ -5272,13 +5272,15 @@
       <c r="E5" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>3</v>
+      <c r="F5" s="9" t="s">
+        <v>4</v>
       </c>
       <c r="G5" s="9">
-        <v>-1</v>
-      </c>
-      <c r="H5" s="9"/>
+        <v>3.0319702616531905</v>
+      </c>
+      <c r="H5" s="9">
+        <v>8.0319702616531909</v>
+      </c>
       <c r="I5" s="9"/>
       <c r="J5" s="10"/>
       <c r="K5" s="2"/>
@@ -5294,7 +5296,7 @@
       </c>
       <c r="Q5" s="21"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>72</v>
       </c>
@@ -5314,7 +5316,7 @@
         <v>3</v>
       </c>
       <c r="G6" s="12">
-        <v>2682.8539999999998</v>
+        <v>0</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
@@ -5331,7 +5333,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>72</v>
       </c>
@@ -5348,14 +5350,12 @@
         <v>148</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7">
-        <v>5.6318533337268804</v>
-      </c>
-      <c r="H7" s="12">
-        <v>6.1323408067707499</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="G7" s="12">
+        <v>-1</v>
+      </c>
+      <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="13"/>
       <c r="K7" s="16"/>
@@ -5370,7 +5370,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>71</v>
       </c>
@@ -5407,7 +5407,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>71</v>
       </c>
@@ -5427,7 +5427,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -5444,7 +5444,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>71</v>
       </c>
@@ -5481,7 +5481,7 @@
         <v>1.0000000000000001E-9</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>71</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>71</v>
       </c>
@@ -5555,7 +5555,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>71</v>
       </c>
@@ -5592,7 +5592,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>71</v>
       </c>
@@ -5629,7 +5629,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>70</v>
       </c>
@@ -5666,7 +5666,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>70</v>
       </c>
@@ -5703,7 +5703,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>70</v>
       </c>
@@ -5740,7 +5740,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>70</v>
       </c>
@@ -5777,7 +5777,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>70</v>
       </c>
@@ -5814,7 +5814,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>70</v>
       </c>
@@ -5851,7 +5851,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>72</v>
       </c>
@@ -5871,7 +5871,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="12">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
@@ -5888,7 +5888,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>72</v>
       </c>
@@ -5908,7 +5908,7 @@
         <v>3</v>
       </c>
       <c r="G22" s="12">
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
@@ -5925,7 +5925,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>72</v>
       </c>
@@ -5962,7 +5962,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>72</v>
       </c>
@@ -5982,7 +5982,7 @@
         <v>3</v>
       </c>
       <c r="G24" s="12">
-        <v>0.125</v>
+        <v>0</v>
       </c>
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
@@ -5999,7 +5999,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>72</v>
       </c>
@@ -6019,7 +6019,7 @@
         <v>3</v>
       </c>
       <c r="G25" s="12">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
@@ -6036,7 +6036,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>72</v>
       </c>
@@ -6073,7 +6073,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>71</v>
       </c>
@@ -6093,7 +6093,7 @@
         <v>3</v>
       </c>
       <c r="G27" s="12">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
@@ -6110,7 +6110,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>71</v>
       </c>
@@ -6130,7 +6130,7 @@
         <v>3</v>
       </c>
       <c r="G28" s="12">
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
@@ -6147,7 +6147,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>71</v>
       </c>
@@ -6167,7 +6167,7 @@
         <v>3</v>
       </c>
       <c r="G29" s="12">
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
@@ -6184,7 +6184,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>71</v>
       </c>
@@ -6204,7 +6204,7 @@
         <v>3</v>
       </c>
       <c r="G30" s="12">
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="H30" s="12"/>
       <c r="I30" s="12"/>
@@ -6221,7 +6221,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>71</v>
       </c>
@@ -6241,7 +6241,7 @@
         <v>3</v>
       </c>
       <c r="G31" s="12">
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
@@ -6258,7 +6258,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>71</v>
       </c>
@@ -6278,7 +6278,7 @@
         <v>3</v>
       </c>
       <c r="G32" s="12">
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="H32" s="12"/>
       <c r="I32" s="12"/>
@@ -6297,7 +6297,7 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="A2:L6 A8:L32 A7:F7 H7:L7">
+  <conditionalFormatting sqref="A2:L32">
     <cfRule type="expression" dxfId="155" priority="43">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
@@ -6325,16 +6325,16 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="67.5703125" customWidth="1"/>
-    <col min="5" max="15" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="67.5546875" customWidth="1"/>
+    <col min="5" max="15" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -6381,7 +6381,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -6418,7 +6418,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -6453,7 +6453,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -6490,7 +6490,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>71</v>
       </c>
@@ -6527,7 +6527,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>71</v>
       </c>
@@ -6564,7 +6564,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>71</v>
       </c>
@@ -6601,7 +6601,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>71</v>
       </c>
@@ -6638,7 +6638,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>71</v>
       </c>
@@ -6704,16 +6704,16 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="67.5703125" customWidth="1"/>
-    <col min="5" max="15" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="67.5546875" customWidth="1"/>
+    <col min="5" max="15" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -6760,7 +6760,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -6797,7 +6797,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -6832,7 +6832,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -6869,7 +6869,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>71</v>
       </c>
@@ -6906,7 +6906,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>71</v>
       </c>
@@ -6943,7 +6943,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>71</v>
       </c>
@@ -6980,7 +6980,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>71</v>
       </c>
@@ -7017,7 +7017,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>71</v>
       </c>
@@ -7091,16 +7091,16 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="67.5703125" customWidth="1"/>
-    <col min="5" max="15" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="67.5546875" customWidth="1"/>
+    <col min="5" max="15" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -7147,7 +7147,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -7184,7 +7184,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -7219,7 +7219,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -7256,7 +7256,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>71</v>
       </c>
@@ -7293,7 +7293,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>71</v>
       </c>
@@ -7330,7 +7330,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>71</v>
       </c>
@@ -7367,7 +7367,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>71</v>
       </c>
@@ -7404,7 +7404,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>71</v>
       </c>
@@ -7478,16 +7478,16 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="67.5703125" customWidth="1"/>
-    <col min="5" max="15" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="67.5546875" customWidth="1"/>
+    <col min="5" max="15" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -7534,7 +7534,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -7571,7 +7571,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -7606,7 +7606,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -7643,7 +7643,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>71</v>
       </c>
@@ -7680,7 +7680,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>71</v>
       </c>
@@ -7717,7 +7717,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>71</v>
       </c>
@@ -7754,7 +7754,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>71</v>
       </c>
@@ -7791,7 +7791,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>71</v>
       </c>
@@ -7865,16 +7865,16 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="67.5703125" customWidth="1"/>
-    <col min="5" max="15" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5546875" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="67.5546875" customWidth="1"/>
+    <col min="5" max="15" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -7921,7 +7921,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>71</v>
       </c>
@@ -7958,7 +7958,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>71</v>
       </c>
@@ -7993,7 +7993,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -8030,7 +8030,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>71</v>
       </c>
@@ -8067,7 +8067,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>71</v>
       </c>
@@ -8104,7 +8104,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>71</v>
       </c>
@@ -8141,7 +8141,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>71</v>
       </c>
@@ -8178,7 +8178,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>71</v>
       </c>

</xml_diff>

<commit_message>
Added in baseline parameters datasheets
</commit_message>
<xml_diff>
--- a/InputFiles/DefineScenario.xlsx
+++ b/InputFiles/DefineScenario.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peraza\Box\TO 19F0117 Framework for Sampling\Task 5\Deliverables\(14) Verification Cases\BOTE Input Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peraza\Box\TO 19F0117 Framework for Sampling\Task 5\Deliverables\(14) Verification Cases\Original Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DCC5AD-F1BD-4628-9535-E630E15D3625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FA6B07-C637-45B8-8105-43B8BC7F00AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="649" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="649" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal - File Info" sheetId="1" r:id="rId1"/>
@@ -391,6 +391,9 @@
     <t>Fraction of residential buildings that are miscellaneous</t>
   </si>
   <si>
+    <t>log(PFU / m^2)</t>
+  </si>
+  <si>
     <t>Outdoor Surface Type Breakout</t>
   </si>
   <si>
@@ -497,9 +500,6 @@
   </si>
   <si>
     <t>Underground Walls</t>
-  </si>
-  <si>
-    <t>log(CFU / m^2)</t>
   </si>
   <si>
     <t>Underground HVAC</t>
@@ -747,7 +747,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -769,13 +769,12 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="156">
+  <dxfs count="144">
     <dxf>
       <border>
         <left style="thin">
@@ -1089,6 +1088,300 @@
       </fill>
     </dxf>
     <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <i/>
         <strike/>
@@ -1419,6 +1712,300 @@
       </fill>
     </dxf>
     <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="medium">
+          <color rgb="FF000000"/>
+        </left>
+        <right style="medium">
+          <color rgb="FF000000"/>
+        </right>
+        <top style="medium">
+          <color rgb="FF000000"/>
+        </top>
+        <bottom style="medium">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <i/>
         <strike/>
@@ -1749,24 +2336,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <i/>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color indexed="64"/>
@@ -2059,684 +2628,6 @@
           <color rgb="FF000000"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="medium">
-          <color rgb="FF000000"/>
-        </left>
-        <right style="medium">
-          <color rgb="FF000000"/>
-        </right>
-        <top style="medium">
-          <color rgb="FF000000"/>
-        </top>
-        <bottom style="medium">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <i/>
-        <strike/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -3394,168 +3285,168 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{77E3C927-1FC6-443B-87ED-00E2959DD317}" name="Table1568" displayName="Table1568" ref="A1:O32" totalsRowShown="0" tableBorderDxfId="153">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{77E3C927-1FC6-443B-87ED-00E2959DD317}" name="Table1568" displayName="Table1568" ref="A1:O32" totalsRowShown="0" tableBorderDxfId="141">
   <autoFilter ref="A1:O32" xr:uid="{58F00973-C0E2-47D9-9C5E-C7B7F684A0C3}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{62A6D655-D638-4005-9525-C140421ED9AB}" name="Phase" dataDxfId="152"/>
-    <tableColumn id="1" xr3:uid="{1BC04ADD-0426-4785-9F97-FCE0BCC1E547}" name="Category" dataDxfId="151"/>
-    <tableColumn id="2" xr3:uid="{3089FC2E-257C-4BA5-A9A7-5D0E01D5E6F5}" name="Name" dataDxfId="150"/>
-    <tableColumn id="10" xr3:uid="{E1A27E6E-82E5-4CF6-9164-A680FF7F05A5}" name="Description" dataDxfId="149"/>
-    <tableColumn id="3" xr3:uid="{BA85C23F-8236-43E3-885F-DF8CCDB84F06}" name="Units" dataDxfId="148"/>
-    <tableColumn id="4" xr3:uid="{9121EDDE-A8D8-4E28-AAAC-953CC1A14CB2}" name="Distribution Type" dataDxfId="147"/>
-    <tableColumn id="5" xr3:uid="{67D6DF1C-45B3-456F-B960-B8F495F6867D}" name="Parameter 1" dataDxfId="146"/>
-    <tableColumn id="6" xr3:uid="{A2BB8730-6626-47D8-AABB-90C19B218AFB}" name="Parameter 2" dataDxfId="145"/>
-    <tableColumn id="7" xr3:uid="{B7BC4EB1-7616-4A3A-899A-F01A87DD3B48}" name="Parameter 3" dataDxfId="144"/>
-    <tableColumn id="8" xr3:uid="{32D71C9B-2B39-4A83-9EB0-1934F2F6FC91}" name="Parameter 4" dataDxfId="143"/>
-    <tableColumn id="14" xr3:uid="{31AC778C-1A4A-45DD-8A12-F22858D3CD3A}" name="Parameter 5" dataDxfId="142"/>
-    <tableColumn id="15" xr3:uid="{91C3BDC4-4893-4CF7-9830-76CC4A9BF6F1}" name="Parameter 6" dataDxfId="141"/>
-    <tableColumn id="11" xr3:uid="{6BCEB05C-9FCE-48DE-91F0-D2ACC21C6C3E}" name="Lower Limit" dataDxfId="140"/>
-    <tableColumn id="12" xr3:uid="{CDC89704-43FE-407F-B8B4-079E5E991263}" name="Upper Limit" dataDxfId="139"/>
-    <tableColumn id="13" xr3:uid="{0758CB79-3F38-44D8-B78B-CC33BB1D2C70}" name="Step" dataDxfId="138"/>
+    <tableColumn id="9" xr3:uid="{62A6D655-D638-4005-9525-C140421ED9AB}" name="Phase" dataDxfId="140"/>
+    <tableColumn id="1" xr3:uid="{1BC04ADD-0426-4785-9F97-FCE0BCC1E547}" name="Category" dataDxfId="139"/>
+    <tableColumn id="2" xr3:uid="{3089FC2E-257C-4BA5-A9A7-5D0E01D5E6F5}" name="Name" dataDxfId="138"/>
+    <tableColumn id="10" xr3:uid="{E1A27E6E-82E5-4CF6-9164-A680FF7F05A5}" name="Description" dataDxfId="137"/>
+    <tableColumn id="3" xr3:uid="{BA85C23F-8236-43E3-885F-DF8CCDB84F06}" name="Units" dataDxfId="136"/>
+    <tableColumn id="4" xr3:uid="{9121EDDE-A8D8-4E28-AAAC-953CC1A14CB2}" name="Distribution Type" dataDxfId="135"/>
+    <tableColumn id="5" xr3:uid="{67D6DF1C-45B3-456F-B960-B8F495F6867D}" name="Parameter 1" dataDxfId="134"/>
+    <tableColumn id="6" xr3:uid="{A2BB8730-6626-47D8-AABB-90C19B218AFB}" name="Parameter 2" dataDxfId="133"/>
+    <tableColumn id="7" xr3:uid="{B7BC4EB1-7616-4A3A-899A-F01A87DD3B48}" name="Parameter 3" dataDxfId="132"/>
+    <tableColumn id="8" xr3:uid="{32D71C9B-2B39-4A83-9EB0-1934F2F6FC91}" name="Parameter 4" dataDxfId="131"/>
+    <tableColumn id="14" xr3:uid="{31AC778C-1A4A-45DD-8A12-F22858D3CD3A}" name="Parameter 5" dataDxfId="130"/>
+    <tableColumn id="15" xr3:uid="{91C3BDC4-4893-4CF7-9830-76CC4A9BF6F1}" name="Parameter 6" dataDxfId="129"/>
+    <tableColumn id="11" xr3:uid="{6BCEB05C-9FCE-48DE-91F0-D2ACC21C6C3E}" name="Lower Limit" dataDxfId="128"/>
+    <tableColumn id="12" xr3:uid="{CDC89704-43FE-407F-B8B4-079E5E991263}" name="Upper Limit" dataDxfId="127"/>
+    <tableColumn id="13" xr3:uid="{0758CB79-3F38-44D8-B78B-CC33BB1D2C70}" name="Step" dataDxfId="126"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{72F3CA1E-AAFF-44BC-A114-2AA862291D9E}" name="Table1568102" displayName="Table1568102" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="135">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{72F3CA1E-AAFF-44BC-A114-2AA862291D9E}" name="Table1568102" displayName="Table1568102" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="123">
   <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{8FD38CEB-1D1A-41E8-821F-58DD4FBD85EB}" name="Phase" dataDxfId="134"/>
-    <tableColumn id="1" xr3:uid="{574AE483-6154-4EC6-AC18-5FDEBC0931CD}" name="Category" dataDxfId="133"/>
-    <tableColumn id="2" xr3:uid="{EC332146-FEF7-42A1-9698-0FB7656BE557}" name="Name" dataDxfId="132"/>
-    <tableColumn id="10" xr3:uid="{F0942CE2-9658-4EB8-A19F-B3B76B6A5F95}" name="Description" dataDxfId="131"/>
-    <tableColumn id="3" xr3:uid="{B909ADC8-9FD8-4714-A691-8AD0F1933057}" name="Units" dataDxfId="130"/>
-    <tableColumn id="4" xr3:uid="{F8B8B123-0CBC-450A-B098-9FFA08F7FC89}" name="Distribution Type" dataDxfId="129"/>
-    <tableColumn id="5" xr3:uid="{AADB8566-896F-40D4-8181-BB145E678F9B}" name="Parameter 1" dataDxfId="128"/>
-    <tableColumn id="6" xr3:uid="{13B0114C-55D3-4603-92C6-09319B7E315B}" name="Parameter 2" dataDxfId="127"/>
-    <tableColumn id="7" xr3:uid="{7548BB98-B29E-4F39-B198-D6F9994CC04D}" name="Parameter 3" dataDxfId="126"/>
-    <tableColumn id="8" xr3:uid="{355D4B98-B5B0-461B-90E8-3D81112B89E2}" name="Parameter 4" dataDxfId="125"/>
-    <tableColumn id="14" xr3:uid="{14667F24-6EC2-4F8F-8EAA-56B4FF372D98}" name="Parameter 5" dataDxfId="124"/>
-    <tableColumn id="15" xr3:uid="{B058DB6A-9C46-4ED3-9483-5713AD52AE40}" name="Parameter 6" dataDxfId="123"/>
-    <tableColumn id="11" xr3:uid="{0E22E7A3-8506-41E8-AC60-E103665C60A2}" name="Lower Limit" dataDxfId="122"/>
-    <tableColumn id="12" xr3:uid="{479761C6-7DBC-4557-9E7C-984A37ABCB8A}" name="Upper Limit" dataDxfId="121"/>
-    <tableColumn id="13" xr3:uid="{F96695B6-2ADD-458A-A424-B58482082C80}" name="Step" dataDxfId="120"/>
+    <tableColumn id="9" xr3:uid="{8FD38CEB-1D1A-41E8-821F-58DD4FBD85EB}" name="Phase" dataDxfId="122"/>
+    <tableColumn id="1" xr3:uid="{574AE483-6154-4EC6-AC18-5FDEBC0931CD}" name="Category" dataDxfId="121"/>
+    <tableColumn id="2" xr3:uid="{EC332146-FEF7-42A1-9698-0FB7656BE557}" name="Name" dataDxfId="120"/>
+    <tableColumn id="10" xr3:uid="{F0942CE2-9658-4EB8-A19F-B3B76B6A5F95}" name="Description" dataDxfId="119"/>
+    <tableColumn id="3" xr3:uid="{B909ADC8-9FD8-4714-A691-8AD0F1933057}" name="Units" dataDxfId="118"/>
+    <tableColumn id="4" xr3:uid="{F8B8B123-0CBC-450A-B098-9FFA08F7FC89}" name="Distribution Type" dataDxfId="117"/>
+    <tableColumn id="5" xr3:uid="{AADB8566-896F-40D4-8181-BB145E678F9B}" name="Parameter 1" dataDxfId="116"/>
+    <tableColumn id="6" xr3:uid="{13B0114C-55D3-4603-92C6-09319B7E315B}" name="Parameter 2" dataDxfId="115"/>
+    <tableColumn id="7" xr3:uid="{7548BB98-B29E-4F39-B198-D6F9994CC04D}" name="Parameter 3" dataDxfId="114"/>
+    <tableColumn id="8" xr3:uid="{355D4B98-B5B0-461B-90E8-3D81112B89E2}" name="Parameter 4" dataDxfId="113"/>
+    <tableColumn id="14" xr3:uid="{14667F24-6EC2-4F8F-8EAA-56B4FF372D98}" name="Parameter 5" dataDxfId="112"/>
+    <tableColumn id="15" xr3:uid="{B058DB6A-9C46-4ED3-9483-5713AD52AE40}" name="Parameter 6" dataDxfId="111"/>
+    <tableColumn id="11" xr3:uid="{0E22E7A3-8506-41E8-AC60-E103665C60A2}" name="Lower Limit" dataDxfId="110"/>
+    <tableColumn id="12" xr3:uid="{479761C6-7DBC-4557-9E7C-984A37ABCB8A}" name="Upper Limit" dataDxfId="109"/>
+    <tableColumn id="13" xr3:uid="{F96695B6-2ADD-458A-A424-B58482082C80}" name="Step" dataDxfId="108"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{88C3C7FF-7D66-4C1C-A80E-12CD3AFBFB8D}" name="Table156810210" displayName="Table156810210" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="115">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{88C3C7FF-7D66-4C1C-A80E-12CD3AFBFB8D}" name="Table156810210" displayName="Table156810210" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="105">
   <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{5AC7EE20-3F52-40E0-87F1-21D82A7C3AA2}" name="Phase" dataDxfId="114"/>
-    <tableColumn id="1" xr3:uid="{9A9754BC-4FF9-4BBA-B750-B911CE430E6A}" name="Category" dataDxfId="113"/>
-    <tableColumn id="2" xr3:uid="{0A114B0A-D97E-4073-8E4E-5B16FB19520E}" name="Name" dataDxfId="112"/>
-    <tableColumn id="10" xr3:uid="{D1A72F97-70A3-4EEB-9316-B31F108E3FD5}" name="Description" dataDxfId="111"/>
-    <tableColumn id="3" xr3:uid="{E8F09B1A-D952-4236-B6AD-8AC480554D73}" name="Units" dataDxfId="110"/>
-    <tableColumn id="4" xr3:uid="{B1DC9551-CBBD-4BF4-B876-9237E0FB121D}" name="Distribution Type" dataDxfId="109"/>
-    <tableColumn id="5" xr3:uid="{72C76302-CA88-4629-BF3A-72DD8971E0B7}" name="Parameter 1" dataDxfId="108"/>
-    <tableColumn id="6" xr3:uid="{C319BB6E-60FD-4F37-B898-C033C52FE070}" name="Parameter 2" dataDxfId="107"/>
-    <tableColumn id="7" xr3:uid="{B370DF9A-4768-49F1-B38B-F65D182A01B4}" name="Parameter 3" dataDxfId="106"/>
-    <tableColumn id="8" xr3:uid="{7BADEC71-6529-4D26-804E-5C9B93DA84E8}" name="Parameter 4" dataDxfId="105"/>
-    <tableColumn id="14" xr3:uid="{125149FE-86DA-4053-8A54-90E57B52F8B0}" name="Parameter 5" dataDxfId="104"/>
-    <tableColumn id="15" xr3:uid="{BAA75930-0A4F-4888-8CAF-A3AFA6F3FF44}" name="Parameter 6" dataDxfId="103"/>
-    <tableColumn id="11" xr3:uid="{7442F6EC-3907-41A8-BBEF-87C9374C67E5}" name="Lower Limit" dataDxfId="102"/>
-    <tableColumn id="12" xr3:uid="{86E2B2CA-B8F0-4FF5-8C59-2D3C44061DFD}" name="Upper Limit" dataDxfId="101"/>
-    <tableColumn id="13" xr3:uid="{C697FE06-06BB-49EC-93BB-FF753593319A}" name="Step" dataDxfId="100"/>
+    <tableColumn id="9" xr3:uid="{5AC7EE20-3F52-40E0-87F1-21D82A7C3AA2}" name="Phase" dataDxfId="104"/>
+    <tableColumn id="1" xr3:uid="{9A9754BC-4FF9-4BBA-B750-B911CE430E6A}" name="Category" dataDxfId="103"/>
+    <tableColumn id="2" xr3:uid="{0A114B0A-D97E-4073-8E4E-5B16FB19520E}" name="Name" dataDxfId="102"/>
+    <tableColumn id="10" xr3:uid="{D1A72F97-70A3-4EEB-9316-B31F108E3FD5}" name="Description" dataDxfId="101"/>
+    <tableColumn id="3" xr3:uid="{E8F09B1A-D952-4236-B6AD-8AC480554D73}" name="Units" dataDxfId="100"/>
+    <tableColumn id="4" xr3:uid="{B1DC9551-CBBD-4BF4-B876-9237E0FB121D}" name="Distribution Type" dataDxfId="99"/>
+    <tableColumn id="5" xr3:uid="{72C76302-CA88-4629-BF3A-72DD8971E0B7}" name="Parameter 1" dataDxfId="98"/>
+    <tableColumn id="6" xr3:uid="{C319BB6E-60FD-4F37-B898-C033C52FE070}" name="Parameter 2" dataDxfId="97"/>
+    <tableColumn id="7" xr3:uid="{B370DF9A-4768-49F1-B38B-F65D182A01B4}" name="Parameter 3" dataDxfId="96"/>
+    <tableColumn id="8" xr3:uid="{7BADEC71-6529-4D26-804E-5C9B93DA84E8}" name="Parameter 4" dataDxfId="95"/>
+    <tableColumn id="14" xr3:uid="{125149FE-86DA-4053-8A54-90E57B52F8B0}" name="Parameter 5" dataDxfId="94"/>
+    <tableColumn id="15" xr3:uid="{BAA75930-0A4F-4888-8CAF-A3AFA6F3FF44}" name="Parameter 6" dataDxfId="93"/>
+    <tableColumn id="11" xr3:uid="{7442F6EC-3907-41A8-BBEF-87C9374C67E5}" name="Lower Limit" dataDxfId="92"/>
+    <tableColumn id="12" xr3:uid="{86E2B2CA-B8F0-4FF5-8C59-2D3C44061DFD}" name="Upper Limit" dataDxfId="91"/>
+    <tableColumn id="13" xr3:uid="{C697FE06-06BB-49EC-93BB-FF753593319A}" name="Step" dataDxfId="90"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6794810C-E49F-4CB0-9B2F-0FA2655BD884}" name="Table15681021011" displayName="Table15681021011" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="95">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{6794810C-E49F-4CB0-9B2F-0FA2655BD884}" name="Table15681021011" displayName="Table15681021011" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="87">
   <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{5DEAB66E-0CAB-4BF7-B4EA-D8D12FB47328}" name="Phase" dataDxfId="94"/>
-    <tableColumn id="1" xr3:uid="{69C64F5C-9979-4ACA-9A42-C1032E3D98BA}" name="Category" dataDxfId="93"/>
-    <tableColumn id="2" xr3:uid="{D4385687-B64B-46FB-B987-6E74F19DC1AF}" name="Name" dataDxfId="92"/>
-    <tableColumn id="10" xr3:uid="{BE461B66-2B72-42A7-9F3F-5916187828CF}" name="Description" dataDxfId="91"/>
-    <tableColumn id="3" xr3:uid="{9EE711F7-7C5D-4C54-8A9A-D54F8833D434}" name="Units" dataDxfId="90"/>
-    <tableColumn id="4" xr3:uid="{6EAA6194-27E9-4B7C-8A4D-8C0FE7B617F4}" name="Distribution Type" dataDxfId="89"/>
-    <tableColumn id="5" xr3:uid="{75BC5E4C-C28D-4614-8AB6-165A9F7FE7CE}" name="Parameter 1" dataDxfId="88"/>
-    <tableColumn id="6" xr3:uid="{F5AD0C00-9187-4F91-ADA7-5B461FC355CE}" name="Parameter 2" dataDxfId="87"/>
-    <tableColumn id="7" xr3:uid="{34B0A2DF-5607-43F6-AA9E-1106CCB7621B}" name="Parameter 3" dataDxfId="86"/>
-    <tableColumn id="8" xr3:uid="{B0950426-083D-4CE9-A30E-9D71766BA154}" name="Parameter 4" dataDxfId="85"/>
-    <tableColumn id="14" xr3:uid="{88E7A84D-F80D-416C-9037-2E5927AE2697}" name="Parameter 5" dataDxfId="84"/>
-    <tableColumn id="15" xr3:uid="{E3DCF8BA-29B1-4A24-B6E6-DE9435CB3AC9}" name="Parameter 6" dataDxfId="83"/>
-    <tableColumn id="11" xr3:uid="{E8661EBF-62F4-4D4A-BCDC-7C8ABD4866B0}" name="Lower Limit" dataDxfId="82"/>
-    <tableColumn id="12" xr3:uid="{83DA3A0E-E097-4281-9822-6FE3F8FB0CDD}" name="Upper Limit" dataDxfId="81"/>
-    <tableColumn id="13" xr3:uid="{24B0E0E0-CA9C-4655-9B23-EA0BBD517B67}" name="Step" dataDxfId="80"/>
+    <tableColumn id="9" xr3:uid="{5DEAB66E-0CAB-4BF7-B4EA-D8D12FB47328}" name="Phase" dataDxfId="86"/>
+    <tableColumn id="1" xr3:uid="{69C64F5C-9979-4ACA-9A42-C1032E3D98BA}" name="Category" dataDxfId="85"/>
+    <tableColumn id="2" xr3:uid="{D4385687-B64B-46FB-B987-6E74F19DC1AF}" name="Name" dataDxfId="84"/>
+    <tableColumn id="10" xr3:uid="{BE461B66-2B72-42A7-9F3F-5916187828CF}" name="Description" dataDxfId="83"/>
+    <tableColumn id="3" xr3:uid="{9EE711F7-7C5D-4C54-8A9A-D54F8833D434}" name="Units" dataDxfId="82"/>
+    <tableColumn id="4" xr3:uid="{6EAA6194-27E9-4B7C-8A4D-8C0FE7B617F4}" name="Distribution Type" dataDxfId="81"/>
+    <tableColumn id="5" xr3:uid="{75BC5E4C-C28D-4614-8AB6-165A9F7FE7CE}" name="Parameter 1" dataDxfId="80"/>
+    <tableColumn id="6" xr3:uid="{F5AD0C00-9187-4F91-ADA7-5B461FC355CE}" name="Parameter 2" dataDxfId="79"/>
+    <tableColumn id="7" xr3:uid="{34B0A2DF-5607-43F6-AA9E-1106CCB7621B}" name="Parameter 3" dataDxfId="78"/>
+    <tableColumn id="8" xr3:uid="{B0950426-083D-4CE9-A30E-9D71766BA154}" name="Parameter 4" dataDxfId="77"/>
+    <tableColumn id="14" xr3:uid="{88E7A84D-F80D-416C-9037-2E5927AE2697}" name="Parameter 5" dataDxfId="76"/>
+    <tableColumn id="15" xr3:uid="{E3DCF8BA-29B1-4A24-B6E6-DE9435CB3AC9}" name="Parameter 6" dataDxfId="75"/>
+    <tableColumn id="11" xr3:uid="{E8661EBF-62F4-4D4A-BCDC-7C8ABD4866B0}" name="Lower Limit" dataDxfId="74"/>
+    <tableColumn id="12" xr3:uid="{83DA3A0E-E097-4281-9822-6FE3F8FB0CDD}" name="Upper Limit" dataDxfId="73"/>
+    <tableColumn id="13" xr3:uid="{24B0E0E0-CA9C-4655-9B23-EA0BBD517B67}" name="Step" dataDxfId="72"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{81C05191-4139-4D49-BA19-E7D2B74357F9}" name="Table15681021012" displayName="Table15681021012" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{81C05191-4139-4D49-BA19-E7D2B74357F9}" name="Table15681021012" displayName="Table15681021012" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="69">
   <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{64A27C3D-2E18-40E6-9166-742BDA2B413C}" name="Phase" dataDxfId="74"/>
-    <tableColumn id="1" xr3:uid="{0243CFE4-EBE7-4500-A226-23C63BE2FB81}" name="Category" dataDxfId="73"/>
-    <tableColumn id="2" xr3:uid="{69F68BF8-9E6A-4766-AB29-A8B943A84522}" name="Name" dataDxfId="72"/>
-    <tableColumn id="10" xr3:uid="{1E4511F0-B286-4973-A437-9638677030CA}" name="Description" dataDxfId="71"/>
-    <tableColumn id="3" xr3:uid="{B80720A6-55E5-4A17-9FE9-9951AF480E02}" name="Units" dataDxfId="70"/>
-    <tableColumn id="4" xr3:uid="{54B33DED-7F55-4D76-B95F-B7050BBA4BD1}" name="Distribution Type" dataDxfId="69"/>
-    <tableColumn id="5" xr3:uid="{BC7C6514-68B9-48F6-9938-4088DF28B37C}" name="Parameter 1" dataDxfId="68"/>
-    <tableColumn id="6" xr3:uid="{4D372042-F7DE-4E72-A309-C4266E0FA9E8}" name="Parameter 2" dataDxfId="67"/>
-    <tableColumn id="7" xr3:uid="{8D92705D-1A42-46F5-89EA-C4113CC26587}" name="Parameter 3" dataDxfId="66"/>
-    <tableColumn id="8" xr3:uid="{13B56E18-7C36-4950-847A-A7544475E1D1}" name="Parameter 4" dataDxfId="65"/>
-    <tableColumn id="14" xr3:uid="{2649C7B2-1C48-4B13-969D-684D0045538B}" name="Parameter 5" dataDxfId="64"/>
-    <tableColumn id="15" xr3:uid="{5D6C4F8D-D31E-4EED-BABF-A0A688F3A916}" name="Parameter 6" dataDxfId="63"/>
-    <tableColumn id="11" xr3:uid="{1CB1896E-F77C-4DFC-9AB0-D0C102F3F80F}" name="Lower Limit" dataDxfId="62"/>
-    <tableColumn id="12" xr3:uid="{837665AD-748D-4B51-9CCA-780B67A76815}" name="Upper Limit" dataDxfId="61"/>
-    <tableColumn id="13" xr3:uid="{A8F2935C-D451-47EA-A1E1-1E4F0CAE8D87}" name="Step" dataDxfId="60"/>
+    <tableColumn id="9" xr3:uid="{64A27C3D-2E18-40E6-9166-742BDA2B413C}" name="Phase" dataDxfId="68"/>
+    <tableColumn id="1" xr3:uid="{0243CFE4-EBE7-4500-A226-23C63BE2FB81}" name="Category" dataDxfId="67"/>
+    <tableColumn id="2" xr3:uid="{69F68BF8-9E6A-4766-AB29-A8B943A84522}" name="Name" dataDxfId="66"/>
+    <tableColumn id="10" xr3:uid="{1E4511F0-B286-4973-A437-9638677030CA}" name="Description" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{B80720A6-55E5-4A17-9FE9-9951AF480E02}" name="Units" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{54B33DED-7F55-4D76-B95F-B7050BBA4BD1}" name="Distribution Type" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{BC7C6514-68B9-48F6-9938-4088DF28B37C}" name="Parameter 1" dataDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{4D372042-F7DE-4E72-A309-C4266E0FA9E8}" name="Parameter 2" dataDxfId="61"/>
+    <tableColumn id="7" xr3:uid="{8D92705D-1A42-46F5-89EA-C4113CC26587}" name="Parameter 3" dataDxfId="60"/>
+    <tableColumn id="8" xr3:uid="{13B56E18-7C36-4950-847A-A7544475E1D1}" name="Parameter 4" dataDxfId="59"/>
+    <tableColumn id="14" xr3:uid="{2649C7B2-1C48-4B13-969D-684D0045538B}" name="Parameter 5" dataDxfId="58"/>
+    <tableColumn id="15" xr3:uid="{5D6C4F8D-D31E-4EED-BABF-A0A688F3A916}" name="Parameter 6" dataDxfId="57"/>
+    <tableColumn id="11" xr3:uid="{1CB1896E-F77C-4DFC-9AB0-D0C102F3F80F}" name="Lower Limit" dataDxfId="56"/>
+    <tableColumn id="12" xr3:uid="{837665AD-748D-4B51-9CCA-780B67A76815}" name="Upper Limit" dataDxfId="55"/>
+    <tableColumn id="13" xr3:uid="{A8F2935C-D451-47EA-A1E1-1E4F0CAE8D87}" name="Step" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{2EC220FC-5886-477C-8B2C-57082D8749AA}" name="Table1568102101213" displayName="Table1568102101213" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{2EC220FC-5886-477C-8B2C-57082D8749AA}" name="Table1568102101213" displayName="Table1568102101213" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="51">
   <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{525577E1-B46F-47FB-A042-A56D8D45D9AD}" name="Phase" dataDxfId="54"/>
-    <tableColumn id="1" xr3:uid="{30AFC0FE-4503-4A4B-91CA-E5B88AA24F98}" name="Category" dataDxfId="53"/>
-    <tableColumn id="2" xr3:uid="{6333C26F-3D36-4A65-8F1B-CC515ADCE181}" name="Name" dataDxfId="52"/>
-    <tableColumn id="10" xr3:uid="{057A52C2-DED0-48A5-8844-3950CD398F8D}" name="Description" dataDxfId="51"/>
-    <tableColumn id="3" xr3:uid="{EF447B65-8A6A-4F12-ABCB-7BFE84B734A9}" name="Units" dataDxfId="50"/>
-    <tableColumn id="4" xr3:uid="{6E658D46-B4D3-46B1-A15B-9F0095A7EADD}" name="Distribution Type" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{FE235A77-6EFF-4D9A-926F-ACE5D51D4BC8}" name="Parameter 1" dataDxfId="48"/>
-    <tableColumn id="6" xr3:uid="{26694561-3958-440C-BDDC-2DB16EB8A614}" name="Parameter 2" dataDxfId="47"/>
-    <tableColumn id="7" xr3:uid="{DA96F9A2-3DEB-4C42-BECF-B9C30ADA7428}" name="Parameter 3" dataDxfId="46"/>
-    <tableColumn id="8" xr3:uid="{5F8A48E3-9BBF-4210-88D8-F668C1FD845D}" name="Parameter 4" dataDxfId="45"/>
-    <tableColumn id="14" xr3:uid="{21514092-10F7-41E0-B078-A15175C73E93}" name="Parameter 5" dataDxfId="44"/>
-    <tableColumn id="15" xr3:uid="{8BFA8A6A-2BCB-4512-8B77-28D2C28FEEE3}" name="Parameter 6" dataDxfId="43"/>
-    <tableColumn id="11" xr3:uid="{9CB23DDB-2513-48F3-960F-EF0D57CD9724}" name="Lower Limit" dataDxfId="42"/>
-    <tableColumn id="12" xr3:uid="{EDE53E3A-8BAE-4FD6-9C38-CD4B63274C67}" name="Upper Limit" dataDxfId="41"/>
-    <tableColumn id="13" xr3:uid="{980D57FA-1EDD-484A-9D56-BF7EAA580C8D}" name="Step" dataDxfId="40"/>
+    <tableColumn id="9" xr3:uid="{525577E1-B46F-47FB-A042-A56D8D45D9AD}" name="Phase" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{30AFC0FE-4503-4A4B-91CA-E5B88AA24F98}" name="Category" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{6333C26F-3D36-4A65-8F1B-CC515ADCE181}" name="Name" dataDxfId="48"/>
+    <tableColumn id="10" xr3:uid="{057A52C2-DED0-48A5-8844-3950CD398F8D}" name="Description" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{EF447B65-8A6A-4F12-ABCB-7BFE84B734A9}" name="Units" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{6E658D46-B4D3-46B1-A15B-9F0095A7EADD}" name="Distribution Type" dataDxfId="45"/>
+    <tableColumn id="5" xr3:uid="{FE235A77-6EFF-4D9A-926F-ACE5D51D4BC8}" name="Parameter 1" dataDxfId="44"/>
+    <tableColumn id="6" xr3:uid="{26694561-3958-440C-BDDC-2DB16EB8A614}" name="Parameter 2" dataDxfId="43"/>
+    <tableColumn id="7" xr3:uid="{DA96F9A2-3DEB-4C42-BECF-B9C30ADA7428}" name="Parameter 3" dataDxfId="42"/>
+    <tableColumn id="8" xr3:uid="{5F8A48E3-9BBF-4210-88D8-F668C1FD845D}" name="Parameter 4" dataDxfId="41"/>
+    <tableColumn id="14" xr3:uid="{21514092-10F7-41E0-B078-A15175C73E93}" name="Parameter 5" dataDxfId="40"/>
+    <tableColumn id="15" xr3:uid="{8BFA8A6A-2BCB-4512-8B77-28D2C28FEEE3}" name="Parameter 6" dataDxfId="39"/>
+    <tableColumn id="11" xr3:uid="{9CB23DDB-2513-48F3-960F-EF0D57CD9724}" name="Lower Limit" dataDxfId="38"/>
+    <tableColumn id="12" xr3:uid="{EDE53E3A-8BAE-4FD6-9C38-CD4B63274C67}" name="Upper Limit" dataDxfId="37"/>
+    <tableColumn id="13" xr3:uid="{980D57FA-1EDD-484A-9D56-BF7EAA580C8D}" name="Step" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3DDD9CB2-968B-4A43-A20B-C749950155AA}" name="Table156810210121314" displayName="Table156810210121314" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{3DDD9CB2-968B-4A43-A20B-C749950155AA}" name="Table156810210121314" displayName="Table156810210121314" ref="A1:O9" totalsRowShown="0" tableBorderDxfId="33">
   <autoFilter ref="A1:O9" xr:uid="{6517A09C-F3AC-4B68-94FA-1AD3D2AE52FD}"/>
   <tableColumns count="15">
-    <tableColumn id="9" xr3:uid="{6B814874-1824-4E56-A967-04F9F6F3E584}" name="Phase" dataDxfId="34"/>
-    <tableColumn id="1" xr3:uid="{FE1635BE-F6C3-4D5B-B06E-7A92EBAB074D}" name="Category" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{9C16A715-E236-4930-A633-7510E082392C}" name="Name" dataDxfId="32"/>
-    <tableColumn id="10" xr3:uid="{B556C16A-1909-46E7-BC6D-8479761F1F65}" name="Description" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{5EFB6F3C-9894-43AA-AFAC-1013F8F0714B}" name="Units" dataDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{6E3C1049-1D84-4FD5-B7CF-1E130CD32BCA}" name="Distribution Type" dataDxfId="29"/>
-    <tableColumn id="5" xr3:uid="{57E979B1-A630-4AC5-8C4D-CED1A62F587D}" name="Parameter 1" dataDxfId="28"/>
-    <tableColumn id="6" xr3:uid="{C9EF8DDD-DA1F-44E2-AC90-B6993C60CF1F}" name="Parameter 2" dataDxfId="27"/>
-    <tableColumn id="7" xr3:uid="{6FEFD03F-983B-47E2-9525-7EDD875A9C7C}" name="Parameter 3" dataDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{0B661DB2-D286-4AEE-88C3-124B37F1B246}" name="Parameter 4" dataDxfId="25"/>
-    <tableColumn id="14" xr3:uid="{08C4ACC8-5A7B-4864-96E4-CF69FD654892}" name="Parameter 5" dataDxfId="24"/>
-    <tableColumn id="15" xr3:uid="{5505BBCC-5C52-4400-9C19-9ED7DBB490B8}" name="Parameter 6" dataDxfId="23"/>
-    <tableColumn id="11" xr3:uid="{E151AC3B-28ED-4186-A803-48B7F8B7AE5B}" name="Lower Limit" dataDxfId="22"/>
-    <tableColumn id="12" xr3:uid="{223709CC-AD09-4677-85AC-DF8A1619BF81}" name="Upper Limit" dataDxfId="21"/>
-    <tableColumn id="13" xr3:uid="{5FAAB5F5-A70D-4A6B-BE36-5CC1FD787BC5}" name="Step" dataDxfId="20"/>
+    <tableColumn id="9" xr3:uid="{6B814874-1824-4E56-A967-04F9F6F3E584}" name="Phase" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{FE1635BE-F6C3-4D5B-B06E-7A92EBAB074D}" name="Category" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{9C16A715-E236-4930-A633-7510E082392C}" name="Name" dataDxfId="30"/>
+    <tableColumn id="10" xr3:uid="{B556C16A-1909-46E7-BC6D-8479761F1F65}" name="Description" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{5EFB6F3C-9894-43AA-AFAC-1013F8F0714B}" name="Units" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{6E3C1049-1D84-4FD5-B7CF-1E130CD32BCA}" name="Distribution Type" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{57E979B1-A630-4AC5-8C4D-CED1A62F587D}" name="Parameter 1" dataDxfId="26"/>
+    <tableColumn id="6" xr3:uid="{C9EF8DDD-DA1F-44E2-AC90-B6993C60CF1F}" name="Parameter 2" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{6FEFD03F-983B-47E2-9525-7EDD875A9C7C}" name="Parameter 3" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{0B661DB2-D286-4AEE-88C3-124B37F1B246}" name="Parameter 4" dataDxfId="23"/>
+    <tableColumn id="14" xr3:uid="{08C4ACC8-5A7B-4864-96E4-CF69FD654892}" name="Parameter 5" dataDxfId="22"/>
+    <tableColumn id="15" xr3:uid="{5505BBCC-5C52-4400-9C19-9ED7DBB490B8}" name="Parameter 6" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{E151AC3B-28ED-4186-A803-48B7F8B7AE5B}" name="Lower Limit" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{223709CC-AD09-4677-85AC-DF8A1619BF81}" name="Upper Limit" dataDxfId="19"/>
+    <tableColumn id="13" xr3:uid="{5FAAB5F5-A70D-4A6B-BE36-5CC1FD787BC5}" name="Step" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3909,7 +3800,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4017,7 +3908,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -4045,7 +3936,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
@@ -4263,20 +4154,12 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L2 A4:L9 A3:D3 F3:L3">
-    <cfRule type="expression" dxfId="39" priority="3">
+  <conditionalFormatting sqref="A2:L9">
+    <cfRule type="expression" dxfId="35" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="4">
+    <cfRule type="expression" dxfId="34" priority="2">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="37" priority="1">
-      <formula>ISBLANK($F3)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="36" priority="2">
-      <formula>NOT((COLUMN(E3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -4296,7 +4179,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4404,7 +4287,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -4432,7 +4315,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
@@ -4650,20 +4533,12 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L2 A4:L9 A3:D3 F3:L3">
-    <cfRule type="expression" dxfId="19" priority="3">
+  <conditionalFormatting sqref="A2:L9">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="4">
+    <cfRule type="expression" dxfId="16" priority="2">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="17" priority="1">
-      <formula>ISBLANK($F3)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="16" priority="2">
-      <formula>NOT((COLUMN(E3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -5083,10 +4958,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097870CC-1A0F-461E-BDFD-29BDDFDDF05C}">
-  <dimension ref="A1:Q32"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5098,7 +4973,7 @@
     <col min="5" max="15" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -5145,7 +5020,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>70</v>
       </c>
@@ -5153,7 +5028,7 @@
         <v>70</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>53</v>
@@ -5164,16 +5039,14 @@
       <c r="F2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="5">
-        <v>0</v>
-      </c>
+      <c r="G2" s="5"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="6"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="17">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="N2" s="17">
         <v>50000000</v>
@@ -5182,7 +5055,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>70</v>
       </c>
@@ -5190,20 +5063,18 @@
         <v>70</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D3" s="9" t="s">
         <v>93</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="9">
-        <v>-1</v>
-      </c>
+      <c r="G3" s="9"/>
       <c r="H3" s="9"/>
       <c r="I3" s="9"/>
       <c r="J3" s="10"/>
@@ -5219,7 +5090,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>71</v>
       </c>
@@ -5227,7 +5098,7 @@
         <v>71</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>52</v>
@@ -5238,25 +5109,23 @@
       <c r="F4" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="12">
-        <v>747.86950000000002</v>
-      </c>
+      <c r="G4" s="12"/>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
       <c r="J4" s="13"/>
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
-      <c r="M4" s="17">
-        <v>0</v>
+      <c r="M4" s="18">
+        <v>10000</v>
       </c>
       <c r="N4" s="18">
         <v>50000000</v>
       </c>
       <c r="O4" s="18">
-        <v>1.0000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
         <v>71</v>
       </c>
@@ -5264,23 +5133,19 @@
         <v>71</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D5" s="9" t="s">
         <v>94</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="9">
-        <v>3.0319702616531905</v>
-      </c>
-      <c r="H5" s="9">
-        <v>8.0319702616531909</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="10"/>
       <c r="K5" s="2"/>
@@ -5291,12 +5156,11 @@
       <c r="N5" s="19">
         <v>10</v>
       </c>
-      <c r="O5" s="18">
-        <v>1.0000000000000001E-9</v>
-      </c>
-      <c r="Q5" s="21"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O5" s="19">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>72</v>
       </c>
@@ -5304,7 +5168,7 @@
         <v>72</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D6" s="12" t="s">
         <v>73</v>
@@ -5315,16 +5179,14 @@
       <c r="F6" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="12">
-        <v>0</v>
-      </c>
+      <c r="G6" s="12"/>
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="13"/>
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
       <c r="M6" s="18">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="N6" s="18">
         <v>50000000</v>
@@ -5333,7 +5195,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>72</v>
       </c>
@@ -5341,20 +5203,18 @@
         <v>72</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D7" s="12" t="s">
         <v>95</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F7" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="12">
-        <v>-1</v>
-      </c>
+      <c r="G7" s="12"/>
       <c r="H7" s="12"/>
       <c r="I7" s="12"/>
       <c r="J7" s="13"/>
@@ -5370,7 +5230,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
         <v>71</v>
       </c>
@@ -5403,11 +5263,11 @@
       <c r="N8" s="9">
         <v>1</v>
       </c>
-      <c r="O8" s="18">
-        <v>1.0000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O8" s="9">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
         <v>71</v>
       </c>
@@ -5427,7 +5287,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="9">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
@@ -5440,11 +5300,11 @@
       <c r="N9" s="9">
         <v>1</v>
       </c>
-      <c r="O9" s="18">
-        <v>1.0000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O9" s="9">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
         <v>71</v>
       </c>
@@ -5464,7 +5324,7 @@
         <v>3</v>
       </c>
       <c r="G10" s="9">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
@@ -5477,11 +5337,11 @@
       <c r="N10" s="9">
         <v>1</v>
       </c>
-      <c r="O10" s="18">
-        <v>1.0000000000000001E-9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="O10" s="9">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="8" t="s">
         <v>71</v>
       </c>
@@ -5518,7 +5378,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="8" t="s">
         <v>71</v>
       </c>
@@ -5555,7 +5415,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="8" t="s">
         <v>71</v>
       </c>
@@ -5592,7 +5452,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>71</v>
       </c>
@@ -5629,18 +5489,18 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>70</v>
       </c>
       <c r="B15" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>115</v>
-      </c>
       <c r="D15" s="12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E15" s="12" t="s">
         <v>68</v>
@@ -5649,7 +5509,7 @@
         <v>3</v>
       </c>
       <c r="G15" s="12">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
@@ -5666,18 +5526,18 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>70</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>68</v>
@@ -5686,7 +5546,7 @@
         <v>3</v>
       </c>
       <c r="G16" s="12">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="H16" s="12"/>
       <c r="I16" s="12"/>
@@ -5708,13 +5568,13 @@
         <v>70</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E17" s="12" t="s">
         <v>68</v>
@@ -5723,7 +5583,7 @@
         <v>3</v>
       </c>
       <c r="G17" s="12">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
@@ -5745,13 +5605,13 @@
         <v>70</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>68</v>
@@ -5760,7 +5620,7 @@
         <v>3</v>
       </c>
       <c r="G18" s="12">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H18" s="12"/>
       <c r="I18" s="12"/>
@@ -5782,13 +5642,13 @@
         <v>70</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>68</v>
@@ -5797,7 +5657,7 @@
         <v>3</v>
       </c>
       <c r="G19" s="12">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="H19" s="12"/>
       <c r="I19" s="12"/>
@@ -5819,13 +5679,13 @@
         <v>70</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E20" s="12" t="s">
         <v>68</v>
@@ -5834,7 +5694,7 @@
         <v>3</v>
       </c>
       <c r="G20" s="12">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="H20" s="12"/>
       <c r="I20" s="12"/>
@@ -5856,13 +5716,13 @@
         <v>72</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>68</v>
@@ -5871,7 +5731,7 @@
         <v>3</v>
       </c>
       <c r="G21" s="12">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H21" s="12"/>
       <c r="I21" s="12"/>
@@ -5893,13 +5753,13 @@
         <v>72</v>
       </c>
       <c r="B22" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="C22" s="12" t="s">
-        <v>127</v>
-      </c>
       <c r="D22" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>68</v>
@@ -5908,7 +5768,7 @@
         <v>3</v>
       </c>
       <c r="G22" s="12">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
@@ -5930,13 +5790,13 @@
         <v>72</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>68</v>
@@ -5945,7 +5805,7 @@
         <v>3</v>
       </c>
       <c r="G23" s="12">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H23" s="12"/>
       <c r="I23" s="12"/>
@@ -5967,13 +5827,13 @@
         <v>72</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>68</v>
@@ -5982,7 +5842,7 @@
         <v>3</v>
       </c>
       <c r="G24" s="12">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="H24" s="12"/>
       <c r="I24" s="12"/>
@@ -6004,13 +5864,13 @@
         <v>72</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>68</v>
@@ -6019,7 +5879,7 @@
         <v>3</v>
       </c>
       <c r="G25" s="12">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="H25" s="12"/>
       <c r="I25" s="12"/>
@@ -6044,10 +5904,10 @@
         <v>152</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>68</v>
@@ -6056,7 +5916,7 @@
         <v>3</v>
       </c>
       <c r="G26" s="12">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="H26" s="12"/>
       <c r="I26" s="12"/>
@@ -6078,13 +5938,13 @@
         <v>71</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E27" s="12" t="s">
         <v>68</v>
@@ -6093,7 +5953,7 @@
         <v>3</v>
       </c>
       <c r="G27" s="12">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="12"/>
@@ -6118,10 +5978,10 @@
         <v>104</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>68</v>
@@ -6130,7 +5990,7 @@
         <v>3</v>
       </c>
       <c r="G28" s="12">
-        <v>0.125</v>
+        <v>0.1</v>
       </c>
       <c r="H28" s="12"/>
       <c r="I28" s="12"/>
@@ -6144,7 +6004,7 @@
         <v>1</v>
       </c>
       <c r="O28" s="12">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
@@ -6155,10 +6015,10 @@
         <v>105</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>68</v>
@@ -6167,7 +6027,7 @@
         <v>3</v>
       </c>
       <c r="G29" s="12">
-        <v>6.25E-2</v>
+        <v>0.05</v>
       </c>
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
@@ -6181,7 +6041,7 @@
         <v>1</v>
       </c>
       <c r="O29" s="12">
-        <v>1E-4</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
@@ -6192,10 +6052,10 @@
         <v>106</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>68</v>
@@ -6204,7 +6064,7 @@
         <v>3</v>
       </c>
       <c r="G30" s="12">
-        <v>6.25E-2</v>
+        <v>0.3</v>
       </c>
       <c r="H30" s="12"/>
       <c r="I30" s="12"/>
@@ -6218,7 +6078,7 @@
         <v>1</v>
       </c>
       <c r="O30" s="12">
-        <v>1E-4</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
@@ -6229,10 +6089,10 @@
         <v>153</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>68</v>
@@ -6241,7 +6101,7 @@
         <v>3</v>
       </c>
       <c r="G31" s="12">
-        <v>0.125</v>
+        <v>0.15</v>
       </c>
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
@@ -6266,10 +6126,10 @@
         <v>108</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>68</v>
@@ -6278,7 +6138,7 @@
         <v>3</v>
       </c>
       <c r="G32" s="12">
-        <v>0.125</v>
+        <v>0.1</v>
       </c>
       <c r="H32" s="12"/>
       <c r="I32" s="12"/>
@@ -6298,10 +6158,10 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A2:L32">
-    <cfRule type="expression" dxfId="155" priority="43">
+    <cfRule type="expression" dxfId="143" priority="43">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="154" priority="44">
+    <cfRule type="expression" dxfId="142" priority="44">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6322,7 +6182,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6430,7 +6290,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -6458,7 +6318,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
@@ -6677,10 +6537,10 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:L9">
-    <cfRule type="expression" dxfId="137" priority="1">
+    <cfRule type="expression" dxfId="125" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="136" priority="2">
+    <cfRule type="expression" dxfId="124" priority="2">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6701,7 +6561,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B4" sqref="B4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6809,7 +6669,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -6837,7 +6697,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
@@ -7055,20 +6915,12 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L2 A4:L9 A3:D3 F3:L3">
-    <cfRule type="expression" dxfId="119" priority="3">
+  <conditionalFormatting sqref="A2:L9">
+    <cfRule type="expression" dxfId="107" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="118" priority="4">
+    <cfRule type="expression" dxfId="106" priority="2">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="117" priority="1">
-      <formula>ISBLANK($F3)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="116" priority="2">
-      <formula>NOT((COLUMN(E3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -7088,7 +6940,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7196,7 +7048,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -7224,7 +7076,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
@@ -7442,20 +7294,12 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L2 A4:L9 A3:D3 F3:L3">
-    <cfRule type="expression" dxfId="99" priority="5">
+  <conditionalFormatting sqref="A2:L9">
+    <cfRule type="expression" dxfId="89" priority="3">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="98" priority="6">
+    <cfRule type="expression" dxfId="88" priority="4">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="97" priority="1">
-      <formula>ISBLANK($F3)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="96" priority="2">
-      <formula>NOT((COLUMN(E3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -7475,7 +7319,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7583,7 +7427,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -7611,7 +7455,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
@@ -7829,20 +7673,12 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L2 A4:L9 A3:D3 F3:L3">
-    <cfRule type="expression" dxfId="79" priority="3">
+  <conditionalFormatting sqref="A2:L9">
+    <cfRule type="expression" dxfId="71" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="4">
+    <cfRule type="expression" dxfId="70" priority="2">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="77" priority="1">
-      <formula>ISBLANK($F3)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="76" priority="2">
-      <formula>NOT((COLUMN(E3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -7862,7 +7698,7 @@
   <dimension ref="A1:O9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7970,7 +7806,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="12" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="F3" s="12" t="s">
         <v>3</v>
@@ -7998,7 +7834,7 @@
         <v>71</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>103</v>
@@ -8216,20 +8052,12 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:L2 A4:L9 A3:D3 F3:L3">
-    <cfRule type="expression" dxfId="59" priority="3">
+  <conditionalFormatting sqref="A2:L9">
+    <cfRule type="expression" dxfId="53" priority="1">
       <formula>ISBLANK($F2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="4">
+    <cfRule type="expression" dxfId="52" priority="2">
       <formula>NOT((COLUMN(A2)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F2, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="57" priority="1">
-      <formula>ISBLANK($F3)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="56" priority="2">
-      <formula>NOT((COLUMN(E3)-COLUMN($F:$F))&lt;=IFERROR(VLOOKUP($F3, Validation_Distribution_Parameter_Count, 2, FALSE), 0))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">

</xml_diff>

<commit_message>
Updated the minimum for contaminated areas
</commit_message>
<xml_diff>
--- a/InputFiles/DefineScenario.xlsx
+++ b/InputFiles/DefineScenario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peraza\Box\TO 19F0117 Framework for Sampling\Task 5\Deliverables\(14) Verification Cases\Original Input Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peraza\Documents\Tasking\(4) Wide Area Decon\Task 5 Repo\WideAreaDecon\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5FA6B07-C637-45B8-8105-43B8BC7F00AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A15BF7D-F9D8-4A78-AA0E-44B81EEEE6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="649" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="649" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal - File Info" sheetId="1" r:id="rId1"/>
@@ -4960,8 +4960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097870CC-1A0F-461E-BDFD-29BDDFDDF05C}">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5046,7 +5046,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="17">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="N2" s="17">
         <v>50000000</v>
@@ -5116,7 +5116,7 @@
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
       <c r="M4" s="18">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="N4" s="18">
         <v>50000000</v>
@@ -5186,7 +5186,7 @@
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
       <c r="M6" s="18">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="N6" s="18">
         <v>50000000</v>

</xml_diff>

<commit_message>
Updated contaminated area maximums
</commit_message>
<xml_diff>
--- a/InputFiles/DefineScenario.xlsx
+++ b/InputFiles/DefineScenario.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peraza\Documents\Tasking\(4) Wide Area Decon\Task 5 Repo\WideAreaDecon\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A15BF7D-F9D8-4A78-AA0E-44B81EEEE6AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F9047F-E91C-4388-AA21-52C13A0515AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="649" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="649" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal - File Info" sheetId="1" r:id="rId1"/>
@@ -4961,7 +4961,7 @@
   <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5119,7 +5119,7 @@
         <v>0</v>
       </c>
       <c r="N4" s="18">
-        <v>50000000</v>
+        <v>50000</v>
       </c>
       <c r="O4" s="18">
         <v>10000</v>
@@ -5189,7 +5189,7 @@
         <v>0</v>
       </c>
       <c r="N6" s="18">
-        <v>50000000</v>
+        <v>500000</v>
       </c>
       <c r="O6" s="18">
         <v>10000</v>

</xml_diff>

<commit_message>
Merged PR 49: Finalization of the capabilities in the tool (#11)
* Merged PR 49: Finalization of the capabilities in the tool

* Adding in nuget configs for the builds

* Add packages

* Some fixes to charting
</commit_message>
<xml_diff>
--- a/InputFiles/DefineScenario.xlsx
+++ b/InputFiles/DefineScenario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PERAZA\Documents\Tasking\(4) EPA Stuff\Task 5 Repo\WideAreaDecon\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peraza\Documents\Tasking\(4) Wide Area Decon\Task 5 Repo\WideAreaDecon\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9F6AF9-D8C7-4947-8663-BAC9963E88A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F9047F-E91C-4388-AA21-52C13A0515AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="649" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="649" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal - File Info" sheetId="1" r:id="rId1"/>
@@ -4960,8 +4960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097870CC-1A0F-461E-BDFD-29BDDFDDF05C}">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5046,7 +5046,7 @@
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="17">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="N2" s="17">
         <v>50000000</v>
@@ -5116,10 +5116,10 @@
       <c r="K4" s="13"/>
       <c r="L4" s="13"/>
       <c r="M4" s="18">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="N4" s="18">
-        <v>50000000</v>
+        <v>50000</v>
       </c>
       <c r="O4" s="18">
         <v>10000</v>
@@ -5186,10 +5186,10 @@
       <c r="K6" s="12"/>
       <c r="L6" s="12"/>
       <c r="M6" s="18">
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="N6" s="18">
-        <v>50000000</v>
+        <v>500000</v>
       </c>
       <c r="O6" s="18">
         <v>10000</v>

</xml_diff>

<commit_message>
Changes to parameter names and baseline values
</commit_message>
<xml_diff>
--- a/InputFiles/DefineScenario.xlsx
+++ b/InputFiles/DefineScenario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peraza\Documents\Tasking\(4) Wide Area Decon\Task 5 Repo\WideAreaDecon\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F9047F-E91C-4388-AA21-52C13A0515AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39142A4-DBF4-4654-8A5F-35379C6BA147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="649" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="649" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal - File Info" sheetId="1" r:id="rId1"/>
@@ -4960,8 +4960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097870CC-1A0F-461E-BDFD-29BDDFDDF05C}">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5052,7 +5052,7 @@
         <v>50000000</v>
       </c>
       <c r="O2" s="17">
-        <v>10000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -5122,7 +5122,7 @@
         <v>50000</v>
       </c>
       <c r="O4" s="18">
-        <v>10000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -5192,7 +5192,7 @@
         <v>500000</v>
       </c>
       <c r="O6" s="18">
-        <v>10000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
re-add scaled beta to input files
</commit_message>
<xml_diff>
--- a/InputFiles/DefineScenario.xlsx
+++ b/InputFiles/DefineScenario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peraza\Documents\Tasking\(4) Wide Area Decon\Task 5 Repo\WideAreaDecon\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\EPA\WideAreaDecontamination\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39142A4-DBF4-4654-8A5F-35379C6BA147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0CEC4D-5BA0-44A7-A934-A33555C88909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="649" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="649" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal - File Info" sheetId="1" r:id="rId1"/>
@@ -26,8 +26,8 @@
     <sheet name="Educational Characteristics" sheetId="25" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="Validation_Distribution_Parameter_Count">'Internal - Data Validation'!$A$2:$B$11</definedName>
-    <definedName name="Validation_Distribution_Types">'Internal - Data Validation'!$A$2:$A$11</definedName>
+    <definedName name="Validation_Distribution_Parameter_Count">'Internal - Data Validation'!$A$2:$B$12</definedName>
+    <definedName name="Validation_Distribution_Types">'Internal - Data Validation'!$A$2:$A$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="157">
   <si>
     <t>SCWAD</t>
   </si>
@@ -506,6 +506,15 @@
   </si>
   <si>
     <t>Indoor HVAC</t>
+  </si>
+  <si>
+    <t>Scaled Beta</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>Beta</t>
   </si>
 </sst>
 </file>
@@ -4556,10 +4565,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4673,10 +4682,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>87</v>
+        <v>154</v>
       </c>
       <c r="B6" s="9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>40</v>
@@ -4684,17 +4693,21 @@
       <c r="D6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
+      <c r="E6" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>156</v>
+      </c>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>40</v>
@@ -4702,45 +4715,45 @@
       <c r="D7" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B8" s="9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
+      <c r="F8" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B9" s="9">
         <v>2</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
@@ -4749,59 +4762,77 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>81</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="9">
+        <v>4</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B12" s="9">
         <v>6</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C12" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D12" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E12" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F12" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G12" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H12" s="9" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="20" t="s">
         <v>99</v>
       </c>
     </row>
@@ -4960,8 +4991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097870CC-1A0F-461E-BDFD-29BDDFDDF05C}">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Merged PR 58: Merge in master_dev
</commit_message>
<xml_diff>
--- a/InputFiles/DefineScenario.xlsx
+++ b/InputFiles/DefineScenario.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peraza\Documents\Tasking\(4) Wide Area Decon\Task 5 Repo\WideAreaDecon\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\EPA\WideAreaDecontamination\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F9047F-E91C-4388-AA21-52C13A0515AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA0CEC4D-5BA0-44A7-A934-A33555C88909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="649" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="649" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Internal - File Info" sheetId="1" r:id="rId1"/>
@@ -26,8 +26,8 @@
     <sheet name="Educational Characteristics" sheetId="25" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="Validation_Distribution_Parameter_Count">'Internal - Data Validation'!$A$2:$B$11</definedName>
-    <definedName name="Validation_Distribution_Types">'Internal - Data Validation'!$A$2:$A$11</definedName>
+    <definedName name="Validation_Distribution_Parameter_Count">'Internal - Data Validation'!$A$2:$B$12</definedName>
+    <definedName name="Validation_Distribution_Types">'Internal - Data Validation'!$A$2:$A$12</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="157">
   <si>
     <t>SCWAD</t>
   </si>
@@ -506,6 +506,15 @@
   </si>
   <si>
     <t>Indoor HVAC</t>
+  </si>
+  <si>
+    <t>Scaled Beta</t>
+  </si>
+  <si>
+    <t>Alpha</t>
+  </si>
+  <si>
+    <t>Beta</t>
   </si>
 </sst>
 </file>
@@ -4556,10 +4565,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4673,10 +4682,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>87</v>
+        <v>154</v>
       </c>
       <c r="B6" s="9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>40</v>
@@ -4684,17 +4693,21 @@
       <c r="D6" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
+      <c r="E6" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>156</v>
+      </c>
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B7" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>40</v>
@@ -4702,45 +4715,45 @@
       <c r="D7" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>43</v>
-      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
       <c r="G7" s="15"/>
       <c r="H7" s="15"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B8" s="9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
+      <c r="F8" s="9" t="s">
+        <v>43</v>
+      </c>
       <c r="G8" s="15"/>
       <c r="H8" s="15"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B9" s="9">
         <v>2</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>75</v>
+        <v>42</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
@@ -4749,59 +4762,77 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>81</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="15"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="9">
+        <v>4</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B12" s="9">
         <v>6</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C12" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D12" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E12" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F12" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G12" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H12" s="9" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="20" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="20" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="20" t="s">
         <v>99</v>
       </c>
     </row>
@@ -4960,8 +4991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097870CC-1A0F-461E-BDFD-29BDDFDDF05C}">
   <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5052,7 +5083,7 @@
         <v>50000000</v>
       </c>
       <c r="O2" s="17">
-        <v>10000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -5122,7 +5153,7 @@
         <v>50000</v>
       </c>
       <c r="O4" s="18">
-        <v>10000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -5192,7 +5223,7 @@
         <v>500000</v>
       </c>
       <c r="O6" s="18">
-        <v>10000</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">

</xml_diff>